<commit_message>
Correct pre-defined value #3
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A0139C-7F9A-4634-92FB-9B54D0B57B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD04AD3E-601F-48A4-8E62-C1BF668BF521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="432">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Personne_reception_groupe</t>
   </si>
   <si>
-    <t>Type_conservation</t>
-  </si>
-  <si>
     <t>No_Local_entreposage_groupe</t>
   </si>
   <si>
@@ -279,18 +276,6 @@
     <t>Provenance_extrait</t>
   </si>
   <si>
-    <t>Annee_reception</t>
-  </si>
-  <si>
-    <t>Mois_reception</t>
-  </si>
-  <si>
-    <t>Jour_reception</t>
-  </si>
-  <si>
-    <t>Personne_reception</t>
-  </si>
-  <si>
     <t>Nom_projet</t>
   </si>
   <si>
@@ -582,9 +567,6 @@
     <t>Numero_unique_dloop</t>
   </si>
   <si>
-    <t>Tab</t>
-  </si>
-  <si>
     <t>Col</t>
   </si>
   <si>
@@ -624,12 +606,6 @@
     <t>QiaCube</t>
   </si>
   <si>
-    <t>DNeasy Blood and Tissue Kit</t>
-  </si>
-  <si>
-    <t>EZNA mollusc DNA kit</t>
-  </si>
-  <si>
     <t>QIAamp96</t>
   </si>
   <si>
@@ -645,12 +621,6 @@
     <t>PowerWater</t>
   </si>
   <si>
-    <t>DNeasy Blood and Tissue Kit et tampon EB</t>
-  </si>
-  <si>
-    <t>QIAamp Fast DNA stool mini kit</t>
-  </si>
-  <si>
     <t>V_09</t>
   </si>
   <si>
@@ -711,9 +681,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>ADN|ARN|ADE</t>
-  </si>
-  <si>
     <t>BT</t>
   </si>
   <si>
@@ -721,13 +688,658 @@
   </si>
   <si>
     <t>BS</t>
+  </si>
+  <si>
+    <t>Type_conservation_groupe</t>
+  </si>
+  <si>
+    <t>Type_conservation_specimen</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>ADN</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>DMSO</t>
+  </si>
+  <si>
+    <t>EtOH</t>
+  </si>
+  <si>
+    <t>Sec</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>V_15</t>
+  </si>
+  <si>
+    <t>V_16</t>
+  </si>
+  <si>
+    <t>V_17</t>
+  </si>
+  <si>
+    <t>V_18</t>
+  </si>
+  <si>
+    <t>V_19</t>
+  </si>
+  <si>
+    <t>B115</t>
+  </si>
+  <si>
+    <t>B125</t>
+  </si>
+  <si>
+    <t>B136</t>
+  </si>
+  <si>
+    <t>B425</t>
+  </si>
+  <si>
+    <t>B459</t>
+  </si>
+  <si>
+    <t>B460</t>
+  </si>
+  <si>
+    <t>B462</t>
+  </si>
+  <si>
+    <t>B463</t>
+  </si>
+  <si>
+    <t>B464</t>
+  </si>
+  <si>
+    <t>B465</t>
+  </si>
+  <si>
+    <t>B466</t>
+  </si>
+  <si>
+    <t>C120</t>
+  </si>
+  <si>
+    <t>Dneasy_Blood_and_Tissue_Kit</t>
+  </si>
+  <si>
+    <t>EZNA_mollusc_DNA_kit</t>
+  </si>
+  <si>
+    <t>Dneasy_Blood_and_Tissue_Kit_et_tampon_EB</t>
+  </si>
+  <si>
+    <t>QIAamp_Fast_DNA_stool_mini_kit</t>
+  </si>
+  <si>
+    <t>Congelation_80</t>
+  </si>
+  <si>
+    <t>Congelation_20</t>
+  </si>
+  <si>
+    <t>Azote_liquide</t>
+  </si>
+  <si>
+    <t>qPCR_Rosel</t>
+  </si>
+  <si>
+    <t>PON_010502_Sexage_belugas_qPCR</t>
+  </si>
+  <si>
+    <t>EPSG_6622</t>
+  </si>
+  <si>
+    <t>EPSG_3857</t>
+  </si>
+  <si>
+    <t>EPSG_4326</t>
+  </si>
+  <si>
+    <t>BELUGA</t>
+  </si>
+  <si>
+    <t>CRABE_CHINOIS</t>
+  </si>
+  <si>
+    <t>CRABE_VERT</t>
+  </si>
+  <si>
+    <t>CREVETTE_NORDIQUE</t>
+  </si>
+  <si>
+    <t>MACTRE</t>
+  </si>
+  <si>
+    <t>MAQUEREAU</t>
+  </si>
+  <si>
+    <t>NARVAL</t>
+  </si>
+  <si>
+    <t>PALOURDE</t>
+  </si>
+  <si>
+    <t>PETONCLE</t>
+  </si>
+  <si>
+    <t>PETONCLE_GEANT</t>
+  </si>
+  <si>
+    <t>PHOQUE</t>
+  </si>
+  <si>
+    <t>SEBASTE</t>
+  </si>
+  <si>
+    <t>LOUP_ATLANTIQUE</t>
+  </si>
+  <si>
+    <t>CIONA</t>
+  </si>
+  <si>
+    <t>REQUIN_BLANC</t>
+  </si>
+  <si>
+    <t>MOULE_ZEBREE</t>
+  </si>
+  <si>
+    <t>MOULE_QUAGGA</t>
+  </si>
+  <si>
+    <t>CRABE_COMMUN</t>
+  </si>
+  <si>
+    <t>CRABE_ARAIGNEE</t>
+  </si>
+  <si>
+    <t>CRABE_LYRE</t>
+  </si>
+  <si>
+    <t>CRABE_DES_NEIGES</t>
+  </si>
+  <si>
+    <t>CRABE_EPINEUX</t>
+  </si>
+  <si>
+    <t>PHOQUE_GRIS</t>
+  </si>
+  <si>
+    <t>PHOQUE_COMMUN</t>
+  </si>
+  <si>
+    <t>Delphinapterus</t>
+  </si>
+  <si>
+    <t>Eriocheir</t>
+  </si>
+  <si>
+    <t>Carcinus</t>
+  </si>
+  <si>
+    <t>Pandalus</t>
+  </si>
+  <si>
+    <t>Spisula</t>
+  </si>
+  <si>
+    <t>Mactromeris</t>
+  </si>
+  <si>
+    <t>Scomber</t>
+  </si>
+  <si>
+    <t>Monodon</t>
+  </si>
+  <si>
+    <t>Arctica</t>
+  </si>
+  <si>
+    <t>Chlamys</t>
+  </si>
+  <si>
+    <t>Placopecten</t>
+  </si>
+  <si>
+    <t>Phoca</t>
+  </si>
+  <si>
+    <t>Sebastes</t>
+  </si>
+  <si>
+    <t>Anarhichas</t>
+  </si>
+  <si>
+    <t>Ciona</t>
+  </si>
+  <si>
+    <t>Carcharodon</t>
+  </si>
+  <si>
+    <t>Dreissena</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>Hyas</t>
+  </si>
+  <si>
+    <t>Chionoecetes</t>
+  </si>
+  <si>
+    <t>Lithodes</t>
+  </si>
+  <si>
+    <t>Halichoerus</t>
+  </si>
+  <si>
+    <t>leucas</t>
+  </si>
+  <si>
+    <t>sinensis</t>
+  </si>
+  <si>
+    <t>maenas</t>
+  </si>
+  <si>
+    <t>borealis</t>
+  </si>
+  <si>
+    <t>solidissima</t>
+  </si>
+  <si>
+    <t>polynyma</t>
+  </si>
+  <si>
+    <t>scombrus</t>
+  </si>
+  <si>
+    <t>monoceros</t>
+  </si>
+  <si>
+    <t>islandica</t>
+  </si>
+  <si>
+    <t>islandicus</t>
+  </si>
+  <si>
+    <t>magellanicus</t>
+  </si>
+  <si>
+    <t>sp.</t>
+  </si>
+  <si>
+    <t>mentella</t>
+  </si>
+  <si>
+    <t>fasciatus</t>
+  </si>
+  <si>
+    <t>norvegicus</t>
+  </si>
+  <si>
+    <t>lupus</t>
+  </si>
+  <si>
+    <t>intestinalis</t>
+  </si>
+  <si>
+    <t>carcharias</t>
+  </si>
+  <si>
+    <t>polymorpha</t>
+  </si>
+  <si>
+    <t>bugensis</t>
+  </si>
+  <si>
+    <t>irroratus</t>
+  </si>
+  <si>
+    <t>araneus</t>
+  </si>
+  <si>
+    <t>opilio</t>
+  </si>
+  <si>
+    <t>maia</t>
+  </si>
+  <si>
+    <t>grypus</t>
+  </si>
+  <si>
+    <t>vitulina</t>
+  </si>
+  <si>
+    <t>vitulina_mellonae</t>
+  </si>
+  <si>
+    <t>V_20</t>
+  </si>
+  <si>
+    <t>V_21</t>
+  </si>
+  <si>
+    <t>V_22</t>
+  </si>
+  <si>
+    <t>V_23</t>
+  </si>
+  <si>
+    <t>V_24</t>
+  </si>
+  <si>
+    <t>V_25</t>
+  </si>
+  <si>
+    <t>V_26</t>
+  </si>
+  <si>
+    <t>V_27</t>
+  </si>
+  <si>
+    <t>V_28</t>
+  </si>
+  <si>
+    <t>V_29</t>
+  </si>
+  <si>
+    <t>V_30</t>
+  </si>
+  <si>
+    <t>V_31</t>
+  </si>
+  <si>
+    <t>V_32</t>
+  </si>
+  <si>
+    <t>V_33</t>
+  </si>
+  <si>
+    <t>V_34</t>
+  </si>
+  <si>
+    <t>V_35</t>
+  </si>
+  <si>
+    <t>V_36</t>
+  </si>
+  <si>
+    <t>V_37</t>
+  </si>
+  <si>
+    <t>V_38</t>
+  </si>
+  <si>
+    <t>V_39</t>
+  </si>
+  <si>
+    <t>V_40</t>
+  </si>
+  <si>
+    <t>V_41</t>
+  </si>
+  <si>
+    <t>V_42</t>
+  </si>
+  <si>
+    <t>V_43</t>
+  </si>
+  <si>
+    <t>V_44</t>
+  </si>
+  <si>
+    <t>V_45</t>
+  </si>
+  <si>
+    <t>V_46</t>
+  </si>
+  <si>
+    <t>V_47</t>
+  </si>
+  <si>
+    <t>V_48</t>
+  </si>
+  <si>
+    <t>V_49</t>
+  </si>
+  <si>
+    <t>V_50</t>
+  </si>
+  <si>
+    <t>V_51</t>
+  </si>
+  <si>
+    <t>V_52</t>
+  </si>
+  <si>
+    <t>V_53</t>
+  </si>
+  <si>
+    <t>V_54</t>
+  </si>
+  <si>
+    <t>V_55</t>
+  </si>
+  <si>
+    <t>V_56</t>
+  </si>
+  <si>
+    <t>V_57</t>
+  </si>
+  <si>
+    <t>V_58</t>
+  </si>
+  <si>
+    <t>V_59</t>
+  </si>
+  <si>
+    <t>V_60</t>
+  </si>
+  <si>
+    <t>V_61</t>
+  </si>
+  <si>
+    <t>V_62</t>
+  </si>
+  <si>
+    <t>V_63</t>
+  </si>
+  <si>
+    <t>V_64</t>
+  </si>
+  <si>
+    <t>V_65</t>
+  </si>
+  <si>
+    <t>V_66</t>
+  </si>
+  <si>
+    <t>V_67</t>
+  </si>
+  <si>
+    <t>V_68</t>
+  </si>
+  <si>
+    <t>V_69</t>
+  </si>
+  <si>
+    <t>V_70</t>
+  </si>
+  <si>
+    <t>V_71</t>
+  </si>
+  <si>
+    <t>V_72</t>
+  </si>
+  <si>
+    <t>V_73</t>
+  </si>
+  <si>
+    <t>V_74</t>
+  </si>
+  <si>
+    <t>V_75</t>
+  </si>
+  <si>
+    <t>V_76</t>
+  </si>
+  <si>
+    <t>V_77</t>
+  </si>
+  <si>
+    <t>V_78</t>
+  </si>
+  <si>
+    <t>V_79</t>
+  </si>
+  <si>
+    <t>V_80</t>
+  </si>
+  <si>
+    <t>V_81</t>
+  </si>
+  <si>
+    <t>V_82</t>
+  </si>
+  <si>
+    <t>V_83</t>
+  </si>
+  <si>
+    <t>V_84</t>
+  </si>
+  <si>
+    <t>V_85</t>
+  </si>
+  <si>
+    <t>V_86</t>
+  </si>
+  <si>
+    <t>V_87</t>
+  </si>
+  <si>
+    <t>V_88</t>
+  </si>
+  <si>
+    <t>V_89</t>
+  </si>
+  <si>
+    <t>V_90</t>
+  </si>
+  <si>
+    <t>V_91</t>
+  </si>
+  <si>
+    <t>V_92</t>
+  </si>
+  <si>
+    <t>V_93</t>
+  </si>
+  <si>
+    <t>V_94</t>
+  </si>
+  <si>
+    <t>V_95</t>
+  </si>
+  <si>
+    <t>V_96</t>
+  </si>
+  <si>
+    <t>V_97</t>
+  </si>
+  <si>
+    <t>V_98</t>
+  </si>
+  <si>
+    <t>V_99</t>
+  </si>
+  <si>
+    <t>Congelation_EtOH</t>
+  </si>
+  <si>
+    <t>EDTA_DMSO</t>
+  </si>
+  <si>
+    <t>Personne_reception_extrait</t>
+  </si>
+  <si>
+    <t>Jour_reception_extrait</t>
+  </si>
+  <si>
+    <t>Mois_reception_extrait</t>
+  </si>
+  <si>
+    <t>Annee_reception_extrait</t>
+  </si>
+  <si>
+    <t>Eric_Parent</t>
+  </si>
+  <si>
+    <t>Gregoire_Cortial</t>
+  </si>
+  <si>
+    <t>Jade_Lariviere</t>
+  </si>
+  <si>
+    <t>Claudie_Bonnet</t>
+  </si>
+  <si>
+    <t>Domynick_Maltais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,6 +1366,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="5">
@@ -809,7 +1431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -829,6 +1451,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,11 +1775,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
@@ -1183,110 +1813,110 @@
     <col min="30" max="30" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33">
       <c r="A1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="W1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1310,475 +1940,475 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>20</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>21</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" t="s">
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" s="6" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>41</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>42</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>45</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>46</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>48</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>49</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>50</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>51</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
+        <v>218</v>
+      </c>
+      <c r="W3" t="s">
         <v>52</v>
       </c>
-      <c r="V3" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>53</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>54</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>56</v>
       </c>
-      <c r="AA3" t="s">
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" t="s">
+        <v>73</v>
+      </c>
+      <c r="T4" t="s">
+        <v>74</v>
+      </c>
+      <c r="U4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="15" thickBot="1">
+      <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" t="s">
-        <v>69</v>
-      </c>
-      <c r="O4" t="s">
-        <v>70</v>
-      </c>
-      <c r="P4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S4" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4" t="s">
-        <v>75</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>426</v>
+      </c>
+      <c r="H5" t="s">
+        <v>425</v>
+      </c>
+      <c r="I5" t="s">
+        <v>424</v>
+      </c>
+      <c r="J5" t="s">
+        <v>423</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S5" t="s">
+        <v>87</v>
+      </c>
+      <c r="T5" t="s">
+        <v>88</v>
+      </c>
+      <c r="U5" t="s">
+        <v>89</v>
+      </c>
+      <c r="V5" t="s">
+        <v>90</v>
+      </c>
+      <c r="W5" t="s">
+        <v>91</v>
+      </c>
+      <c r="X5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M5" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5" t="s">
-        <v>87</v>
-      </c>
-      <c r="O5" t="s">
-        <v>88</v>
-      </c>
-      <c r="P5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>90</v>
-      </c>
-      <c r="R5" t="s">
-        <v>91</v>
-      </c>
-      <c r="S5" t="s">
-        <v>92</v>
-      </c>
-      <c r="T5" t="s">
-        <v>93</v>
-      </c>
-      <c r="U5" t="s">
-        <v>94</v>
-      </c>
-      <c r="V5" t="s">
-        <v>95</v>
-      </c>
-      <c r="W5" t="s">
-        <v>96</v>
-      </c>
-      <c r="X5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>104</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="F7" t="s">
         <v>115</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="P6" s="1" t="s">
+      <c r="G7" t="s">
         <v>116</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="H7" t="s">
         <v>117</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="I7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="J7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" t="s">
+        <v>121</v>
+      </c>
+      <c r="M7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
         <v>123</v>
       </c>
-      <c r="J7" t="s">
+      <c r="F8" t="s">
         <v>124</v>
       </c>
-      <c r="K7" t="s">
+      <c r="G8" t="s">
         <v>125</v>
       </c>
-      <c r="L7" t="s">
+      <c r="H8" t="s">
         <v>126</v>
       </c>
-      <c r="M7" t="s">
+      <c r="I8" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="J8" t="s">
         <v>128</v>
       </c>
-      <c r="F8" t="s">
+      <c r="K8" t="s">
         <v>129</v>
       </c>
-      <c r="G8" t="s">
+      <c r="L8" t="s">
         <v>130</v>
       </c>
-      <c r="H8" t="s">
+      <c r="M8" t="s">
         <v>131</v>
       </c>
-      <c r="I8" t="s">
+      <c r="N8" t="s">
         <v>132</v>
       </c>
-      <c r="J8" t="s">
+      <c r="O8" t="s">
         <v>133</v>
       </c>
-      <c r="K8" t="s">
+      <c r="P8" t="s">
         <v>134</v>
       </c>
-      <c r="L8" t="s">
+      <c r="Q8" t="s">
         <v>135</v>
       </c>
-      <c r="M8" t="s">
+      <c r="R8" t="s">
         <v>136</v>
       </c>
-      <c r="N8" t="s">
-        <v>137</v>
-      </c>
-      <c r="O8" t="s">
-        <v>138</v>
-      </c>
-      <c r="P8" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>140</v>
-      </c>
-      <c r="R8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="9" spans="1:33" s="8" customFormat="1"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1788,211 +2418,1394 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:FR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="100" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:174">
       <c r="A1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="BE1" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="BF1" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="BM1" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="BN1" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="BP1" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="BQ1" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="BR1" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="BU1" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BV1" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="BW1" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="BX1" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="BY1" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="BZ1" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="CC1" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="CD1" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="CF1" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="CG1" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="CH1" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="CJ1" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="CK1" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="CL1" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="CM1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="CN1" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="CO1" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="CP1" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="CR1" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="CS1" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="CT1" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="CU1" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="CV1" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="CW1" s="4"/>
+      <c r="CX1" s="4"/>
+      <c r="CY1" s="4"/>
+      <c r="CZ1" s="4"/>
+      <c r="DA1" s="4"/>
+      <c r="DB1" s="4"/>
+      <c r="DC1" s="4"/>
+      <c r="DD1" s="4"/>
+      <c r="DE1" s="4"/>
+      <c r="DF1" s="4"/>
+      <c r="DG1" s="4"/>
+      <c r="DH1" s="4"/>
+      <c r="DI1" s="4"/>
+      <c r="DJ1" s="4"/>
+      <c r="DK1" s="4"/>
+      <c r="DL1" s="4"/>
+      <c r="DM1" s="4"/>
+      <c r="DN1" s="4"/>
+      <c r="DO1" s="4"/>
+      <c r="DP1" s="4"/>
+      <c r="DQ1" s="4"/>
+      <c r="DR1" s="4"/>
+      <c r="DS1" s="4"/>
+      <c r="DT1" s="4"/>
+      <c r="DU1" s="4"/>
+      <c r="DV1" s="4"/>
+      <c r="DW1" s="4"/>
+      <c r="DX1" s="4"/>
+      <c r="DY1" s="4"/>
+      <c r="DZ1" s="4"/>
+      <c r="EA1" s="4"/>
+      <c r="EB1" s="4"/>
+      <c r="EC1" s="4"/>
+      <c r="ED1" s="4"/>
+      <c r="EE1" s="4"/>
+      <c r="EF1" s="4"/>
+      <c r="EG1" s="4"/>
+      <c r="EH1" s="4"/>
+      <c r="EI1" s="4"/>
+      <c r="EJ1" s="4"/>
+      <c r="EK1" s="4"/>
+      <c r="EL1" s="4"/>
+      <c r="EM1" s="4"/>
+      <c r="EN1" s="4"/>
+      <c r="EO1" s="4"/>
+      <c r="EP1" s="4"/>
+      <c r="EQ1" s="4"/>
+      <c r="ER1" s="4"/>
+      <c r="ES1" s="4"/>
+      <c r="ET1" s="4"/>
+      <c r="EU1" s="4"/>
+      <c r="EV1" s="4"/>
+      <c r="EW1" s="4"/>
+      <c r="EX1" s="4"/>
+      <c r="EY1" s="4"/>
+      <c r="EZ1" s="4"/>
+      <c r="FA1" s="4"/>
+      <c r="FB1" s="4"/>
+      <c r="FC1" s="4"/>
+      <c r="FD1" s="4"/>
+      <c r="FE1" s="4"/>
+      <c r="FF1" s="4"/>
+      <c r="FG1" s="4"/>
+      <c r="FH1" s="4"/>
+      <c r="FI1" s="4"/>
+      <c r="FJ1" s="4"/>
+      <c r="FK1" s="4"/>
+      <c r="FL1" s="4"/>
+      <c r="FM1" s="4"/>
+      <c r="FN1" s="4"/>
+      <c r="FO1" s="4"/>
+      <c r="FP1" s="4"/>
+      <c r="FQ1" s="4"/>
+      <c r="FR1" s="4"/>
+    </row>
+    <row r="2" spans="1:174">
+      <c r="A2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="C2" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:174">
+      <c r="A3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:174">
+      <c r="A4" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:174">
+      <c r="A5" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" t="s">
+        <v>421</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:174">
+      <c r="A6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" t="s">
+        <v>421</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:174">
+      <c r="A7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:174">
+      <c r="A8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
         <v>187</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="C8" t="s">
         <v>188</v>
       </c>
-      <c r="I1" s="4" t="s">
+    </row>
+    <row r="9" spans="1:174">
+      <c r="A9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="E9" t="s">
         <v>190</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="F9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9" t="s">
+        <v>258</v>
+      </c>
+      <c r="J9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:174">
+      <c r="A10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:174">
+      <c r="A11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:174">
+      <c r="A12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" t="s">
         <v>204</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="D12" t="s">
         <v>205</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+    </row>
+    <row r="13" spans="1:174">
+      <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="B13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" t="s">
+        <v>247</v>
+      </c>
+      <c r="F13" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" t="s">
+        <v>249</v>
+      </c>
+      <c r="H13" t="s">
+        <v>250</v>
+      </c>
+      <c r="I13" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" t="s">
+        <v>252</v>
+      </c>
+      <c r="K13" t="s">
+        <v>253</v>
+      </c>
+      <c r="L13" t="s">
+        <v>254</v>
+      </c>
+      <c r="M13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:174">
+      <c r="A14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" t="s">
+        <v>247</v>
+      </c>
+      <c r="F14" t="s">
+        <v>248</v>
+      </c>
+      <c r="G14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H14" t="s">
+        <v>250</v>
+      </c>
+      <c r="I14" t="s">
+        <v>251</v>
+      </c>
+      <c r="J14" t="s">
+        <v>252</v>
+      </c>
+      <c r="K14" t="s">
+        <v>253</v>
+      </c>
+      <c r="L14" t="s">
+        <v>254</v>
+      </c>
+      <c r="M14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:174">
+      <c r="A15" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" t="s">
-        <v>199</v>
-      </c>
-      <c r="H7" t="s">
-        <v>200</v>
-      </c>
-      <c r="I7" t="s">
-        <v>201</v>
-      </c>
-      <c r="J7" t="s">
-        <v>202</v>
-      </c>
-      <c r="K7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D8" t="s">
-        <v>211</v>
-      </c>
-      <c r="E8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+      <c r="B15" t="s">
+        <v>244</v>
+      </c>
+      <c r="C15" t="s">
+        <v>245</v>
+      </c>
+      <c r="D15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F15" t="s">
+        <v>248</v>
+      </c>
+      <c r="G15" t="s">
+        <v>249</v>
+      </c>
+      <c r="H15" t="s">
+        <v>250</v>
+      </c>
+      <c r="I15" t="s">
+        <v>251</v>
+      </c>
+      <c r="J15" t="s">
+        <v>252</v>
+      </c>
+      <c r="K15" t="s">
+        <v>253</v>
+      </c>
+      <c r="L15" t="s">
+        <v>254</v>
+      </c>
+      <c r="M15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:174">
+      <c r="A16" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="A17" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="C18">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E10" t="s">
-        <v>215</v>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18">
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <v>12</v>
+      </c>
+      <c r="N18">
+        <v>13</v>
+      </c>
+      <c r="O18">
+        <v>14</v>
+      </c>
+      <c r="P18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="A19" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <v>9</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <v>11</v>
+      </c>
+      <c r="M19">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>13</v>
+      </c>
+      <c r="O19">
+        <v>14</v>
+      </c>
+      <c r="P19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="15" thickBot="1">
+      <c r="A20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>11</v>
+      </c>
+      <c r="M20">
+        <v>12</v>
+      </c>
+      <c r="N20">
+        <v>13</v>
+      </c>
+      <c r="O20">
+        <v>14</v>
+      </c>
+      <c r="P20">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="15" thickBot="1">
+      <c r="A21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="15" thickBot="1">
+      <c r="A22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q22" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="S22" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="T22" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="U22" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="V22" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="W22" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="X22" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y22" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="Z22" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="AA22" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="AB22" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC22" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15" thickBot="1">
+      <c r="A23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="O23" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="P23" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q23" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="R23" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="S23" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="T23" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="U23" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="V23" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="W23" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+    </row>
+    <row r="24" spans="1:29" ht="15" thickBot="1">
+      <c r="A24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="O24" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q24" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="R24" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="S24" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="T24" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="U24" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="V24" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="W24" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="X24" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y24" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="Z24" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="AA24" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB24" s="13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
+      <c r="A25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
+      <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:29">
+      <c r="A27" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
+      <c r="A28" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
+      <c r="A29" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
+      <c r="A30" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29">
+      <c r="A31" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
+      <c r="A32" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -2007,38 +3820,38 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2047,15 +3860,15 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2064,15 +3877,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2081,15 +3894,15 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>224</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2098,30 +3911,42 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2130,15 +3955,15 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2147,20 +3972,32 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2169,7 +4006,7 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2186,7 +4023,7 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Check numeric + well columns #1
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0FB5A9-22F6-4D40-BDE7-057131DC5DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BA071F-C277-4118-A901-2567A9A05488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ordre" sheetId="2" r:id="rId1"/>
-    <sheet name="Valeurs" sheetId="3" r:id="rId2"/>
-    <sheet name="ID" sheetId="4" r:id="rId3"/>
-    <sheet name="Type" sheetId="5" r:id="rId4"/>
+    <sheet name="NOTES" sheetId="9" r:id="rId1"/>
+    <sheet name="Ordre" sheetId="2" r:id="rId2"/>
+    <sheet name="Valeurs" sheetId="3" r:id="rId3"/>
+    <sheet name="ID" sheetId="4" r:id="rId4"/>
     <sheet name="Date" sheetId="7" r:id="rId5"/>
-    <sheet name="Plaque" sheetId="8" r:id="rId6"/>
+    <sheet name="Others" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="447">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -1341,6 +1341,45 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Feuille</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Ordre</t>
+  </si>
+  <si>
+    <t>Liste dans l'ordre le nom exacte que les colonnes de chaque table doivent prendre. Doivent correspondre aux en-têtes des gabarits</t>
+  </si>
+  <si>
+    <t>Valeurs</t>
+  </si>
+  <si>
+    <t>Pour certaines colonnes, la liste des valeurs possibles</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Format pour les quelques colonnes avec ID particulier, p.ex. ADN_20_00001</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Colonnes qui format des dates</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>puit</t>
   </si>
 </sst>
 </file>
@@ -1789,11 +1828,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2083E8D-166D-4FCC-8936-54C727A4D55E}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="109.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B4" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2433,12 +2531,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
   <dimension ref="A1:FR33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
@@ -3832,12 +3930,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C72DEFF-7720-4B8E-B4D3-1283341468DF}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD8"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4005,26 +4103,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A5ED52-15D8-45D5-AF42-FD6A8E34DAD4}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4357,15 +4441,211 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985FA1D1-A43E-4AC4-948A-2E29D5BA4122}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1">
+      <c r="A16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1">
+      <c r="A17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>446</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Split min max profondeur
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BA071F-C277-4118-A901-2567A9A05488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443A2974-EF4D-4EAB-A062-C89720BD9449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="285" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="448">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Referentiel_geographique</t>
   </si>
   <si>
-    <t>Profondeur_m</t>
-  </si>
-  <si>
     <t>Annee_echantillonnage</t>
   </si>
   <si>
@@ -1380,6 +1377,12 @@
   </si>
   <si>
     <t>puit</t>
+  </si>
+  <si>
+    <t>Profondeur_m_debut</t>
+  </si>
+  <si>
+    <t>Profondeur_m_fin</t>
   </si>
 </sst>
 </file>
@@ -1842,42 +1845,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B2" t="s">
         <v>436</v>
-      </c>
-      <c r="B2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B3" t="s">
         <v>438</v>
-      </c>
-      <c r="B3" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4" t="s">
         <v>440</v>
-      </c>
-      <c r="B4" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" t="s">
         <v>442</v>
-      </c>
-      <c r="B5" t="s">
-        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -1890,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1917,7 +1920,7 @@
     <col min="19" max="19" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.5546875" bestFit="1" customWidth="1"/>
@@ -1930,108 +1933,108 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="W1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="AD1" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="AE1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2055,7 +2058,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
@@ -2094,433 +2097,436 @@
         <v>18</v>
       </c>
       <c r="V2" t="s">
+        <v>446</v>
+      </c>
+      <c r="W2" t="s">
+        <v>447</v>
+      </c>
+      <c r="X2" t="s">
         <v>19</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>20</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>26</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>41</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>44</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>45</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>47</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>48</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>49</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>50</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
+        <v>217</v>
+      </c>
+      <c r="W3" t="s">
         <v>51</v>
       </c>
-      <c r="V3" t="s">
-        <v>218</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>52</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>55</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>61</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>62</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>63</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>64</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>65</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>66</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>67</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>68</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>69</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>70</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>71</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>72</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>73</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>74</v>
-      </c>
-      <c r="U4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>77</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>425</v>
+      </c>
+      <c r="H5" t="s">
+        <v>424</v>
+      </c>
+      <c r="I5" t="s">
+        <v>423</v>
+      </c>
+      <c r="J5" t="s">
+        <v>422</v>
+      </c>
+      <c r="K5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" t="s">
-        <v>426</v>
-      </c>
-      <c r="H5" t="s">
-        <v>425</v>
-      </c>
-      <c r="I5" t="s">
-        <v>424</v>
-      </c>
-      <c r="J5" t="s">
-        <v>423</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>79</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>80</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>82</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>83</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>84</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>85</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>86</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>87</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>88</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>89</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>90</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>91</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>92</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>93</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>94</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>95</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>96</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>97</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>98</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>99</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:33">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
         <v>114</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>115</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>116</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>117</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>118</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>119</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>120</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>121</v>
-      </c>
-      <c r="M7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:33">
       <c r="A8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
       <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" t="s">
         <v>123</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>124</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>125</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>126</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>127</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>128</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>129</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>130</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>131</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>132</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>133</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>134</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>135</v>
-      </c>
-      <c r="R8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:33" s="8" customFormat="1"/>
@@ -2573,304 +2579,304 @@
   <sheetData>
     <row r="1" spans="1:174">
       <c r="A1" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="P1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="U1" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="CN1" s="4" t="s">
+      <c r="CO1" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CP1" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="CP1" s="4" t="s">
+      <c r="CQ1" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="CQ1" s="4" t="s">
+      <c r="CR1" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="CR1" s="4" t="s">
+      <c r="CS1" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="CS1" s="4" t="s">
+      <c r="CT1" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="CT1" s="4" t="s">
+      <c r="CU1" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="CU1" s="4" t="s">
+      <c r="CV1" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="CV1" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="CW1" s="4"/>
       <c r="CX1" s="4"/>
@@ -2949,244 +2955,244 @@
     </row>
     <row r="2" spans="1:174">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
         <v>185</v>
       </c>
-      <c r="C2" t="s">
-        <v>186</v>
-      </c>
       <c r="D2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" t="s">
         <v>221</v>
-      </c>
-      <c r="E2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:174">
       <c r="A3" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
         <v>185</v>
       </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:174">
       <c r="A4" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" t="s">
         <v>260</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:174">
       <c r="A5" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" t="s">
         <v>260</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:174">
       <c r="A6" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" t="s">
         <v>260</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>420</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:174">
       <c r="A7" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" t="s">
         <v>226</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="F7" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q7" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="P7" s="11" t="s">
+      <c r="R7" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="Q7" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="R7" s="11" t="s">
+      <c r="S7" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="T7" s="11" t="s">
         <v>237</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:174">
       <c r="A8" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" t="s">
         <v>187</v>
-      </c>
-      <c r="C8" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:174">
       <c r="A9" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" t="s">
         <v>256</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" t="s">
+        <v>192</v>
+      </c>
+      <c r="I9" t="s">
         <v>257</v>
       </c>
-      <c r="D9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E9" t="s">
-        <v>190</v>
-      </c>
-      <c r="F9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G9" t="s">
-        <v>192</v>
-      </c>
-      <c r="H9" t="s">
-        <v>193</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>258</v>
-      </c>
-      <c r="J9" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:174">
       <c r="A10" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" t="s">
         <v>200</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>201</v>
-      </c>
-      <c r="D10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:174">
       <c r="A11" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3200,16 +3206,16 @@
     </row>
     <row r="12" spans="1:174">
       <c r="A12" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" t="s">
         <v>203</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>204</v>
-      </c>
-      <c r="D12" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:174">
@@ -3217,143 +3223,143 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" t="s">
         <v>244</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>245</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>246</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>247</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>248</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>249</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>250</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>251</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>252</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>253</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>254</v>
-      </c>
-      <c r="M13" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:174">
       <c r="A14" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" t="s">
         <v>244</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>245</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>246</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>247</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>248</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>249</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>250</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>251</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>252</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>253</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>254</v>
-      </c>
-      <c r="M14" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:174">
       <c r="A15" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C15" t="s">
         <v>244</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>245</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>246</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>247</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>248</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>249</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>250</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>251</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>252</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>253</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>254</v>
-      </c>
-      <c r="M15" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:174">
       <c r="A16" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3453,7 +3459,7 @@
     </row>
     <row r="20" spans="1:29" ht="15" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3506,173 +3512,173 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="15" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="G22" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="H22" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="H22" s="13" t="s">
+      <c r="I22" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="J22" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="K22" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="L22" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="L22" s="13" t="s">
+      <c r="M22" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="N22" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="N22" s="13" t="s">
+      <c r="O22" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q22" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="O22" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q22" s="13" t="s">
+      <c r="R22" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="R22" s="13" t="s">
+      <c r="S22" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="S22" s="13" t="s">
+      <c r="T22" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="T22" s="13" t="s">
+      <c r="U22" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="U22" s="13" t="s">
+      <c r="V22" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="V22" s="13" t="s">
+      <c r="W22" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="W22" s="13" t="s">
+      <c r="X22" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="X22" s="13" t="s">
+      <c r="Y22" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="Y22" s="13" t="s">
+      <c r="Z22" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="Z22" s="13" t="s">
+      <c r="AA22" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="AA22" s="13" t="s">
+      <c r="AB22" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="AB22" s="13" t="s">
-        <v>291</v>
-      </c>
       <c r="AC22" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="15" thickBot="1">
       <c r="A23" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="G23" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="H23" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="I23" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="K23" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="L23" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="N23" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="N23" s="13" t="s">
+      <c r="O23" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="P23" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="P23" s="13" t="s">
+      <c r="Q23" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="Q23" s="13" t="s">
+      <c r="R23" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="S23" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="T23" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="T23" s="13" t="s">
+      <c r="U23" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="U23" s="13" t="s">
+      <c r="V23" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="V23" s="13" t="s">
+      <c r="W23" s="13" t="s">
         <v>312</v>
-      </c>
-      <c r="W23" s="13" t="s">
-        <v>313</v>
       </c>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
@@ -3682,228 +3688,228 @@
     </row>
     <row r="24" spans="1:29" ht="15" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="D24" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="E24" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="H24" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="I24" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="J24" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="K24" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="L24" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="M24" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="M24" s="13" t="s">
+      <c r="N24" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="N24" s="13" t="s">
+      <c r="O24" s="13" t="s">
         <v>326</v>
       </c>
-      <c r="O24" s="13" t="s">
+      <c r="P24" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="P24" s="13" t="s">
+      <c r="Q24" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="Q24" s="13" t="s">
+      <c r="R24" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="S24" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="S24" s="13" t="s">
+      <c r="T24" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="T24" s="13" t="s">
+      <c r="U24" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="U24" s="13" t="s">
+      <c r="V24" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="V24" s="13" t="s">
+      <c r="W24" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="W24" s="13" t="s">
+      <c r="X24" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="X24" s="13" t="s">
+      <c r="Y24" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="Y24" s="13" t="s">
+      <c r="Z24" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="Z24" s="13" t="s">
+      <c r="AA24" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="AA24" s="13" t="s">
+      <c r="AB24" s="13" t="s">
         <v>339</v>
-      </c>
-      <c r="AB24" s="13" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="E25" s="14" t="s">
         <v>429</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="F25" s="14" t="s">
         <v>430</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>430</v>
       </c>
       <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E27" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B30" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="D31" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="E31" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3911,16 +3917,16 @@
         <v>6</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="D33" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="E33" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3946,19 +3952,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3966,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -3975,15 +3981,15 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3992,15 +3998,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4009,15 +4015,15 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -4026,15 +4032,15 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -4043,15 +4049,15 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -4060,7 +4066,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4068,7 +4074,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -4077,15 +4083,15 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -4094,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -4107,8 +4113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A5ED52-15D8-45D5-AF42-FD6A8E34DAD4}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4123,18 +4129,18 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1" t="s">
         <v>432</v>
-      </c>
-      <c r="C1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>1980</v>
@@ -4145,7 +4151,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>1980</v>
@@ -4156,7 +4162,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.6">
       <c r="A4" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4">
         <v>1980</v>
@@ -4167,7 +4173,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>1980</v>
@@ -4178,7 +4184,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B6">
         <v>1980</v>
@@ -4200,7 +4206,7 @@
     </row>
     <row r="8" spans="1:13" ht="16.2" thickBot="1">
       <c r="A8" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>1980</v>
@@ -4214,7 +4220,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>1980</v>
@@ -4225,7 +4231,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10">
         <v>1980</v>
@@ -4236,7 +4242,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4247,7 +4253,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4258,7 +4264,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.6">
       <c r="A13" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -4269,7 +4275,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4280,7 +4286,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4302,7 +4308,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4313,7 +4319,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4324,7 +4330,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4335,7 +4341,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4346,7 +4352,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -4357,7 +4363,7 @@
     </row>
     <row r="22" spans="1:3" ht="16.2" thickBot="1">
       <c r="A22" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4368,7 +4374,7 @@
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4379,7 +4385,7 @@
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4401,7 +4407,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4412,7 +4418,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4423,7 +4429,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4442,10 +4448,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4455,10 +4461,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4466,7 +4472,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4474,175 +4480,183 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>446</v>
       </c>
       <c r="B4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>447</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1">
+      <c r="A16" t="s">
         <v>91</v>
       </c>
-      <c r="B14" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1">
-      <c r="A15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1">
-      <c r="A16" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="B16" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>130</v>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>446</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvement step 1 to 6
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BonnetC\Desktop\LabGen\GitHub\BD-LabGeno-IML_gestion\inst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62204A0-CBCB-4793-81EF-6BA609DF6201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399DDA81-E709-475E-85B4-BC50FAC7BD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-420" yWindow="555" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="459">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -122,15 +122,6 @@
     <t>Notes_groupe</t>
   </si>
   <si>
-    <t>Specimen</t>
-  </si>
-  <si>
-    <t>Tissu</t>
-  </si>
-  <si>
-    <t>ExtraitADN_ARN</t>
-  </si>
-  <si>
     <t>Sexage</t>
   </si>
   <si>
@@ -515,9 +506,6 @@
     <t>Col_21</t>
   </si>
   <si>
-    <t>Groupe</t>
-  </si>
-  <si>
     <t>Col_22</t>
   </si>
   <si>
@@ -707,45 +695,6 @@
     <t>Sec</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>MK</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>FO</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>IC</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>BR</t>
-  </si>
-  <si>
-    <t>LU</t>
-  </si>
-  <si>
     <t>V_15</t>
   </si>
   <si>
@@ -1398,6 +1347,75 @@
   </si>
   <si>
     <t>PON_010307_V01</t>
+  </si>
+  <si>
+    <t>Groupes</t>
+  </si>
+  <si>
+    <t>Specimens</t>
+  </si>
+  <si>
+    <t>Tissus</t>
+  </si>
+  <si>
+    <t>Extraits_ADN_ARN</t>
+  </si>
+  <si>
+    <t>Blubber</t>
+  </si>
+  <si>
+    <t>Eye</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Kidney</t>
+  </si>
+  <si>
+    <t>Liver</t>
+  </si>
+  <si>
+    <t>Muscle</t>
+  </si>
+  <si>
+    <t>Muktuk</t>
+  </si>
+  <si>
+    <t>Skin</t>
+  </si>
+  <si>
+    <t>Tooth</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Mantle</t>
+  </si>
+  <si>
+    <t>Foot</t>
+  </si>
+  <si>
+    <t>Gonade</t>
+  </si>
+  <si>
+    <t>Stomacal_content</t>
+  </si>
+  <si>
+    <t>Intestinal_content</t>
+  </si>
+  <si>
+    <t>Qtip</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Brain</t>
+  </si>
+  <si>
+    <t>Lung</t>
   </si>
 </sst>
 </file>
@@ -1853,49 +1871,49 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="109.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="B3" t="s">
-        <v>435</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="B5" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -1908,148 +1926,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="6" t="s">
-        <v>158</v>
+        <v>436</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2073,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
@@ -2112,10 +2130,10 @@
         <v>18</v>
       </c>
       <c r="V2" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
       <c r="W2" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="X2" t="s">
         <v>19</v>
@@ -2144,404 +2162,404 @@
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>437</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>41</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>42</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>43</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>44</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>46</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>47</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
+        <v>210</v>
+      </c>
+      <c r="W3" t="s">
         <v>48</v>
       </c>
-      <c r="T3" t="s">
+      <c r="X3" t="s">
         <v>49</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Y3" t="s">
         <v>50</v>
       </c>
-      <c r="V3" t="s">
-        <v>214</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>51</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>52</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>438</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>57</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>58</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>59</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>61</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>62</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>63</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>64</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>65</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>66</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>67</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>68</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>70</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>71</v>
       </c>
-      <c r="S4" t="s">
+    </row>
+    <row r="5" spans="1:33" ht="15" thickBot="1">
+      <c r="A5" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="T4" t="s">
+      <c r="E5" t="s">
         <v>73</v>
       </c>
-      <c r="U4" t="s">
+      <c r="F5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" thickBot="1">
-      <c r="A5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
+        <v>405</v>
+      </c>
+      <c r="H5" t="s">
+        <v>404</v>
+      </c>
+      <c r="I5" t="s">
+        <v>403</v>
+      </c>
+      <c r="J5" t="s">
+        <v>402</v>
+      </c>
+      <c r="K5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" t="s">
+      <c r="L5" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s">
+      <c r="M5" t="s">
         <v>77</v>
       </c>
-      <c r="G5" t="s">
-        <v>422</v>
-      </c>
-      <c r="H5" t="s">
-        <v>421</v>
-      </c>
-      <c r="I5" t="s">
-        <v>420</v>
-      </c>
-      <c r="J5" t="s">
-        <v>419</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>78</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>79</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>80</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>81</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>82</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>83</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>84</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>85</v>
       </c>
-      <c r="S5" t="s">
+      <c r="V5" t="s">
         <v>86</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>87</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>88</v>
       </c>
-      <c r="V5" t="s">
+      <c r="Y5" t="s">
         <v>89</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Z5" t="s">
         <v>90</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AA5" t="s">
         <v>91</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AB5" t="s">
         <v>92</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AC5" t="s">
         <v>93</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AD5" t="s">
         <v>94</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AE5" t="s">
         <v>95</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AF5" t="s">
         <v>96</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="P6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="S6" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:33">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" t="s">
         <v>113</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>114</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>115</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
         <v>116</v>
       </c>
-      <c r="I7" t="s">
+      <c r="L7" t="s">
         <v>117</v>
       </c>
-      <c r="J7" t="s">
+      <c r="M7" t="s">
         <v>118</v>
-      </c>
-      <c r="K7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L7" t="s">
-        <v>120</v>
-      </c>
-      <c r="M7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:33">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s">
         <v>122</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>123</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>124</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>125</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>126</v>
       </c>
-      <c r="J8" t="s">
+      <c r="M8" t="s">
         <v>127</v>
       </c>
-      <c r="K8" t="s">
+      <c r="N8" t="s">
         <v>128</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>129</v>
       </c>
-      <c r="M8" t="s">
+      <c r="P8" t="s">
         <v>130</v>
       </c>
-      <c r="N8" t="s">
+      <c r="Q8" t="s">
         <v>131</v>
       </c>
-      <c r="O8" t="s">
+      <c r="R8" t="s">
         <v>132</v>
-      </c>
-      <c r="P8" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>134</v>
-      </c>
-      <c r="R8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:33" s="8" customFormat="1"/>
@@ -2557,340 +2575,340 @@
   <dimension ref="A1:FR33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="41.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="100" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="100" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:174">
       <c r="A1" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="P1" s="4" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="U1" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="AL1" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CO1" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CP1" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CQ1" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CR1" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CS1" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CT1" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CU1" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CV1" s="4" t="s">
         <v>399</v>
-      </c>
-      <c r="CF1" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="CG1" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="CH1" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="CI1" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="CJ1" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="CK1" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="CL1" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="CM1" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="CN1" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO1" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="CP1" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="CQ1" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="CR1" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="CS1" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="CT1" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="CU1" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="CV1" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="CW1" s="4"/>
       <c r="CX1" s="4"/>
@@ -2969,259 +2987,259 @@
     </row>
     <row r="2" spans="1:174">
       <c r="A2" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:174">
       <c r="A3" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:174">
       <c r="A4" s="10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:174">
       <c r="A5" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="D5" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:174">
       <c r="A6" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="D6" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:174">
       <c r="A7" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>222</v>
+        <v>440</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>441</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>184</v>
+        <v>442</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>224</v>
+        <v>443</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>225</v>
+        <v>444</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>185</v>
+        <v>445</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>226</v>
+        <v>446</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>208</v>
+        <v>447</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>209</v>
+        <v>448</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>217</v>
+        <v>449</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>228</v>
+        <v>450</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>229</v>
+        <v>451</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>207</v>
+        <v>452</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>230</v>
+        <v>453</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>231</v>
+        <v>454</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>227</v>
+        <v>455</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>232</v>
+        <v>456</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>233</v>
+        <v>457</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>234</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:174">
       <c r="A8" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D8" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:174">
       <c r="A9" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="C9" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="D9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" t="s">
         <v>188</v>
       </c>
-      <c r="E9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F9" t="s">
-        <v>190</v>
-      </c>
-      <c r="G9" t="s">
-        <v>191</v>
-      </c>
-      <c r="H9" t="s">
-        <v>192</v>
-      </c>
       <c r="I9" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="J9" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:174">
       <c r="A10" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="C10" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="D10" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="G10" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="H10" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
     </row>
     <row r="11" spans="1:174">
       <c r="A11" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3235,16 +3253,16 @@
     </row>
     <row r="12" spans="1:174">
       <c r="A12" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:174">
@@ -3252,143 +3270,143 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E13" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="F13" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="G13" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="H13" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="I13" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="J13" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="K13" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="L13" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="M13" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:174">
       <c r="A14" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="C14" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E14" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="F14" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="G14" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="H14" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="I14" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="J14" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="K14" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="L14" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="M14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:174">
       <c r="A15" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="C15" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E15" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="F15" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="G15" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="H15" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="I15" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="J15" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="K15" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="L15" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="M15" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:174">
       <c r="A16" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3486,9 +3504,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15.75" thickBot="1">
+    <row r="20" spans="1:29" ht="15" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3536,178 +3554,178 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15.75" thickBot="1">
+    <row r="21" spans="1:29" ht="15" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="29.4" thickBot="1">
+      <c r="A22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q22" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="S22" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="T22" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="U22" s="13" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" ht="30.75" thickBot="1">
-      <c r="A22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="13" t="s">
+      <c r="V22" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="W22" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="X22" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="Y22" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="Z22" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="H22" s="13" t="s">
+      <c r="AA22" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="AB22" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="AC22" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15" thickBot="1">
+      <c r="A23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="C23" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="L22" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="N22" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="O22" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q22" s="13" t="s">
+      <c r="G23" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="R22" s="13" t="s">
+      <c r="H23" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="S22" s="13" t="s">
+      <c r="I23" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="T22" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="U22" s="13" t="s">
+      <c r="K23" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="V22" s="13" t="s">
+      <c r="L23" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="W22" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="X22" s="13" t="s">
+      <c r="N23" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="Y22" s="13" t="s">
+      <c r="O23" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="Z22" s="13" t="s">
+      <c r="P23" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="AA22" s="13" t="s">
+      <c r="Q23" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="AB22" s="13" t="s">
+      <c r="R23" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="AC22" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" ht="30.75" thickBot="1">
-      <c r="A23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="13" t="s">
+      <c r="S23" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="T23" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="U23" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="V23" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="W23" s="13" t="s">
         <v>292</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="N23" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="O23" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="P23" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q23" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="R23" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="S23" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="T23" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="U23" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="V23" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="W23" s="13" t="s">
-        <v>309</v>
       </c>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
@@ -3715,230 +3733,230 @@
       <c r="AA23" s="8"/>
       <c r="AB23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="30.75" thickBot="1">
+    <row r="24" spans="1:29" ht="15" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B24" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="O24" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q24" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="R24" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="S24" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="T24" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="U24" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="V24" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="W24" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="X24" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="Y24" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="Z24" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="AA24" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="AB24" s="13" t="s">
         <v>319</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="M24" s="13" t="s">
-        <v>321</v>
-      </c>
-      <c r="N24" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="O24" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="P24" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="Q24" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="R24" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="S24" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="T24" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="U24" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="V24" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="W24" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="X24" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="Y24" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="Z24" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="AA24" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="AB24" s="13" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3946,16 +3964,16 @@
         <v>6</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -3973,27 +3991,27 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4001,7 +4019,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -4010,15 +4028,15 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4027,15 +4045,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4044,15 +4062,15 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -4061,15 +4079,15 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -4078,15 +4096,15 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -4095,7 +4113,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4103,7 +4121,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -4112,15 +4130,15 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -4129,7 +4147,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4146,30 +4164,30 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="C1" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>1980</v>
@@ -4189,9 +4207,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75">
+    <row r="4" spans="1:13" ht="15.6">
       <c r="A4" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4">
         <v>1980</v>
@@ -4202,7 +4220,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>1980</v>
@@ -4213,7 +4231,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="B6">
         <v>1980</v>
@@ -4222,7 +4240,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
+    <row r="7" spans="1:13" ht="15" thickBot="1">
       <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
@@ -4233,9 +4251,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1">
+    <row r="8" spans="1:13" ht="16.2" thickBot="1">
       <c r="A8" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>1980</v>
@@ -4249,7 +4267,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>1980</v>
@@ -4260,7 +4278,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B10">
         <v>1980</v>
@@ -4271,7 +4289,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4291,9 +4309,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75">
+    <row r="13" spans="1:13" ht="15.6">
       <c r="A13" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -4304,7 +4322,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4315,7 +4333,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="15" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4337,7 +4355,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4348,7 +4366,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4359,7 +4377,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4370,7 +4388,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4390,9 +4408,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.5" thickBot="1">
+    <row r="22" spans="1:3" ht="16.2" thickBot="1">
       <c r="A22" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4401,9 +4419,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1">
+    <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4412,9 +4430,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+    <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="17" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4423,7 +4441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+    <row r="25" spans="1:3" ht="15" thickBot="1">
       <c r="A25" s="17" t="s">
         <v>4</v>
       </c>
@@ -4436,7 +4454,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4447,7 +4465,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4458,7 +4476,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4481,20 +4499,20 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4502,7 +4520,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4510,183 +4528,183 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
       <c r="B4" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="B5" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sexage column name change
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B9ABDA-6589-473E-A32B-E67E514E87CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE845E2-DF8B-4F08-A7ED-6C24D828F115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="489">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -2057,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2611,24 +2611,21 @@
         <v>471</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="M7" s="16" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2737,7 +2734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
   <dimension ref="A1:FR37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -4005,7 +4002,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="28.8">
+    <row r="26" spans="1:29">
       <c r="A26" s="6" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Correct typo in Hormones sheet
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE845E2-DF8B-4F08-A7ED-6C24D828F115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4714E20D-E128-4CE3-81FA-503B4070668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
@@ -1463,9 +1463,6 @@
     <t>colias</t>
   </si>
   <si>
-    <t>Hormone</t>
-  </si>
-  <si>
     <t>Sandrine_Guillou</t>
   </si>
   <si>
@@ -1506,6 +1503,9 @@
   </si>
   <si>
     <t>Frederique_Paquin</t>
+  </si>
+  <si>
+    <t>Hormones</t>
   </si>
 </sst>
 </file>
@@ -2057,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2702,25 +2702,25 @@
     </row>
     <row r="9" spans="1:33" s="22" customFormat="1" ht="15" thickBot="1">
       <c r="A9" s="17" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>480</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>481</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>482</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="F9" s="25" t="s">
         <v>483</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="G9" s="25" t="s">
         <v>484</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -4019,13 +4019,13 @@
         <v>396</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G26" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="H26" s="10" t="s">
         <v>479</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -4096,10 +4096,10 @@
         <v>396</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -4183,24 +4183,24 @@
         <v>102</v>
       </c>
       <c r="B36" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>477</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="26" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>486</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -4936,7 +4936,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B26" t="s">
         <v>411</v>

</xml_diff>

<commit_message>
Correct NA and columns name problem
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79D71F5-86B9-4C87-BAB1-6D8C53DE2280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD826135-B40F-4724-B8EC-D4A856612862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="491">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -323,15 +323,6 @@
     <t>Notes_extraitADN</t>
   </si>
   <si>
-    <t>No_puits</t>
-  </si>
-  <si>
-    <t>Concentration</t>
-  </si>
-  <si>
-    <t>Volume_preleve</t>
-  </si>
-  <si>
     <t>Responsable_preparation</t>
   </si>
   <si>
@@ -387,12 +378,6 @@
   </si>
   <si>
     <t>Nom_Projet</t>
-  </si>
-  <si>
-    <t>No_puits_F</t>
-  </si>
-  <si>
-    <t>No_puits_R</t>
   </si>
   <si>
     <t>Sequence_consensus</t>
@@ -2030,42 +2015,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B4" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -2078,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2119,108 +2104,108 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="Z1" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="17" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>0</v>
@@ -2244,7 +2229,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>7</v>
@@ -2283,10 +2268,10 @@
         <v>18</v>
       </c>
       <c r="V2" s="16" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="W2" s="16" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="X2" s="16" t="s">
         <v>19</v>
@@ -2315,7 +2300,7 @@
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="17" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>0</v>
@@ -2378,7 +2363,7 @@
         <v>47</v>
       </c>
       <c r="V3" s="16" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="W3" s="16" t="s">
         <v>48</v>
@@ -2398,7 +2383,7 @@
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="17" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>29</v>
@@ -2463,7 +2448,7 @@
     </row>
     <row r="5" spans="1:33" ht="15" thickBot="1">
       <c r="A5" s="17" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>29</v>
@@ -2481,16 +2466,16 @@
         <v>74</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>76</v>
@@ -2541,13 +2526,13 @@
         <v>91</v>
       </c>
       <c r="AA5" s="16" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="AB5" s="16" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="AC5" s="16" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="AD5" s="16" t="s">
         <v>92</v>
@@ -2558,7 +2543,7 @@
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>29</v>
@@ -2567,49 +2552,49 @@
         <v>72</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H6" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="L6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="M6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="N6" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="O6" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="P6" s="18" t="s">
         <v>75</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="15" thickBot="1">
@@ -2623,36 +2608,36 @@
         <v>72</v>
       </c>
       <c r="D7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="H7" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>466</v>
-      </c>
-      <c r="G7" s="16" t="s">
+      <c r="I7" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="K7" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="L7" s="16" t="s">
         <v>111</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="15" thickBot="1">
       <c r="A8" s="17" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>72</v>
@@ -2661,87 +2646,87 @@
         <v>29</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>439</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>442</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>443</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>467</v>
-      </c>
-      <c r="H8" s="18" t="s">
+      <c r="Q8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="T8" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="U8" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="V8" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>445</v>
-      </c>
-      <c r="L8" s="16" t="s">
+      <c r="W8" s="16" t="s">
         <v>448</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>449</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>450</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>451</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>454</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>452</v>
-      </c>
-      <c r="W8" s="16" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:33" s="22" customFormat="1" ht="15" thickBot="1">
       <c r="A9" s="17" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -2755,7 +2740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
   <dimension ref="A1:FR37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -2792,304 +2777,304 @@
   <sheetData>
     <row r="1" spans="1:174">
       <c r="A1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CM1" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="CL1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CV1" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="CR1" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="CS1" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="CT1" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="CU1" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="CV1" s="3" t="s">
-        <v>386</v>
       </c>
       <c r="CW1" s="3"/>
       <c r="CX1" s="3"/>
@@ -3171,88 +3156,88 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:174">
       <c r="A3" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:174">
       <c r="A4" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:174">
       <c r="A5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" t="s">
+        <v>382</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5" t="s">
-        <v>387</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:174">
@@ -3260,28 +3245,28 @@
         <v>60</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D6" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:174">
@@ -3289,67 +3274,67 @@
         <v>64</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="S7" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="P7" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>440</v>
-      </c>
       <c r="U7" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:174">
@@ -3357,13 +3342,13 @@
         <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:174">
@@ -3371,31 +3356,31 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I9" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:174">
@@ -3403,25 +3388,25 @@
         <v>81</v>
       </c>
       <c r="B10" t="s">
+        <v>406</v>
+      </c>
+      <c r="C10" t="s">
+        <v>407</v>
+      </c>
+      <c r="D10" t="s">
+        <v>408</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F10" t="s">
+        <v>410</v>
+      </c>
+      <c r="G10" t="s">
         <v>411</v>
       </c>
-      <c r="C10" t="s">
+      <c r="H10" t="s">
         <v>412</v>
-      </c>
-      <c r="D10" t="s">
-        <v>413</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="F10" t="s">
-        <v>415</v>
-      </c>
-      <c r="G10" t="s">
-        <v>416</v>
-      </c>
-      <c r="H10" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:174">
@@ -3440,16 +3425,16 @@
     </row>
     <row r="12" spans="1:174">
       <c r="A12" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:174">
@@ -3457,40 +3442,40 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" t="s">
         <v>210</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
         <v>211</v>
       </c>
-      <c r="D13" t="s">
+      <c r="I13" t="s">
         <v>212</v>
       </c>
-      <c r="E13" t="s">
+      <c r="J13" t="s">
         <v>213</v>
       </c>
-      <c r="F13" t="s">
+      <c r="K13" t="s">
         <v>214</v>
       </c>
-      <c r="G13" t="s">
+      <c r="L13" t="s">
         <v>215</v>
       </c>
-      <c r="H13" t="s">
+      <c r="M13" t="s">
         <v>216</v>
-      </c>
-      <c r="I13" t="s">
-        <v>217</v>
-      </c>
-      <c r="J13" t="s">
-        <v>218</v>
-      </c>
-      <c r="K13" t="s">
-        <v>219</v>
-      </c>
-      <c r="L13" t="s">
-        <v>220</v>
-      </c>
-      <c r="M13" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:174">
@@ -3498,40 +3483,40 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" t="s">
+        <v>209</v>
+      </c>
+      <c r="G14" t="s">
         <v>210</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H14" t="s">
         <v>211</v>
       </c>
-      <c r="D14" t="s">
+      <c r="I14" t="s">
         <v>212</v>
       </c>
-      <c r="E14" t="s">
+      <c r="J14" t="s">
         <v>213</v>
       </c>
-      <c r="F14" t="s">
+      <c r="K14" t="s">
         <v>214</v>
       </c>
-      <c r="G14" t="s">
+      <c r="L14" t="s">
         <v>215</v>
       </c>
-      <c r="H14" t="s">
+      <c r="M14" t="s">
         <v>216</v>
-      </c>
-      <c r="I14" t="s">
-        <v>217</v>
-      </c>
-      <c r="J14" t="s">
-        <v>218</v>
-      </c>
-      <c r="K14" t="s">
-        <v>219</v>
-      </c>
-      <c r="L14" t="s">
-        <v>220</v>
-      </c>
-      <c r="M14" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:174">
@@ -3539,56 +3524,56 @@
         <v>61</v>
       </c>
       <c r="B15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F15" t="s">
+        <v>209</v>
+      </c>
+      <c r="G15" t="s">
         <v>210</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
         <v>211</v>
       </c>
-      <c r="D15" t="s">
+      <c r="I15" t="s">
         <v>212</v>
       </c>
-      <c r="E15" t="s">
+      <c r="J15" t="s">
         <v>213</v>
       </c>
-      <c r="F15" t="s">
+      <c r="K15" t="s">
         <v>214</v>
       </c>
-      <c r="G15" t="s">
+      <c r="L15" t="s">
         <v>215</v>
       </c>
-      <c r="H15" t="s">
+      <c r="M15" t="s">
         <v>216</v>
-      </c>
-      <c r="I15" t="s">
-        <v>217</v>
-      </c>
-      <c r="J15" t="s">
-        <v>218</v>
-      </c>
-      <c r="K15" t="s">
-        <v>219</v>
-      </c>
-      <c r="L15" t="s">
-        <v>220</v>
-      </c>
-      <c r="M15" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:174">
       <c r="A16" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:29">
@@ -3746,13 +3731,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="29.4" thickBot="1">
@@ -3760,88 +3745,88 @@
         <v>31</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="J22" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="K22" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="L22" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="H22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="O22" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q22" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="R22" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="S22" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="T22" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="U22" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="O22" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q22" s="9" t="s">
+      <c r="V22" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="R22" s="9" t="s">
+      <c r="W22" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="S22" s="9" t="s">
+      <c r="X22" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="T22" s="9" t="s">
+      <c r="Y22" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="U22" s="9" t="s">
+      <c r="Z22" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="V22" s="9" t="s">
+      <c r="AA22" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="W22" s="9" t="s">
+      <c r="AB22" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="X22" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="Y22" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="Z22" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="AA22" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="AB22" s="9" t="s">
-        <v>257</v>
-      </c>
       <c r="AC22" s="9" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="15" thickBot="1">
@@ -3849,70 +3834,70 @@
         <v>32</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="J23" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="K23" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="L23" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="M23" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="N23" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="O23" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="P23" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="L23" s="9" t="s">
+      <c r="Q23" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="R23" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="S23" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="O23" s="9" t="s">
+      <c r="T23" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="U23" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="Q23" s="9" t="s">
+      <c r="V23" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="R23" s="9" t="s">
+      <c r="W23" s="9" t="s">
         <v>274</v>
-      </c>
-      <c r="S23" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="T23" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="U23" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="V23" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="W23" s="9" t="s">
-        <v>279</v>
       </c>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
@@ -3925,88 +3910,88 @@
         <v>33</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="K24" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="L24" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="M24" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="N24" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="O24" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="Q24" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="M24" s="9" t="s">
+      <c r="R24" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="S24" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="O24" s="9" t="s">
+      <c r="T24" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="U24" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="Q24" s="9" t="s">
+      <c r="V24" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="R24" s="9" t="s">
+      <c r="W24" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="S24" s="9" t="s">
+      <c r="X24" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="T24" s="9" t="s">
+      <c r="Y24" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="U24" s="9" t="s">
+      <c r="Z24" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="V24" s="9" t="s">
+      <c r="AA24" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="W24" s="9" t="s">
+      <c r="AB24" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="X24" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y24" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="Z24" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="AA24" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AB24" s="9" t="s">
-        <v>306</v>
-      </c>
       <c r="AC24" s="24" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -4014,19 +3999,19 @@
         <v>68</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26" spans="1:29">
@@ -4034,174 +4019,174 @@
         <v>82</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="I26" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="J26" t="s">
         <v>486</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="K26" t="s">
         <v>488</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J26" t="s">
-        <v>491</v>
-      </c>
-      <c r="K26" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="H27" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="I27" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="J27" t="s">
         <v>486</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G27" s="10" t="s">
+      <c r="K27" t="s">
         <v>488</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J27" t="s">
-        <v>491</v>
-      </c>
-      <c r="K27" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="I28" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="J28" t="s">
         <v>486</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G28" s="10" t="s">
+      <c r="K28" t="s">
         <v>488</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J28" t="s">
-        <v>491</v>
-      </c>
-      <c r="K28" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B29" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="H29" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="J29" t="s">
         <v>486</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G29" s="10" t="s">
+      <c r="K29" t="s">
         <v>488</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J29" t="s">
-        <v>491</v>
-      </c>
-      <c r="K29" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="I30" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="J30" t="s">
         <v>486</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G30" s="10" t="s">
+      <c r="K30" t="s">
         <v>488</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J30" t="s">
-        <v>491</v>
-      </c>
-      <c r="K30" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -4209,34 +4194,34 @@
         <v>59</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="H31" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="I31" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="J31" t="s">
         <v>486</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G31" s="10" t="s">
+      <c r="K31" t="s">
         <v>488</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J31" t="s">
-        <v>491</v>
-      </c>
-      <c r="K31" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -4244,34 +4229,34 @@
         <v>47</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="I32" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="J32" t="s">
         <v>486</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G32" s="10" t="s">
+      <c r="K32" t="s">
         <v>488</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J32" t="s">
-        <v>491</v>
-      </c>
-      <c r="K32" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -4279,93 +4264,93 @@
         <v>6</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="H33" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="I33" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="J33" t="s">
         <v>486</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="G33" s="10" t="s">
+      <c r="K33" t="s">
         <v>488</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J33" t="s">
-        <v>491</v>
-      </c>
-      <c r="K33" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="6" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="26" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -4391,19 +4376,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4411,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -4420,7 +4405,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4428,7 +4413,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4437,7 +4422,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4445,7 +4430,7 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4454,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4462,7 +4447,7 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -4471,7 +4456,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4479,7 +4464,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -4488,7 +4473,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4496,7 +4481,7 @@
         <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -4505,7 +4490,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4513,7 +4498,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -4522,7 +4507,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4530,7 +4515,7 @@
         <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -4539,7 +4524,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4568,13 +4553,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4601,7 +4586,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.6">
       <c r="A4" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B4">
         <v>1980</v>
@@ -4623,7 +4608,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="11" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B6">
         <v>1980</v>
@@ -4670,7 +4655,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>1980</v>
@@ -4703,7 +4688,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.6">
       <c r="A13" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -4725,7 +4710,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4769,7 +4754,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4802,7 +4787,7 @@
     </row>
     <row r="22" spans="1:3" ht="16.2" thickBot="1">
       <c r="A22" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4824,7 +4809,7 @@
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="13" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4868,7 +4853,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4890,8 +4875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4901,10 +4886,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4912,7 +4897,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4920,23 +4905,23 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4944,7 +4929,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4952,7 +4937,7 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4960,7 +4945,7 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4968,7 +4953,7 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4976,7 +4961,7 @@
         <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4984,7 +4969,7 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4992,7 +4977,7 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5000,7 +4985,7 @@
         <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5008,7 +4993,7 @@
         <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5016,7 +5001,7 @@
         <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1">
@@ -5024,47 +5009,47 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>456</v>
       </c>
       <c r="B17" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="1" t="s">
-        <v>96</v>
+        <v>457</v>
       </c>
       <c r="B18" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5072,39 +5057,39 @@
         <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>455</v>
       </c>
       <c r="B23" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>440</v>
       </c>
       <c r="B24" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>444</v>
       </c>
       <c r="B25" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B26" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add frigo plaque vs boite
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19694278-D536-426B-A134-2DFAAB6FB1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEFAD3D-F0CC-43E3-989B-CA4F6C644A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="513">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -1355,9 +1355,6 @@
     <t>Haplotype</t>
   </si>
   <si>
-    <t>Used_for_librairie_ref</t>
-  </si>
-  <si>
     <t>Modifications_sequencages</t>
   </si>
   <si>
@@ -1391,15 +1388,6 @@
     <t>Volume_preleve_envoi</t>
   </si>
   <si>
-    <t>Etage_congelateur_extrait</t>
-  </si>
-  <si>
-    <t>Numero_congelateur_extrait</t>
-  </si>
-  <si>
-    <t>Rack_congelateur_extrait</t>
-  </si>
-  <si>
     <t>PON_sexage</t>
   </si>
   <si>
@@ -1521,6 +1509,75 @@
   </si>
   <si>
     <t>A_Atikesse</t>
+  </si>
+  <si>
+    <t>G_Bardaxoglou_G_Cortial</t>
+  </si>
+  <si>
+    <t>Numero_congelateur_extrait_boite</t>
+  </si>
+  <si>
+    <t>Etage_congelateur_extrait_boite</t>
+  </si>
+  <si>
+    <t>Rack_congelateur_extrait_boite</t>
+  </si>
+  <si>
+    <t>Numero_congelateur_extrait_plaque</t>
+  </si>
+  <si>
+    <t>Etage_congelateur_extrait_plaque</t>
+  </si>
+  <si>
+    <t>Rack_congelateur_extrait_plaque</t>
+  </si>
+  <si>
+    <t>Col_33</t>
+  </si>
+  <si>
+    <t>Col_34</t>
+  </si>
+  <si>
+    <t>Col_35</t>
+  </si>
+  <si>
+    <t>Col_36</t>
+  </si>
+  <si>
+    <t>Col_37</t>
+  </si>
+  <si>
+    <t>Col_38</t>
+  </si>
+  <si>
+    <t>Col_39</t>
+  </si>
+  <si>
+    <t>Col_40</t>
+  </si>
+  <si>
+    <t>Col_41</t>
+  </si>
+  <si>
+    <t>Col_42</t>
+  </si>
+  <si>
+    <t>Col_43</t>
+  </si>
+  <si>
+    <t>Col_44</t>
+  </si>
+  <si>
+    <t>Col_45</t>
+  </si>
+  <si>
+    <t>Col_46</t>
+  </si>
+  <si>
+    <t>Col_47</t>
+  </si>
+  <si>
+    <t>Col_48</t>
   </si>
 </sst>
 </file>
@@ -2076,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AX9"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2117,7 +2174,7 @@
     <col min="31" max="16384" width="11.5546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:50">
       <c r="A1" s="14" t="s">
         <v>117</v>
       </c>
@@ -2217,8 +2274,57 @@
       <c r="AG1" s="15" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:33">
+      <c r="AH1" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="AI1" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="AK1" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="AL1" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="AO1" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="AP1" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="AQ1" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="AR1" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="AS1" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="AT1" s="15" t="s">
+        <v>509</v>
+      </c>
+      <c r="AU1" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="AV1" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="AW1" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="AX1" s="15"/>
+    </row>
+    <row r="2" spans="1:50">
       <c r="A2" s="17" t="s">
         <v>405</v>
       </c>
@@ -2313,7 +2419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:50">
       <c r="A3" s="17" t="s">
         <v>406</v>
       </c>
@@ -2396,7 +2502,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:50">
       <c r="A4" s="17" t="s">
         <v>407</v>
       </c>
@@ -2461,7 +2567,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15" thickBot="1">
+    <row r="5" spans="1:50" ht="15" thickBot="1">
       <c r="A5" s="17" t="s">
         <v>408</v>
       </c>
@@ -2529,7 +2635,7 @@
         <v>87</v>
       </c>
       <c r="W5" s="16" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="X5" s="16" t="s">
         <v>88</v>
@@ -2538,28 +2644,37 @@
         <v>89</v>
       </c>
       <c r="Z5" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="AA5" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="AB5" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AC5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AA5" s="16" t="s">
+      <c r="AD5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="AB5" s="16" t="s">
-        <v>451</v>
-      </c>
-      <c r="AC5" s="16" t="s">
-        <v>450</v>
-      </c>
-      <c r="AD5" s="16" t="s">
-        <v>452</v>
-      </c>
       <c r="AE5" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="AF5" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="AG5" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="AH5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AF5" s="16" t="s">
+      <c r="AI5" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:50" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="17" t="s">
         <v>147</v>
       </c>
@@ -2570,16 +2685,16 @@
         <v>72</v>
       </c>
       <c r="D6" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>448</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>449</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>94</v>
@@ -2615,7 +2730,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="15" thickBot="1">
+    <row r="7" spans="1:50" ht="15" thickBot="1">
       <c r="A7" s="17" t="s">
         <v>27</v>
       </c>
@@ -2632,7 +2747,7 @@
         <v>104</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>105</v>
@@ -2653,7 +2768,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="15" thickBot="1">
+    <row r="8" spans="1:50" ht="15" thickBot="1">
       <c r="A8" s="17" t="s">
         <v>428</v>
       </c>
@@ -2673,7 +2788,7 @@
         <v>430</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>433</v>
@@ -2712,39 +2827,36 @@
         <v>116</v>
       </c>
       <c r="T8" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="U8" s="16" t="s">
         <v>438</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>441</v>
       </c>
       <c r="V8" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="W8" s="16" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" s="22" customFormat="1" ht="15" thickBot="1">
+    </row>
+    <row r="9" spans="1:50" s="22" customFormat="1" ht="15" thickBot="1">
       <c r="A9" s="17" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>455</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>456</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>457</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>459</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>460</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>461</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>462</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -2758,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
   <dimension ref="A1:FR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
@@ -2777,7 +2889,7 @@
     <col min="11" max="11" width="9.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" customWidth="1"/>
     <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -3349,13 +3461,13 @@
         <v>427</v>
       </c>
       <c r="U7" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8" spans="1:174">
@@ -3377,7 +3489,7 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C9" t="s">
         <v>213</v>
@@ -3441,13 +3553,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F11" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="G11" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:174">
@@ -3578,18 +3690,18 @@
         <v>104</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C15" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:174">
       <c r="A16" s="6" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:29">
@@ -4007,7 +4119,7 @@
         <v>293</v>
       </c>
       <c r="AC23" s="24" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -4015,19 +4127,19 @@
         <v>68</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>469</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="28.8">
@@ -4035,40 +4147,43 @@
         <v>82</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="H25" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="I25" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H25" s="10" t="s">
+      <c r="J25" t="s">
+        <v>473</v>
+      </c>
+      <c r="K25" t="s">
         <v>475</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J25" t="s">
-        <v>477</v>
-      </c>
-      <c r="K25" t="s">
-        <v>479</v>
-      </c>
       <c r="L25" s="10" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>493</v>
+        <v>489</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="26" spans="1:29">
@@ -4076,34 +4191,34 @@
         <v>94</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C26" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="I26" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H26" s="10" t="s">
+      <c r="J26" t="s">
+        <v>473</v>
+      </c>
+      <c r="K26" t="s">
         <v>475</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J26" t="s">
-        <v>477</v>
-      </c>
-      <c r="K26" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -4111,34 +4226,34 @@
         <v>98</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="H27" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="I27" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H27" s="10" t="s">
+      <c r="J27" t="s">
+        <v>473</v>
+      </c>
+      <c r="K27" t="s">
         <v>475</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J27" t="s">
-        <v>477</v>
-      </c>
-      <c r="K27" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -4146,34 +4261,34 @@
         <v>108</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="I28" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H28" s="10" t="s">
+      <c r="J28" t="s">
+        <v>473</v>
+      </c>
+      <c r="K28" t="s">
         <v>475</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J28" t="s">
-        <v>477</v>
-      </c>
-      <c r="K28" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -4181,34 +4296,34 @@
         <v>429</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C29" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="H29" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H29" s="10" t="s">
+      <c r="J29" t="s">
+        <v>473</v>
+      </c>
+      <c r="K29" t="s">
         <v>475</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J29" t="s">
-        <v>477</v>
-      </c>
-      <c r="K29" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -4216,34 +4331,34 @@
         <v>59</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C30" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="I30" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H30" s="10" t="s">
+      <c r="J30" t="s">
+        <v>473</v>
+      </c>
+      <c r="K30" t="s">
         <v>475</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J30" t="s">
-        <v>477</v>
-      </c>
-      <c r="K30" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -4251,34 +4366,34 @@
         <v>47</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C31" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="H31" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="I31" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H31" s="10" t="s">
+      <c r="J31" t="s">
+        <v>473</v>
+      </c>
+      <c r="K31" t="s">
         <v>475</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J31" t="s">
-        <v>477</v>
-      </c>
-      <c r="K31" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -4286,34 +4401,34 @@
         <v>6</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C32" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="I32" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H32" s="10" t="s">
+      <c r="J32" t="s">
+        <v>473</v>
+      </c>
+      <c r="K32" t="s">
         <v>475</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="J32" t="s">
-        <v>477</v>
-      </c>
-      <c r="K32" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4324,13 +4439,13 @@
         <v>28</v>
       </c>
       <c r="C33" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>443</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4338,10 +4453,10 @@
         <v>151</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4349,30 +4464,30 @@
         <v>99</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>461</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>464</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -5028,7 +5143,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B16" t="s">
         <v>393</v>
@@ -5044,7 +5159,7 @@
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B18" t="s">
         <v>393</v>
@@ -5052,7 +5167,7 @@
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B19" t="s">
         <v>393</v>
@@ -5092,7 +5207,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B24" t="s">
         <v>394</v>
@@ -5116,7 +5231,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B27" t="s">
         <v>393</v>

</xml_diff>

<commit_message>
Add pre-format congelateur extrait
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEFAD3D-F0CC-43E3-989B-CA4F6C644A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549BEED2-8A7F-447E-BE6B-B4A72FBB454E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="515">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -1578,13 +1578,19 @@
   </si>
   <si>
     <t>Col_48</t>
+  </si>
+  <si>
+    <t>Numero_congelateur_extraits_boite</t>
+  </si>
+  <si>
+    <t>Numero_congelateur_extraits_plaque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1633,6 +1639,13 @@
       <sz val="9"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1693,7 +1706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1760,6 +1773,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2135,7 +2149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+    <sheetView topLeftCell="AH1" workbookViewId="0">
       <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
@@ -2868,15 +2882,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
-  <dimension ref="A1:FR36"/>
+  <dimension ref="A1:FR38"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -3804,7 +3818,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15" thickBot="1">
+    <row r="19" spans="1:29">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -3854,341 +3868,377 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15" thickBot="1">
-      <c r="A20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" ht="16.8" customHeight="1" thickBot="1">
-      <c r="A21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="R21" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="S21" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="T21" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="U21" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="V21" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="W21" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="X21" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="Y21" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z21" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="AA21" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="AB21" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="AC21" s="9" t="s">
-        <v>244</v>
+    <row r="20" spans="1:29">
+      <c r="A20" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>11</v>
+      </c>
+      <c r="M20">
+        <v>12</v>
+      </c>
+      <c r="N20">
+        <v>13</v>
+      </c>
+      <c r="O20">
+        <v>14</v>
+      </c>
+      <c r="P20">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="15" thickBot="1">
+      <c r="A21" s="28" t="s">
+        <v>514</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>9</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>11</v>
+      </c>
+      <c r="M21">
+        <v>12</v>
+      </c>
+      <c r="N21">
+        <v>13</v>
+      </c>
+      <c r="O21">
+        <v>14</v>
+      </c>
+      <c r="P21">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="15" thickBot="1">
       <c r="A22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="16.8" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="X23" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y23" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z23" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB23" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="15" thickBot="1">
+      <c r="A24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K24" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="L24" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="M24" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="N24" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="O24" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="P22" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="Q22" s="9" t="s">
+      <c r="Q24" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="R22" s="9" t="s">
+      <c r="R24" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="S22" s="9" t="s">
+      <c r="S24" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="T22" s="9" t="s">
+      <c r="T24" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="U22" s="9" t="s">
+      <c r="U24" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="V22" s="9" t="s">
+      <c r="V24" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="W22" s="9" t="s">
+      <c r="W24" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-    </row>
-    <row r="23" spans="1:29" ht="15" thickBot="1">
-      <c r="A23" s="6" t="s">
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+    </row>
+    <row r="25" spans="1:29" ht="15" thickBot="1">
+      <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I25" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J25" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="L23" s="9" t="s">
+      <c r="L25" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="M25" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="N25" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="O23" s="9" t="s">
+      <c r="O25" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P25" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="Q23" s="9" t="s">
+      <c r="Q25" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="R23" s="9" t="s">
+      <c r="R25" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="S23" s="9" t="s">
+      <c r="S25" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="T23" s="9" t="s">
+      <c r="T25" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="U23" s="9" t="s">
+      <c r="U25" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="V23" s="9" t="s">
+      <c r="V25" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="W23" s="9" t="s">
+      <c r="W25" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="X23" s="9" t="s">
+      <c r="X25" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="Y23" s="9" t="s">
+      <c r="Y25" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="Z23" s="9" t="s">
+      <c r="Z25" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="AA23" s="9" t="s">
+      <c r="AA25" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="AB23" s="9" t="s">
+      <c r="AB25" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="AC23" s="24" t="s">
+      <c r="AC25" s="24" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29">
-      <c r="A24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" ht="28.8">
-      <c r="A25" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J25" t="s">
-        <v>473</v>
-      </c>
-      <c r="K25" t="s">
-        <v>475</v>
-      </c>
-      <c r="L25" s="10" t="s">
-        <v>487</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="N25" s="10" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="6" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>465</v>
@@ -4203,27 +4253,12 @@
         <v>468</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J26" t="s">
-        <v>473</v>
-      </c>
-      <c r="K26" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="28.8">
       <c r="A27" s="6" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>465</v>
@@ -4255,10 +4290,19 @@
       <c r="K27" t="s">
         <v>475</v>
       </c>
+      <c r="L27" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="6" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>465</v>
@@ -4293,7 +4337,7 @@
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="6" t="s">
-        <v>429</v>
+        <v>98</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>465</v>
@@ -4328,7 +4372,7 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="6" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>465</v>
@@ -4363,7 +4407,7 @@
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="6" t="s">
-        <v>47</v>
+        <v>429</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>465</v>
@@ -4398,7 +4442,7 @@
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="6" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>465</v>
@@ -4431,62 +4475,132 @@
         <v>475</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:11">
       <c r="A33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="J33" t="s">
+        <v>473</v>
+      </c>
+      <c r="K33" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="J34" t="s">
+        <v>473</v>
+      </c>
+      <c r="K34" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C35" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="6" t="s">
+    <row r="36" spans="1:11">
+      <c r="A36" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="6" t="s">
+    <row r="37" spans="1:11">
+      <c r="A37" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="26" t="s">
+    <row r="38" spans="1:11">
+      <c r="A38" s="26" t="s">
         <v>457</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>461</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improvement project + minor changes
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549BEED2-8A7F-447E-BE6B-B4A72FBB454E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E55228-E9D9-4180-B273-6EA50B521F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="35085" yWindow="1680" windowWidth="17280" windowHeight="12810" activeTab="2" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="522">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -716,9 +716,6 @@
     <t>CREVETTE_NORDIQUE</t>
   </si>
   <si>
-    <t>MACTRE</t>
-  </si>
-  <si>
     <t>MAQUEREAU</t>
   </si>
   <si>
@@ -1584,6 +1581,30 @@
   </si>
   <si>
     <t>Numero_congelateur_extraits_plaque</t>
+  </si>
+  <si>
+    <t>MACTRE_DE_STIMPSON</t>
+  </si>
+  <si>
+    <t>MACTRE_D_AMERIQUE</t>
+  </si>
+  <si>
+    <t>PLIE_GRISE</t>
+  </si>
+  <si>
+    <t>Glyptocephalus</t>
+  </si>
+  <si>
+    <t>cynoglossus</t>
+  </si>
+  <si>
+    <t>Frais</t>
+  </si>
+  <si>
+    <t>Gum</t>
+  </si>
+  <si>
+    <t>M_Chevrinais</t>
   </si>
 </sst>
 </file>
@@ -2101,42 +2122,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B2" t="s">
         <v>384</v>
-      </c>
-      <c r="B2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" t="s">
         <v>386</v>
-      </c>
-      <c r="B3" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B4" t="s">
         <v>388</v>
-      </c>
-      <c r="B4" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5" t="s">
         <v>390</v>
-      </c>
-      <c r="B5" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -2289,58 +2310,58 @@
         <v>150</v>
       </c>
       <c r="AH1" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>497</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>498</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="15" t="s">
         <v>499</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AL1" s="15" t="s">
         <v>500</v>
       </c>
-      <c r="AL1" s="15" t="s">
+      <c r="AM1" s="15" t="s">
         <v>501</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AN1" s="15" t="s">
         <v>502</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AO1" s="15" t="s">
         <v>503</v>
       </c>
-      <c r="AO1" s="15" t="s">
+      <c r="AP1" s="15" t="s">
         <v>504</v>
       </c>
-      <c r="AP1" s="15" t="s">
+      <c r="AQ1" s="15" t="s">
         <v>505</v>
       </c>
-      <c r="AQ1" s="15" t="s">
+      <c r="AR1" s="15" t="s">
         <v>506</v>
       </c>
-      <c r="AR1" s="15" t="s">
+      <c r="AS1" s="15" t="s">
         <v>507</v>
       </c>
-      <c r="AS1" s="15" t="s">
+      <c r="AT1" s="15" t="s">
         <v>508</v>
       </c>
-      <c r="AT1" s="15" t="s">
+      <c r="AU1" s="15" t="s">
         <v>509</v>
       </c>
-      <c r="AU1" s="15" t="s">
+      <c r="AV1" s="15" t="s">
         <v>510</v>
       </c>
-      <c r="AV1" s="15" t="s">
+      <c r="AW1" s="15" t="s">
         <v>511</v>
-      </c>
-      <c r="AW1" s="15" t="s">
-        <v>512</v>
       </c>
       <c r="AX1" s="15"/>
     </row>
     <row r="2" spans="1:50">
       <c r="A2" s="17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>0</v>
@@ -2403,10 +2424,10 @@
         <v>18</v>
       </c>
       <c r="V2" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="W2" s="16" t="s">
         <v>395</v>
-      </c>
-      <c r="W2" s="16" t="s">
-        <v>396</v>
       </c>
       <c r="X2" s="16" t="s">
         <v>19</v>
@@ -2435,7 +2456,7 @@
     </row>
     <row r="3" spans="1:50">
       <c r="A3" s="17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>0</v>
@@ -2518,7 +2539,7 @@
     </row>
     <row r="4" spans="1:50">
       <c r="A4" s="17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>29</v>
@@ -2583,7 +2604,7 @@
     </row>
     <row r="5" spans="1:50" ht="15" thickBot="1">
       <c r="A5" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>29</v>
@@ -2601,16 +2622,16 @@
         <v>74</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>76</v>
@@ -2649,7 +2670,7 @@
         <v>87</v>
       </c>
       <c r="W5" s="16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="X5" s="16" t="s">
         <v>88</v>
@@ -2658,13 +2679,13 @@
         <v>89</v>
       </c>
       <c r="Z5" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="AA5" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="AA5" s="16" t="s">
+      <c r="AB5" s="16" t="s">
         <v>492</v>
-      </c>
-      <c r="AB5" s="16" t="s">
-        <v>493</v>
       </c>
       <c r="AC5" s="16" t="s">
         <v>90</v>
@@ -2673,13 +2694,13 @@
         <v>91</v>
       </c>
       <c r="AE5" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AF5" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="AF5" s="16" t="s">
+      <c r="AG5" s="16" t="s">
         <v>495</v>
-      </c>
-      <c r="AG5" s="16" t="s">
-        <v>496</v>
       </c>
       <c r="AH5" s="16" t="s">
         <v>92</v>
@@ -2699,16 +2720,16 @@
         <v>72</v>
       </c>
       <c r="D6" s="18" t="s">
+        <v>444</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>445</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>447</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>448</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>94</v>
@@ -2761,7 +2782,7 @@
         <v>104</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>105</v>
@@ -2784,7 +2805,7 @@
     </row>
     <row r="8" spans="1:50" ht="15" thickBot="1">
       <c r="A8" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>72</v>
@@ -2796,31 +2817,31 @@
         <v>111</v>
       </c>
       <c r="E8" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>429</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G8" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="J8" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>433</v>
-      </c>
-      <c r="I8" s="18" t="s">
+      <c r="K8" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>431</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>432</v>
-      </c>
-      <c r="L8" s="16" t="s">
+      <c r="M8" s="16" t="s">
         <v>435</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>436</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>112</v>
@@ -2835,42 +2856,42 @@
         <v>115</v>
       </c>
       <c r="R8" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="S8" s="16" t="s">
         <v>116</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="U8" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="V8" s="16" t="s">
         <v>438</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:50" s="22" customFormat="1" ht="15" thickBot="1">
       <c r="A9" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>456</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="F9" s="25" t="s">
         <v>457</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="G9" s="25" t="s">
         <v>458</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -2884,8 +2905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
   <dimension ref="A1:FR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
@@ -2916,7 +2937,8 @@
     <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="100" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="100" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:174">
@@ -2981,244 +3003,244 @@
         <v>200</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="CL1" s="3" t="s">
+      <c r="CM1" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="CU1" s="3" t="s">
+      <c r="CV1" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="CV1" s="3" t="s">
-        <v>373</v>
       </c>
       <c r="CW1" s="3"/>
       <c r="CX1" s="3"/>
@@ -3337,7 +3359,7 @@
         <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>217</v>
@@ -3349,7 +3371,7 @@
         <v>194</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>195</v>
@@ -3366,7 +3388,7 @@
         <v>216</v>
       </c>
       <c r="D5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>217</v>
@@ -3378,10 +3400,13 @@
         <v>194</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>195</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="6" spans="1:174">
@@ -3395,7 +3420,7 @@
         <v>216</v>
       </c>
       <c r="D6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>217</v>
@@ -3407,10 +3432,13 @@
         <v>194</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>195</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="7" spans="1:174">
@@ -3418,70 +3446,73 @@
         <v>64</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" t="s">
         <v>409</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="S7" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="T7" s="7" t="s">
-        <v>427</v>
-      </c>
       <c r="U7" t="s">
+        <v>475</v>
+      </c>
+      <c r="V7" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="V7" s="7" t="s">
-        <v>477</v>
-      </c>
       <c r="W7" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:174">
@@ -3495,7 +3526,7 @@
         <v>164</v>
       </c>
       <c r="D8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:174">
@@ -3503,7 +3534,7 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C9" t="s">
         <v>213</v>
@@ -3532,25 +3563,25 @@
         <v>81</v>
       </c>
       <c r="B10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C10" t="s">
         <v>398</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>399</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" t="s">
         <v>401</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>402</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>403</v>
-      </c>
-      <c r="H10" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:174">
@@ -3567,13 +3598,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="27" t="s">
+        <v>479</v>
+      </c>
+      <c r="F11" t="s">
         <v>480</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>481</v>
-      </c>
-      <c r="G11" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:174">
@@ -3704,21 +3735,21 @@
         <v>104</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="C15" t="s">
         <v>478</v>
-      </c>
-      <c r="C15" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:174">
       <c r="A16" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" s="6" t="s">
         <v>62</v>
       </c>
@@ -3768,7 +3799,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:30">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
@@ -3818,7 +3849,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:30">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -3868,9 +3899,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:30">
       <c r="A20" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3918,9 +3949,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15" thickBot="1">
+    <row r="21" spans="1:30" ht="15" thickBot="1">
       <c r="A21" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3968,7 +3999,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="15" thickBot="1">
+    <row r="22" spans="1:30" ht="15" thickBot="1">
       <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
@@ -3982,7 +4013,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="16.8" customHeight="1" thickBot="1">
+    <row r="23" spans="1:30" ht="16.8" customHeight="1" thickBot="1">
       <c r="A23" s="6" t="s">
         <v>31</v>
       </c>
@@ -3999,609 +4030,626 @@
         <v>224</v>
       </c>
       <c r="F23" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="H23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="J23" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="K23" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="L23" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="L23" s="9" t="s">
+      <c r="M23" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="N23" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="O23" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q23" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="O23" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q23" s="9" t="s">
+      <c r="R23" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="R23" s="9" t="s">
+      <c r="S23" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="S23" s="9" t="s">
+      <c r="T23" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="T23" s="9" t="s">
+      <c r="U23" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="U23" s="9" t="s">
+      <c r="V23" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="V23" s="9" t="s">
+      <c r="W23" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="W23" s="9" t="s">
+      <c r="X23" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="X23" s="9" t="s">
+      <c r="Y23" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="Y23" s="9" t="s">
+      <c r="Z23" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z23" s="9" t="s">
+      <c r="AA23" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="AA23" s="9" t="s">
+      <c r="AB23" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="AB23" s="9" t="s">
-        <v>244</v>
-      </c>
       <c r="AC23" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" ht="15" thickBot="1">
+        <v>243</v>
+      </c>
+      <c r="AD23" s="24" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="29.4" thickBot="1">
       <c r="A24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="K24" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="L24" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="M24" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="M24" s="9" t="s">
+      <c r="N24" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="O24" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="O24" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="Q24" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="Q24" s="9" t="s">
+      <c r="R24" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="R24" s="9" t="s">
+      <c r="S24" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="S24" s="9" t="s">
+      <c r="T24" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="T24" s="9" t="s">
+      <c r="U24" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="U24" s="9" t="s">
+      <c r="V24" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="V24" s="9" t="s">
+      <c r="W24" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="W24" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="X24" s="4"/>
+      <c r="X24" s="24" t="s">
+        <v>517</v>
+      </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
     </row>
-    <row r="25" spans="1:29" ht="15" thickBot="1">
+    <row r="25" spans="1:30" ht="43.8" thickBot="1">
       <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="I25" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="J25" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="L25" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="L25" s="9" t="s">
+      <c r="M25" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="M25" s="9" t="s">
+      <c r="N25" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="N25" s="9" t="s">
+      <c r="O25" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="O25" s="9" t="s">
+      <c r="P25" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="Q25" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="R25" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="R25" s="9" t="s">
+      <c r="S25" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="S25" s="9" t="s">
+      <c r="T25" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="T25" s="9" t="s">
+      <c r="U25" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="U25" s="9" t="s">
+      <c r="V25" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="V25" s="9" t="s">
+      <c r="W25" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="W25" s="9" t="s">
+      <c r="X25" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="X25" s="9" t="s">
+      <c r="Y25" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="Y25" s="9" t="s">
+      <c r="Z25" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="Z25" s="9" t="s">
+      <c r="AA25" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="AA25" s="9" t="s">
+      <c r="AB25" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="AB25" s="9" t="s">
-        <v>293</v>
-      </c>
       <c r="AC25" s="24" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29">
+        <v>450</v>
+      </c>
+      <c r="AD25" s="24" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30">
       <c r="A26" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" ht="28.8">
+    </row>
+    <row r="27" spans="1:30" ht="28.8">
       <c r="A27" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F27" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J27" t="s">
+        <v>472</v>
+      </c>
+      <c r="K27" t="s">
         <v>474</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J27" t="s">
-        <v>473</v>
-      </c>
-      <c r="K27" t="s">
-        <v>475</v>
-      </c>
       <c r="L27" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="M27" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="N27" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="N27" s="10" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29">
+    </row>
+    <row r="28" spans="1:30">
       <c r="A28" s="6" t="s">
         <v>94</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F28" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J28" t="s">
+        <v>472</v>
+      </c>
+      <c r="K28" t="s">
         <v>474</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J28" t="s">
-        <v>473</v>
-      </c>
-      <c r="K28" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29">
+    </row>
+    <row r="29" spans="1:30">
       <c r="A29" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B29" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F29" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J29" t="s">
+        <v>472</v>
+      </c>
+      <c r="K29" t="s">
         <v>474</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J29" t="s">
-        <v>473</v>
-      </c>
-      <c r="K29" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29">
+    </row>
+    <row r="30" spans="1:30">
       <c r="A30" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F30" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J30" t="s">
+        <v>472</v>
+      </c>
+      <c r="K30" t="s">
         <v>474</v>
       </c>
-      <c r="G30" s="10" t="s">
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H31" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="I31" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="J31" t="s">
         <v>472</v>
       </c>
-      <c r="J30" t="s">
-        <v>473</v>
-      </c>
-      <c r="K30" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29">
-      <c r="A31" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="F31" s="10" t="s">
+      <c r="K31" t="s">
         <v>474</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J31" t="s">
-        <v>473</v>
-      </c>
-      <c r="K31" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29">
+    </row>
+    <row r="32" spans="1:30">
       <c r="A32" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F32" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J32" t="s">
+        <v>472</v>
+      </c>
+      <c r="K32" t="s">
         <v>474</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J32" t="s">
-        <v>473</v>
-      </c>
-      <c r="K32" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F33" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J33" t="s">
+        <v>472</v>
+      </c>
+      <c r="K33" t="s">
         <v>474</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J33" t="s">
-        <v>473</v>
-      </c>
-      <c r="K33" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" s="10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>468</v>
-      </c>
       <c r="F34" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J34" t="s">
+        <v>472</v>
+      </c>
+      <c r="K34" t="s">
         <v>474</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="J34" t="s">
-        <v>473</v>
-      </c>
-      <c r="K34" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" s="10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="6" t="s">
         <v>151</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>454</v>
-      </c>
       <c r="E37" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>460</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -4807,10 +4855,10 @@
         <v>152</v>
       </c>
       <c r="B1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" t="s">
         <v>380</v>
-      </c>
-      <c r="C1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4859,7 +4907,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B6">
         <v>1980</v>
@@ -4961,7 +5009,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5060,7 +5108,7 @@
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5140,7 +5188,7 @@
         <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5148,7 +5196,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5156,23 +5204,23 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5180,7 +5228,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5188,7 +5236,7 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5196,7 +5244,7 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5204,7 +5252,7 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5212,7 +5260,7 @@
         <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5220,7 +5268,7 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5228,7 +5276,7 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5236,7 +5284,7 @@
         <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5244,7 +5292,7 @@
         <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5252,15 +5300,15 @@
         <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1">
@@ -5268,23 +5316,23 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5292,7 +5340,7 @@
         <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5300,7 +5348,7 @@
         <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5308,7 +5356,7 @@
         <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5316,39 +5364,39 @@
         <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add automatic correction of column name for ADNe V3  to V4
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7F2EFF-9A4A-4684-9D56-D07CA5F7D81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01C6237-57AF-4288-9036-A9AA312B8B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="1080" yWindow="444" windowWidth="21600" windowHeight="11328" activeTab="6" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -4433,13 +4433,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="34" style="11" customWidth="1"/>
     <col min="2" max="2" width="31" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.109375" style="11" bestFit="1" customWidth="1"/>
@@ -22870,8 +22870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE84406-98AE-4E64-999D-911172EB9954}">
   <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Add QNC QPC automatic function #8
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01C6237-57AF-4288-9036-A9AA312B8B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1580C956-9B08-4547-86AD-60D297C4ADD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="444" windowWidth="21600" windowHeight="11328" activeTab="6" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1224">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -3709,13 +3709,16 @@
   </si>
   <si>
     <t>Type_echantillon_qPCR_inhibition</t>
+  </si>
+  <si>
+    <t>Modifications_courbes_standard_ADNe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3796,6 +3799,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3916,10 +3930,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4058,9 +4073,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E32D0B1F-6AD7-43D0-B3E0-A03D219265F1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4433,8 +4451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -6015,7 +6033,9 @@
       <c r="V18" s="23" t="s">
         <v>783</v>
       </c>
-      <c r="W18" s="22"/>
+      <c r="W18" s="23" t="s">
+        <v>1223</v>
+      </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
@@ -6065,13 +6085,12 @@
       <c r="I19" s="22" t="s">
         <v>791</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="23" t="s">
+        <v>793</v>
+      </c>
+      <c r="K19" s="22" t="s">
         <v>792</v>
       </c>
-      <c r="K19" s="23" t="s">
-        <v>793</v>
-      </c>
-      <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
@@ -22868,17 +22887,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE84406-98AE-4E64-999D-911172EB9954}">
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:L165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1">
@@ -23035,7 +23055,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29.4" thickBot="1">
+    <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>579</v>
       </c>
@@ -23049,7 +23069,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29.4" thickBot="1">
+    <row r="13" spans="1:4" ht="15" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>579</v>
       </c>
@@ -23063,7 +23083,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29.4" thickBot="1">
+    <row r="14" spans="1:4" ht="15" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>579</v>
       </c>
@@ -23077,7 +23097,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="29.4" thickBot="1">
+    <row r="15" spans="1:4" ht="15" thickBot="1">
       <c r="A15" s="1" t="s">
         <v>579</v>
       </c>
@@ -23091,7 +23111,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.4" thickBot="1">
+    <row r="16" spans="1:4" ht="15" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>579</v>
       </c>
@@ -23105,7 +23125,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29.4" thickBot="1">
+    <row r="17" spans="1:4" ht="15" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>579</v>
       </c>
@@ -23119,7 +23139,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.4" thickBot="1">
+    <row r="18" spans="1:4" ht="15" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>579</v>
       </c>
@@ -23133,7 +23153,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="29.4" thickBot="1">
+    <row r="19" spans="1:4" ht="15" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>579</v>
       </c>
@@ -23147,7 +23167,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="29.4" thickBot="1">
+    <row r="20" spans="1:4" ht="15" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>579</v>
       </c>
@@ -23161,7 +23181,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="29.4" thickBot="1">
+    <row r="21" spans="1:4" ht="15" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>579</v>
       </c>
@@ -23175,7 +23195,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="29.4" thickBot="1">
+    <row r="22" spans="1:4" ht="15" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>579</v>
       </c>
@@ -23189,7 +23209,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="29.4" thickBot="1">
+    <row r="23" spans="1:4" ht="15" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>579</v>
       </c>
@@ -23203,7 +23223,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="29.4" thickBot="1">
+    <row r="24" spans="1:4" ht="15" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>593</v>
       </c>
@@ -23217,7 +23237,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="29.4" thickBot="1">
+    <row r="25" spans="1:4" ht="15" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>593</v>
       </c>
@@ -23231,7 +23251,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="29.4" thickBot="1">
+    <row r="26" spans="1:4" ht="15" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>593</v>
       </c>
@@ -23245,7 +23265,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="29.4" thickBot="1">
+    <row r="27" spans="1:4" ht="15" thickBot="1">
       <c r="A27" s="1" t="s">
         <v>593</v>
       </c>
@@ -23259,7 +23279,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="29.4" thickBot="1">
+    <row r="28" spans="1:4" ht="15" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>593</v>
       </c>
@@ -23273,7 +23293,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="29.4" thickBot="1">
+    <row r="29" spans="1:4" ht="15" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>593</v>
       </c>
@@ -23287,7 +23307,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="29.4" thickBot="1">
+    <row r="30" spans="1:4" ht="15" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>593</v>
       </c>
@@ -23301,7 +23321,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="29.4" thickBot="1">
+    <row r="31" spans="1:4" ht="15" thickBot="1">
       <c r="A31" s="1" t="s">
         <v>593</v>
       </c>
@@ -23315,7 +23335,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="29.4" thickBot="1">
+    <row r="32" spans="1:4" ht="15" thickBot="1">
       <c r="A32" s="1" t="s">
         <v>593</v>
       </c>
@@ -23329,7 +23349,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="29.4" thickBot="1">
+    <row r="33" spans="1:4" ht="15" thickBot="1">
       <c r="A33" s="1" t="s">
         <v>593</v>
       </c>
@@ -23343,7 +23363,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.4" thickBot="1">
+    <row r="34" spans="1:4" ht="15" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>593</v>
       </c>
@@ -23357,7 +23377,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="29.4" thickBot="1">
+    <row r="35" spans="1:4" ht="15" thickBot="1">
       <c r="A35" s="1" t="s">
         <v>593</v>
       </c>
@@ -23371,7 +23391,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="29.4" thickBot="1">
+    <row r="36" spans="1:4" ht="15" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>593</v>
       </c>
@@ -23385,7 +23405,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="29.4" thickBot="1">
+    <row r="37" spans="1:4" ht="15" thickBot="1">
       <c r="A37" s="1" t="s">
         <v>593</v>
       </c>
@@ -23399,7 +23419,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="29.4" thickBot="1">
+    <row r="38" spans="1:4" ht="15" thickBot="1">
       <c r="A38" s="1" t="s">
         <v>593</v>
       </c>
@@ -23413,7 +23433,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="29.4" thickBot="1">
+    <row r="39" spans="1:4" ht="15" thickBot="1">
       <c r="A39" s="1" t="s">
         <v>593</v>
       </c>
@@ -23427,7 +23447,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="29.4" thickBot="1">
+    <row r="40" spans="1:4" ht="15" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>593</v>
       </c>
@@ -23441,7 +23461,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="29.4" thickBot="1">
+    <row r="41" spans="1:4" ht="15" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>593</v>
       </c>
@@ -23455,7 +23475,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="29.4" thickBot="1">
+    <row r="42" spans="1:4" ht="15" thickBot="1">
       <c r="A42" s="1" t="s">
         <v>593</v>
       </c>
@@ -23749,7 +23769,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="29.4" thickBot="1">
+    <row r="63" spans="1:4" ht="15" thickBot="1">
       <c r="A63" s="1" t="s">
         <v>625</v>
       </c>
@@ -23777,7 +23797,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="29.4" thickBot="1">
+    <row r="65" spans="1:4" ht="15" thickBot="1">
       <c r="A65" s="1" t="s">
         <v>665</v>
       </c>
@@ -23791,7 +23811,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="29.4" thickBot="1">
+    <row r="66" spans="1:4" ht="15" thickBot="1">
       <c r="A66" s="1" t="s">
         <v>665</v>
       </c>
@@ -23805,7 +23825,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="29.4" thickBot="1">
+    <row r="67" spans="1:4" ht="15" thickBot="1">
       <c r="A67" s="1" t="s">
         <v>665</v>
       </c>
@@ -23819,7 +23839,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="29.4" thickBot="1">
+    <row r="68" spans="1:4" ht="15" thickBot="1">
       <c r="A68" s="1" t="s">
         <v>665</v>
       </c>
@@ -23833,7 +23853,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="29.4" thickBot="1">
+    <row r="69" spans="1:4" ht="15" thickBot="1">
       <c r="A69" s="1" t="s">
         <v>665</v>
       </c>
@@ -23847,7 +23867,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="29.4" thickBot="1">
+    <row r="70" spans="1:4" ht="15" thickBot="1">
       <c r="A70" s="1" t="s">
         <v>665</v>
       </c>
@@ -23861,7 +23881,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="29.4" thickBot="1">
+    <row r="71" spans="1:4" ht="15" thickBot="1">
       <c r="A71" s="1" t="s">
         <v>665</v>
       </c>
@@ -23875,7 +23895,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="29.4" thickBot="1">
+    <row r="72" spans="1:4" ht="15" thickBot="1">
       <c r="A72" s="1" t="s">
         <v>665</v>
       </c>
@@ -23889,7 +23909,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="29.4" thickBot="1">
+    <row r="73" spans="1:4" ht="15" thickBot="1">
       <c r="A73" s="1" t="s">
         <v>665</v>
       </c>
@@ -23903,7 +23923,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="29.4" thickBot="1">
+    <row r="74" spans="1:4" ht="15" thickBot="1">
       <c r="A74" s="1" t="s">
         <v>665</v>
       </c>
@@ -23917,7 +23937,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="29.4" thickBot="1">
+    <row r="75" spans="1:4" ht="15" thickBot="1">
       <c r="A75" s="1" t="s">
         <v>665</v>
       </c>
@@ -23931,7 +23951,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="29.4" thickBot="1">
+    <row r="76" spans="1:4" ht="15" thickBot="1">
       <c r="A76" s="1" t="s">
         <v>665</v>
       </c>
@@ -23945,7 +23965,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="29.4" thickBot="1">
+    <row r="77" spans="1:4" ht="15" thickBot="1">
       <c r="A77" s="1" t="s">
         <v>665</v>
       </c>
@@ -23959,7 +23979,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="29.4" thickBot="1">
+    <row r="78" spans="1:4" ht="15" thickBot="1">
       <c r="A78" s="1" t="s">
         <v>665</v>
       </c>
@@ -23973,7 +23993,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="29.4" thickBot="1">
+    <row r="79" spans="1:4" ht="15" thickBot="1">
       <c r="A79" s="1" t="s">
         <v>665</v>
       </c>
@@ -23987,7 +24007,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="29.4" thickBot="1">
+    <row r="80" spans="1:4" ht="15" thickBot="1">
       <c r="A80" s="1" t="s">
         <v>665</v>
       </c>
@@ -24001,7 +24021,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="29.4" thickBot="1">
+    <row r="81" spans="1:4" ht="15" thickBot="1">
       <c r="A81" s="1" t="s">
         <v>665</v>
       </c>
@@ -24015,7 +24035,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="29.4" thickBot="1">
+    <row r="82" spans="1:4" ht="15" thickBot="1">
       <c r="A82" s="1" t="s">
         <v>665</v>
       </c>
@@ -24029,7 +24049,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="29.4" thickBot="1">
+    <row r="83" spans="1:4" ht="15" thickBot="1">
       <c r="A83" s="1" t="s">
         <v>665</v>
       </c>
@@ -24043,7 +24063,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="29.4" thickBot="1">
+    <row r="84" spans="1:4" ht="15" thickBot="1">
       <c r="A84" s="1" t="s">
         <v>665</v>
       </c>
@@ -24057,7 +24077,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="29.4" thickBot="1">
+    <row r="85" spans="1:4" ht="15" thickBot="1">
       <c r="A85" s="1" t="s">
         <v>665</v>
       </c>
@@ -24071,7 +24091,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="29.4" thickBot="1">
+    <row r="86" spans="1:4" ht="15" thickBot="1">
       <c r="A86" s="1" t="s">
         <v>665</v>
       </c>
@@ -24085,7 +24105,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="29.4" thickBot="1">
+    <row r="87" spans="1:4" ht="15" thickBot="1">
       <c r="A87" s="1" t="s">
         <v>665</v>
       </c>
@@ -24099,7 +24119,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="29.4" thickBot="1">
+    <row r="88" spans="1:4" ht="15" thickBot="1">
       <c r="A88" s="1" t="s">
         <v>665</v>
       </c>
@@ -24113,7 +24133,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="29.4" thickBot="1">
+    <row r="89" spans="1:4" ht="15" thickBot="1">
       <c r="A89" s="1" t="s">
         <v>665</v>
       </c>
@@ -24127,7 +24147,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="29.4" thickBot="1">
+    <row r="90" spans="1:4" ht="15" thickBot="1">
       <c r="A90" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24141,7 +24161,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="29.4" thickBot="1">
+    <row r="91" spans="1:4" ht="15" thickBot="1">
       <c r="A91" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24155,7 +24175,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="29.4" thickBot="1">
+    <row r="92" spans="1:4" ht="15" thickBot="1">
       <c r="A92" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24169,7 +24189,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="29.4" thickBot="1">
+    <row r="93" spans="1:4" ht="15" thickBot="1">
       <c r="A93" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24183,7 +24203,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="29.4" thickBot="1">
+    <row r="94" spans="1:4" ht="15" thickBot="1">
       <c r="A94" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24197,7 +24217,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="29.4" thickBot="1">
+    <row r="95" spans="1:4" ht="15" thickBot="1">
       <c r="A95" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24211,7 +24231,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="29.4" thickBot="1">
+    <row r="96" spans="1:4" ht="15" thickBot="1">
       <c r="A96" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24225,7 +24245,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="29.4" thickBot="1">
+    <row r="97" spans="1:4" ht="15" thickBot="1">
       <c r="A97" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24239,7 +24259,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="29.4" thickBot="1">
+    <row r="98" spans="1:4" ht="15" thickBot="1">
       <c r="A98" s="22" t="s">
         <v>1159</v>
       </c>
@@ -24449,7 +24469,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" thickBot="1">
+    <row r="113" spans="1:12" ht="15" thickBot="1">
       <c r="A113" s="22" t="s">
         <v>718</v>
       </c>
@@ -24463,7 +24483,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" thickBot="1">
+    <row r="114" spans="1:12" ht="15" thickBot="1">
       <c r="A114" s="22" t="s">
         <v>718</v>
       </c>
@@ -24477,7 +24497,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" thickBot="1">
+    <row r="115" spans="1:12" ht="15" thickBot="1">
       <c r="A115" s="22" t="s">
         <v>718</v>
       </c>
@@ -24491,7 +24511,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" thickBot="1">
+    <row r="116" spans="1:12" ht="15" thickBot="1">
       <c r="A116" s="22" t="s">
         <v>718</v>
       </c>
@@ -24505,7 +24525,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" thickBot="1">
+    <row r="117" spans="1:12" ht="15" thickBot="1">
       <c r="A117" s="22" t="s">
         <v>718</v>
       </c>
@@ -24519,7 +24539,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" thickBot="1">
+    <row r="118" spans="1:12" ht="15" thickBot="1">
       <c r="A118" s="22" t="s">
         <v>718</v>
       </c>
@@ -24532,36 +24552,42 @@
       <c r="D118" s="22" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="43.8" thickBot="1">
+      <c r="G118" s="57"/>
+      <c r="H118" s="57"/>
+      <c r="I118" s="56"/>
+      <c r="J118" s="56"/>
+      <c r="K118" s="56"/>
+      <c r="L118" s="56"/>
+    </row>
+    <row r="119" spans="1:12" ht="15" thickBot="1">
       <c r="A119" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B119" s="22" t="s">
-        <v>784</v>
+        <v>759</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="57" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="43.8" thickBot="1">
+    <row r="120" spans="1:12" ht="15" thickBot="1">
       <c r="A120" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>784</v>
+        <v>759</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D120" s="22" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="43.8" thickBot="1">
+        <v>1178</v>
+      </c>
+      <c r="D120" s="57" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="15" thickBot="1">
       <c r="A121" s="22" t="s">
         <v>718</v>
       </c>
@@ -24569,13 +24595,13 @@
         <v>784</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1183</v>
-      </c>
-      <c r="D121" s="22" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="43.8" thickBot="1">
+        <v>785</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="15" thickBot="1">
       <c r="A122" s="22" t="s">
         <v>718</v>
       </c>
@@ -24583,13 +24609,13 @@
         <v>784</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1184</v>
+        <v>72</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="43.8" thickBot="1">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="15" thickBot="1">
       <c r="A123" s="22" t="s">
         <v>718</v>
       </c>
@@ -24597,13 +24623,13 @@
         <v>784</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="43.8" thickBot="1">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="15" thickBot="1">
       <c r="A124" s="22" t="s">
         <v>718</v>
       </c>
@@ -24611,13 +24637,13 @@
         <v>784</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>428</v>
+        <v>1184</v>
       </c>
       <c r="D124" s="22" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="43.8" thickBot="1">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="15" thickBot="1">
       <c r="A125" s="22" t="s">
         <v>718</v>
       </c>
@@ -24625,13 +24651,13 @@
         <v>784</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D125" s="22" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="43.8" thickBot="1">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="15" thickBot="1">
       <c r="A126" s="22" t="s">
         <v>718</v>
       </c>
@@ -24639,41 +24665,41 @@
         <v>784</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D126" s="22" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="15" thickBot="1">
+      <c r="A127" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B127" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D127" s="22" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" ht="15" thickBot="1">
+      <c r="A128" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B128" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>1187</v>
       </c>
-      <c r="D126" s="22" t="s">
+      <c r="D128" s="22" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="43.8" thickBot="1">
-      <c r="A127" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B127" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>1189</v>
-      </c>
-      <c r="D127" s="22" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="43.8" thickBot="1">
-      <c r="A128" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B128" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D128" s="22" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="43.8" thickBot="1">
+    <row r="129" spans="1:4" ht="15" thickBot="1">
       <c r="A129" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24681,13 +24707,13 @@
         <v>764</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="D129" s="22" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="43.8" thickBot="1">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15" thickBot="1">
       <c r="A130" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24695,13 +24721,13 @@
         <v>764</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="43.8" thickBot="1">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15" thickBot="1">
       <c r="A131" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24709,13 +24735,13 @@
         <v>764</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="43.8" thickBot="1">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" thickBot="1">
       <c r="A132" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24723,13 +24749,13 @@
         <v>764</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="43.8" thickBot="1">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" thickBot="1">
       <c r="A133" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24737,13 +24763,13 @@
         <v>764</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="43.8" thickBot="1">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" thickBot="1">
       <c r="A134" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24751,13 +24777,13 @@
         <v>764</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>736</v>
+        <v>1194</v>
       </c>
       <c r="D134" s="22" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="43.8" thickBot="1">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" thickBot="1">
       <c r="A135" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24765,13 +24791,13 @@
         <v>764</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1178</v>
+        <v>1195</v>
       </c>
       <c r="D135" s="22" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="43.8" thickBot="1">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" thickBot="1">
       <c r="A136" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24779,13 +24805,13 @@
         <v>764</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1164</v>
+        <v>736</v>
       </c>
       <c r="D136" s="22" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="43.8" thickBot="1">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" thickBot="1">
       <c r="A137" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24793,13 +24819,13 @@
         <v>764</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1197</v>
+        <v>1178</v>
       </c>
       <c r="D137" s="22" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="43.8" thickBot="1">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15" thickBot="1">
       <c r="A138" s="22" t="s">
         <v>1188</v>
       </c>
@@ -24807,41 +24833,41 @@
         <v>764</v>
       </c>
       <c r="C138" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D138" s="22" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15" thickBot="1">
+      <c r="A139" s="22" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B139" s="22" t="s">
+        <v>764</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D139" s="22" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="15" thickBot="1">
+      <c r="A140" s="22" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B140" s="22" t="s">
+        <v>764</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>1199</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="29.4" thickBot="1">
-      <c r="A139" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="B139" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D139" s="22" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="29.4" thickBot="1">
-      <c r="A140" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="B140" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D140" s="22" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="29.4" thickBot="1">
+    <row r="141" spans="1:4" ht="15" thickBot="1">
       <c r="A141" s="22" t="s">
         <v>794</v>
       </c>
@@ -24849,13 +24875,13 @@
         <v>794</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1201</v>
+        <v>72</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="29.4" thickBot="1">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15" thickBot="1">
       <c r="A142" s="22" t="s">
         <v>794</v>
       </c>
@@ -24863,13 +24889,13 @@
         <v>794</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="29.4" thickBot="1">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15" thickBot="1">
       <c r="A143" s="22" t="s">
         <v>794</v>
       </c>
@@ -24877,13 +24903,13 @@
         <v>794</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="29.4" thickBot="1">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15" thickBot="1">
       <c r="A144" s="22" t="s">
         <v>794</v>
       </c>
@@ -24891,13 +24917,13 @@
         <v>794</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="29.4" thickBot="1">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15" thickBot="1">
       <c r="A145" s="22" t="s">
         <v>794</v>
       </c>
@@ -24905,13 +24931,13 @@
         <v>794</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>75</v>
+        <v>1203</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="29.4" thickBot="1">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15" thickBot="1">
       <c r="A146" s="22" t="s">
         <v>794</v>
       </c>
@@ -24919,41 +24945,41 @@
         <v>794</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D146" s="22" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="43.8" thickBot="1">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="15" thickBot="1">
       <c r="A147" s="22" t="s">
         <v>794</v>
       </c>
       <c r="B147" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1206</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="43.8" thickBot="1">
+        <v>75</v>
+      </c>
+      <c r="D147" s="22" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="15" thickBot="1">
       <c r="A148" s="22" t="s">
         <v>794</v>
       </c>
       <c r="B148" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1207</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="43.8" thickBot="1">
+        <v>1205</v>
+      </c>
+      <c r="D148" s="22" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="15" thickBot="1">
       <c r="A149" s="22" t="s">
         <v>794</v>
       </c>
@@ -24961,13 +24987,13 @@
         <v>809</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1208</v>
-      </c>
-      <c r="D149" s="22" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="43.8" thickBot="1">
+        <v>1206</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15" thickBot="1">
       <c r="A150" s="22" t="s">
         <v>794</v>
       </c>
@@ -24975,13 +25001,13 @@
         <v>809</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>1209</v>
-      </c>
-      <c r="D150" s="22" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="43.8" thickBot="1">
+        <v>1207</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15" thickBot="1">
       <c r="A151" s="22" t="s">
         <v>794</v>
       </c>
@@ -24989,13 +25015,13 @@
         <v>809</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="43.8" thickBot="1">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15" thickBot="1">
       <c r="A152" s="22" t="s">
         <v>794</v>
       </c>
@@ -25003,13 +25029,13 @@
         <v>809</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="43.8" thickBot="1">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15" thickBot="1">
       <c r="A153" s="22" t="s">
         <v>794</v>
       </c>
@@ -25017,13 +25043,13 @@
         <v>809</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="43.8" thickBot="1">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15" thickBot="1">
       <c r="A154" s="22" t="s">
         <v>794</v>
       </c>
@@ -25031,13 +25057,13 @@
         <v>809</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D154" s="22" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="43.8" thickBot="1">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15" thickBot="1">
       <c r="A155" s="22" t="s">
         <v>794</v>
       </c>
@@ -25045,13 +25071,13 @@
         <v>809</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>84</v>
+        <v>1212</v>
       </c>
       <c r="D155" s="22" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="43.8" thickBot="1">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15" thickBot="1">
       <c r="A156" s="22" t="s">
         <v>794</v>
       </c>
@@ -25059,13 +25085,13 @@
         <v>809</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="43.8" thickBot="1">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15" thickBot="1">
       <c r="A157" s="22" t="s">
         <v>794</v>
       </c>
@@ -25073,13 +25099,13 @@
         <v>809</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>1215</v>
+        <v>84</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="43.8" thickBot="1">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15" thickBot="1">
       <c r="A158" s="22" t="s">
         <v>794</v>
       </c>
@@ -25087,13 +25113,13 @@
         <v>809</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="43.8" thickBot="1">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="15" thickBot="1">
       <c r="A159" s="22" t="s">
         <v>794</v>
       </c>
@@ -25101,41 +25127,41 @@
         <v>809</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="D159" s="22" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="43.8" thickBot="1">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15" thickBot="1">
       <c r="A160" s="22" t="s">
         <v>794</v>
       </c>
       <c r="B160" s="22" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="D160" s="22" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="43.8" thickBot="1">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15" thickBot="1">
       <c r="A161" s="22" t="s">
         <v>794</v>
       </c>
       <c r="B161" s="22" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D161" s="23" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="43.8" thickBot="1">
+        <v>1217</v>
+      </c>
+      <c r="D161" s="22" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15" thickBot="1">
       <c r="A162" s="22" t="s">
         <v>794</v>
       </c>
@@ -25143,13 +25169,13 @@
         <v>833</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D162" s="22" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="43.8" thickBot="1">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15" thickBot="1">
       <c r="A163" s="22" t="s">
         <v>794</v>
       </c>
@@ -25157,9 +25183,37 @@
         <v>833</v>
       </c>
       <c r="C163" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D163" s="23" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="15" thickBot="1">
+      <c r="A164" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B164" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D164" s="22" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="29.4" thickBot="1">
+      <c r="A165" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B165" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>1221</v>
       </c>
-      <c r="D163" s="22" t="s">
+      <c r="D165" s="22" t="s">
         <v>837</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change v3 QNC QPC
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1580C956-9B08-4547-86AD-60D297C4ADD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D46E1-8633-4AB8-B84D-07460F4D0FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="1229">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -3690,12 +3690,6 @@
     <t>Conc. Qubit_ng/uL</t>
   </si>
   <si>
-    <t>Modifications_librairies</t>
-  </si>
-  <si>
-    <t>Notes_librairies</t>
-  </si>
-  <si>
     <t>Puits_plaque_GQ</t>
   </si>
   <si>
@@ -3712,6 +3706,27 @@
   </si>
   <si>
     <t>Modifications_courbes_standard_ADNe</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Modifications</t>
+  </si>
+  <si>
+    <t>Modification_qPCR_inhibition</t>
+  </si>
+  <si>
+    <t>Modifications_qPCR_inhibition</t>
+  </si>
+  <si>
+    <t>Modification_librairies_ADNe</t>
+  </si>
+  <si>
+    <t>Modifications_purification_librairies_ADNe</t>
+  </si>
+  <si>
+    <t>Notes_purification_librairies_ADNe</t>
   </si>
 </sst>
 </file>
@@ -4451,7 +4466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -5693,7 +5708,7 @@
         <v>666</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>697</v>
@@ -5758,7 +5773,9 @@
       <c r="X15" s="22" t="s">
         <v>717</v>
       </c>
-      <c r="Y15" s="22"/>
+      <c r="Y15" s="22" t="s">
+        <v>1224</v>
+      </c>
       <c r="Z15" s="22"/>
       <c r="AA15" s="22"/>
       <c r="AB15" s="22"/>
@@ -6034,7 +6051,7 @@
         <v>783</v>
       </c>
       <c r="W18" s="23" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
@@ -6172,8 +6189,12 @@
       <c r="P20" s="22" t="s">
         <v>808</v>
       </c>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
+      <c r="Q20" s="22" t="s">
+        <v>832</v>
+      </c>
+      <c r="R20" s="22" t="s">
+        <v>1226</v>
+      </c>
       <c r="S20" s="22"/>
       <c r="T20" s="22"/>
       <c r="U20" s="22"/>
@@ -6271,10 +6292,10 @@
         <v>830</v>
       </c>
       <c r="X21" s="22" t="s">
-        <v>831</v>
+        <v>1227</v>
       </c>
       <c r="Y21" s="22" t="s">
-        <v>832</v>
+        <v>1228</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
@@ -16392,7 +16413,7 @@
     </row>
     <row r="75" spans="1:120" ht="19.8" customHeight="1" thickBot="1">
       <c r="A75" s="26" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="B75" s="43" t="s">
         <v>874</v>
@@ -22887,17 +22908,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE84406-98AE-4E64-999D-911172EB9954}">
-  <dimension ref="A1:L165"/>
+  <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:A128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.88671875" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23041,7 +23062,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
+    <row r="11" spans="1:4" ht="18" customHeight="1" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>563</v>
       </c>
@@ -23057,30 +23078,30 @@
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="1" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1092</v>
+        <v>1222</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>564</v>
+        <v>577</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1">
       <c r="A13" s="1" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1101</v>
+        <v>1223</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1">
@@ -23091,10 +23112,10 @@
         <v>579</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1102</v>
+        <v>1092</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1">
@@ -23105,10 +23126,10 @@
         <v>579</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1">
@@ -23119,10 +23140,10 @@
         <v>579</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>1102</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1">
@@ -23133,10 +23154,10 @@
         <v>579</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1">
@@ -23147,10 +23168,10 @@
         <v>579</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1105</v>
+        <v>13</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1">
@@ -23161,10 +23182,10 @@
         <v>579</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1">
@@ -23175,10 +23196,10 @@
         <v>579</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1">
@@ -23189,10 +23210,10 @@
         <v>579</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>1106</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1">
@@ -23203,10 +23224,10 @@
         <v>579</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>1107</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1">
@@ -23217,66 +23238,66 @@
         <v>579</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1">
       <c r="A24" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1092</v>
+        <v>20</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>564</v>
+        <v>589</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1">
       <c r="A25" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1101</v>
+        <v>21</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1">
       <c r="A26" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1108</v>
+        <v>1222</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1">
       <c r="A27" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1109</v>
+        <v>1223</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1">
@@ -23287,10 +23308,10 @@
         <v>593</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1110</v>
+        <v>1092</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>596</v>
+        <v>564</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1">
@@ -23301,10 +23322,10 @@
         <v>593</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1073</v>
+        <v>1101</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" thickBot="1">
@@ -23315,10 +23336,10 @@
         <v>593</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" thickBot="1">
@@ -23329,10 +23350,10 @@
         <v>593</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>1109</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1">
@@ -23343,10 +23364,10 @@
         <v>593</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1">
@@ -23357,10 +23378,10 @@
         <v>593</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1113</v>
+        <v>1073</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" thickBot="1">
@@ -23371,10 +23392,10 @@
         <v>593</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1">
@@ -23385,10 +23406,10 @@
         <v>593</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1115</v>
+        <v>22</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1">
@@ -23399,10 +23420,10 @@
         <v>593</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1">
@@ -23413,10 +23434,10 @@
         <v>593</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1">
@@ -23427,10 +23448,10 @@
         <v>593</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" thickBot="1">
@@ -23441,10 +23462,10 @@
         <v>593</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" thickBot="1">
@@ -23455,10 +23476,10 @@
         <v>593</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" thickBot="1">
@@ -23469,10 +23490,10 @@
         <v>593</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1">
@@ -23483,94 +23504,94 @@
         <v>593</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1108</v>
+        <v>1119</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1">
       <c r="A46" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1">
       <c r="A47" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1126</v>
+        <v>1222</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" thickBot="1">
       <c r="A48" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1127</v>
+        <v>1223</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" thickBot="1">
@@ -23581,10 +23602,10 @@
         <v>625</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1128</v>
+        <v>1108</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>634</v>
+        <v>594</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" thickBot="1">
@@ -23594,11 +23615,11 @@
       <c r="B50" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>1129</v>
+      <c r="C50" s="1" t="s">
+        <v>1123</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" thickBot="1">
@@ -23609,10 +23630,10 @@
         <v>625</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" thickBot="1">
@@ -23623,10 +23644,10 @@
         <v>625</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>637</v>
+        <v>1125</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" thickBot="1">
@@ -23637,10 +23658,10 @@
         <v>625</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1">
@@ -23651,10 +23672,10 @@
         <v>625</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" thickBot="1">
@@ -23665,10 +23686,10 @@
         <v>625</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" thickBot="1">
@@ -23678,11 +23699,11 @@
       <c r="B56" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>1135</v>
+      <c r="C56" s="25" t="s">
+        <v>1129</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1">
@@ -23693,10 +23714,10 @@
         <v>625</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1">
@@ -23707,10 +23728,10 @@
         <v>625</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>652</v>
+        <v>1131</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1">
@@ -23721,10 +23742,10 @@
         <v>625</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" thickBot="1">
@@ -23735,10 +23756,10 @@
         <v>625</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>655</v>
+        <v>639</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1">
@@ -23749,10 +23770,10 @@
         <v>625</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>656</v>
+        <v>640</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" thickBot="1">
@@ -23763,10 +23784,10 @@
         <v>625</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>657</v>
+        <v>1135</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" thickBot="1">
@@ -23777,10 +23798,10 @@
         <v>625</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>658</v>
+        <v>1136</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" thickBot="1">
@@ -23791,122 +23812,122 @@
         <v>625</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" thickBot="1">
       <c r="A65" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>626</v>
+        <v>1138</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1">
       <c r="A66" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D66" s="25" t="s">
-        <v>666</v>
+        <v>1139</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" thickBot="1">
       <c r="A67" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1144</v>
-      </c>
-      <c r="D67" s="25" t="s">
-        <v>668</v>
+        <v>1140</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" thickBot="1">
       <c r="A68" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D68" s="25" t="s">
-        <v>669</v>
+        <v>1141</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1">
       <c r="A69" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1146</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>670</v>
+        <v>1142</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1">
       <c r="A70" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D70" s="25" t="s">
-        <v>671</v>
+        <v>1143</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" thickBot="1">
       <c r="A71" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D71" s="25" t="s">
-        <v>672</v>
+        <v>1222</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" thickBot="1">
       <c r="A72" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>665</v>
+        <v>625</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D72" s="25" t="s">
-        <v>673</v>
+        <v>1223</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" thickBot="1">
@@ -23917,10 +23938,10 @@
         <v>665</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>77</v>
+        <v>1123</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>674</v>
+        <v>626</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" thickBot="1">
@@ -23931,10 +23952,10 @@
         <v>665</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" thickBot="1">
@@ -23945,10 +23966,10 @@
         <v>665</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>79</v>
+        <v>1144</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" thickBot="1">
@@ -23959,10 +23980,10 @@
         <v>665</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>80</v>
+        <v>1145</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" thickBot="1">
@@ -23973,10 +23994,10 @@
         <v>665</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" thickBot="1">
@@ -23987,10 +24008,10 @@
         <v>665</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1148</v>
+        <v>82</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" thickBot="1">
@@ -24001,10 +24022,10 @@
         <v>665</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1149</v>
+        <v>1131</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>683</v>
+        <v>672</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" thickBot="1">
@@ -24015,10 +24036,10 @@
         <v>665</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1150</v>
+        <v>76</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>684</v>
+        <v>673</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" thickBot="1">
@@ -24029,10 +24050,10 @@
         <v>665</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1151</v>
+        <v>77</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>685</v>
+        <v>674</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" thickBot="1">
@@ -24043,10 +24064,10 @@
         <v>665</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" thickBot="1">
@@ -24057,10 +24078,10 @@
         <v>665</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1152</v>
+        <v>79</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" thickBot="1">
@@ -24071,10 +24092,10 @@
         <v>665</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1153</v>
+        <v>80</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" thickBot="1">
@@ -24085,10 +24106,10 @@
         <v>665</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1154</v>
+        <v>1147</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" thickBot="1">
@@ -24099,10 +24120,10 @@
         <v>665</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1155</v>
+        <v>1148</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" thickBot="1">
@@ -24113,10 +24134,10 @@
         <v>665</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1156</v>
+        <v>1149</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" thickBot="1">
@@ -24127,10 +24148,10 @@
         <v>665</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1157</v>
+        <v>1150</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" thickBot="1">
@@ -24141,304 +24162,304 @@
         <v>665</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D89" s="25" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" thickBot="1">
+      <c r="A90" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" thickBot="1">
+      <c r="A91" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" thickBot="1">
+      <c r="A92" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" thickBot="1">
+      <c r="A93" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" thickBot="1">
+      <c r="A94" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D94" s="25" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" thickBot="1">
+      <c r="A95" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D95" s="25" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" thickBot="1">
+      <c r="A96" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D96" s="25" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" thickBot="1">
+      <c r="A97" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" thickBot="1">
+      <c r="A98" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" thickBot="1">
+      <c r="A99" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>1158</v>
       </c>
-      <c r="D89" s="25" t="s">
+      <c r="D99" s="25" t="s">
         <v>693</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" thickBot="1">
-      <c r="A90" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B90" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D90" s="22" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" thickBot="1">
-      <c r="A91" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B91" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>1073</v>
-      </c>
-      <c r="D91" s="22" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" thickBot="1">
-      <c r="A92" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B92" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>1160</v>
-      </c>
-      <c r="D92" s="22" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" thickBot="1">
-      <c r="A93" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B93" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D93" s="22" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15" thickBot="1">
-      <c r="A94" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B94" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>1162</v>
-      </c>
-      <c r="D94" s="22" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" thickBot="1">
-      <c r="A95" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B95" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D95" s="22" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15" thickBot="1">
-      <c r="A96" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B96" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>1163</v>
-      </c>
-      <c r="D96" s="22" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="15" thickBot="1">
-      <c r="A97" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B97" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>1164</v>
-      </c>
-      <c r="D97" s="22" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="15" thickBot="1">
-      <c r="A98" s="22" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B98" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>1165</v>
-      </c>
-      <c r="D98" s="22" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="15" thickBot="1">
-      <c r="A99" s="22" t="s">
-        <v>718</v>
-      </c>
-      <c r="B99" s="22" t="s">
-        <v>718</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" thickBot="1">
       <c r="A100" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1166</v>
+        <v>72</v>
       </c>
       <c r="D100" s="22" t="s">
-        <v>722</v>
+        <v>666</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" thickBot="1">
       <c r="A101" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1167</v>
+        <v>1073</v>
       </c>
       <c r="D101" s="22" t="s">
-        <v>723</v>
+        <v>598</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" thickBot="1">
       <c r="A102" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="D102" s="22" t="s">
-        <v>724</v>
+        <v>698</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" thickBot="1">
       <c r="A103" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B103" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>72</v>
+        <v>1161</v>
       </c>
       <c r="D103" s="22" t="s">
-        <v>666</v>
+        <v>699</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" thickBot="1">
       <c r="A104" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B104" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1169</v>
+        <v>1162</v>
       </c>
       <c r="D104" s="22" t="s">
-        <v>725</v>
+        <v>700</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" thickBot="1">
       <c r="A105" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1170</v>
+        <v>1083</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>727</v>
+        <v>701</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" thickBot="1">
       <c r="A106" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
       <c r="D106" s="22" t="s">
-        <v>728</v>
+        <v>702</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" thickBot="1">
       <c r="A107" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1172</v>
+        <v>1164</v>
       </c>
       <c r="D107" s="22" t="s">
-        <v>729</v>
+        <v>703</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" thickBot="1">
       <c r="A108" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" thickBot="1">
       <c r="A109" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1174</v>
+        <v>1222</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>732</v>
+        <v>717</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" thickBot="1">
       <c r="A110" s="22" t="s">
-        <v>718</v>
+        <v>1159</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1175</v>
+        <v>1223</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>737</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" thickBot="1">
@@ -24449,10 +24470,10 @@
         <v>718</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1176</v>
-      </c>
-      <c r="D111" s="22" t="s">
-        <v>740</v>
+        <v>785</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" thickBot="1">
@@ -24463,13 +24484,13 @@
         <v>718</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1177</v>
+        <v>1166</v>
       </c>
       <c r="D112" s="22" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" ht="15" thickBot="1">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" thickBot="1">
       <c r="A113" s="22" t="s">
         <v>718</v>
       </c>
@@ -24477,13 +24498,13 @@
         <v>718</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1178</v>
+        <v>1167</v>
       </c>
       <c r="D113" s="22" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" ht="15" thickBot="1">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" thickBot="1">
       <c r="A114" s="22" t="s">
         <v>718</v>
       </c>
@@ -24491,13 +24512,13 @@
         <v>718</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" ht="15" thickBot="1">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" thickBot="1">
       <c r="A115" s="22" t="s">
         <v>718</v>
       </c>
@@ -24505,13 +24526,13 @@
         <v>718</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1180</v>
+        <v>72</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" ht="15" thickBot="1">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" thickBot="1">
       <c r="A116" s="22" t="s">
         <v>718</v>
       </c>
@@ -24519,13 +24540,13 @@
         <v>718</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1181</v>
+        <v>1169</v>
       </c>
       <c r="D116" s="22" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" ht="15" thickBot="1">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" thickBot="1">
       <c r="A117" s="22" t="s">
         <v>718</v>
       </c>
@@ -24533,13 +24554,13 @@
         <v>718</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1164</v>
+        <v>1170</v>
       </c>
       <c r="D117" s="22" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" ht="15" thickBot="1">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" thickBot="1">
       <c r="A118" s="22" t="s">
         <v>718</v>
       </c>
@@ -24547,520 +24568,520 @@
         <v>718</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1182</v>
+        <v>1171</v>
       </c>
       <c r="D118" s="22" t="s">
-        <v>755</v>
-      </c>
-      <c r="G118" s="57"/>
-      <c r="H118" s="57"/>
-      <c r="I118" s="56"/>
-      <c r="J118" s="56"/>
-      <c r="K118" s="56"/>
-      <c r="L118" s="56"/>
-    </row>
-    <row r="119" spans="1:12" ht="15" thickBot="1">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15" thickBot="1">
       <c r="A119" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B119" s="22" t="s">
-        <v>759</v>
+        <v>718</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D119" s="57" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" ht="15" thickBot="1">
+        <v>1172</v>
+      </c>
+      <c r="D119" s="22" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15" thickBot="1">
       <c r="A120" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>759</v>
+        <v>718</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1178</v>
-      </c>
-      <c r="D120" s="57" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" ht="15" thickBot="1">
+        <v>1173</v>
+      </c>
+      <c r="D120" s="22" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15" thickBot="1">
       <c r="A121" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" ht="15" thickBot="1">
+        <v>1174</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" thickBot="1">
       <c r="A122" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>72</v>
+        <v>1175</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" ht="15" thickBot="1">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" thickBot="1">
       <c r="A123" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1183</v>
+        <v>1176</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" ht="15" thickBot="1">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" thickBot="1">
       <c r="A124" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1184</v>
+        <v>1177</v>
       </c>
       <c r="D124" s="22" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" ht="15" thickBot="1">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" thickBot="1">
       <c r="A125" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1185</v>
+        <v>1178</v>
       </c>
       <c r="D125" s="22" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" ht="15" thickBot="1">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15" thickBot="1">
       <c r="A126" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>428</v>
+        <v>1179</v>
       </c>
       <c r="D126" s="22" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" ht="15" thickBot="1">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15" thickBot="1">
       <c r="A127" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>784</v>
+        <v>718</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1186</v>
+        <v>1180</v>
       </c>
       <c r="D127" s="22" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" ht="15" thickBot="1">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" thickBot="1">
       <c r="A128" s="22" t="s">
         <v>718</v>
       </c>
       <c r="B128" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D128" s="22" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" ht="15" thickBot="1">
+      <c r="A129" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B129" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D129" s="22" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" ht="15" thickBot="1">
+      <c r="A130" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B130" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D130" s="22" t="s">
+        <v>755</v>
+      </c>
+      <c r="G130" s="57"/>
+      <c r="H130" s="57"/>
+      <c r="I130" s="56"/>
+      <c r="J130" s="56"/>
+      <c r="K130" s="56"/>
+      <c r="L130" s="56"/>
+    </row>
+    <row r="131" spans="1:12" ht="15" thickBot="1">
+      <c r="A131" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B131" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D131" s="22" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" ht="15" thickBot="1">
+      <c r="A132" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B132" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D132" s="22" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" ht="15" thickBot="1">
+      <c r="A133" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B133" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D133" s="57" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" ht="15" thickBot="1">
+      <c r="A134" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B134" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D134" s="57" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="15" thickBot="1">
+      <c r="A135" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B135" s="22" t="s">
         <v>784</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C135" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" ht="15" thickBot="1">
+      <c r="A136" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B136" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D136" s="22" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" ht="15" thickBot="1">
+      <c r="A137" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B137" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D137" s="22" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" ht="15" thickBot="1">
+      <c r="A138" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B138" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D138" s="22" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" ht="15" thickBot="1">
+      <c r="A139" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B139" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D139" s="22" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" ht="15" thickBot="1">
+      <c r="A140" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B140" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D140" s="22" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="15" thickBot="1">
+      <c r="A141" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B141" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D141" s="22" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="15" thickBot="1">
+      <c r="A142" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="B142" s="22" t="s">
+        <v>784</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>1187</v>
       </c>
-      <c r="D128" s="22" t="s">
+      <c r="D142" s="22" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" thickBot="1">
-      <c r="A129" s="22" t="s">
+    <row r="143" spans="1:12" ht="15" thickBot="1">
+      <c r="A143" s="22" t="s">
         <v>1188</v>
       </c>
-      <c r="B129" s="22" t="s">
+      <c r="B143" s="22" t="s">
         <v>764</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C143" s="1" t="s">
         <v>1189</v>
       </c>
-      <c r="D129" s="22" t="s">
+      <c r="D143" s="22" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" thickBot="1">
-      <c r="A130" s="22" t="s">
+    <row r="144" spans="1:12" ht="15" thickBot="1">
+      <c r="A144" s="22" t="s">
         <v>1188</v>
       </c>
-      <c r="B130" s="22" t="s">
+      <c r="B144" s="22" t="s">
         <v>764</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C144" s="1" t="s">
         <v>1190</v>
       </c>
-      <c r="D130" s="22" t="s">
+      <c r="D144" s="22" t="s">
         <v>766</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="15" thickBot="1">
-      <c r="A131" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B131" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>1191</v>
-      </c>
-      <c r="D131" s="22" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="15" thickBot="1">
-      <c r="A132" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B132" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>1192</v>
-      </c>
-      <c r="D132" s="22" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="15" thickBot="1">
-      <c r="A133" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B133" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>1193</v>
-      </c>
-      <c r="D133" s="22" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15" thickBot="1">
-      <c r="A134" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B134" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>1194</v>
-      </c>
-      <c r="D134" s="22" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="15" thickBot="1">
-      <c r="A135" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B135" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>1195</v>
-      </c>
-      <c r="D135" s="22" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="15" thickBot="1">
-      <c r="A136" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B136" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="D136" s="22" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="15" thickBot="1">
-      <c r="A137" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B137" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>1178</v>
-      </c>
-      <c r="D137" s="22" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="15" thickBot="1">
-      <c r="A138" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B138" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>1164</v>
-      </c>
-      <c r="D138" s="22" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="15" thickBot="1">
-      <c r="A139" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B139" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D139" s="22" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="15" thickBot="1">
-      <c r="A140" s="22" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B140" s="22" t="s">
-        <v>764</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="15" thickBot="1">
-      <c r="A141" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="B141" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D141" s="22" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="15" thickBot="1">
-      <c r="A142" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="B142" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D142" s="22" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="15" thickBot="1">
-      <c r="A143" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="B143" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D143" s="22" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15" thickBot="1">
-      <c r="A144" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="B144" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D144" s="22" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" thickBot="1">
       <c r="A145" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B145" s="22" t="s">
-        <v>794</v>
+        <v>764</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1203</v>
+        <v>1191</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>805</v>
+        <v>767</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" thickBot="1">
       <c r="A146" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B146" s="22" t="s">
-        <v>794</v>
+        <v>764</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>1204</v>
+        <v>1192</v>
       </c>
       <c r="D146" s="22" t="s">
-        <v>806</v>
+        <v>768</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" thickBot="1">
       <c r="A147" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B147" s="22" t="s">
-        <v>794</v>
+        <v>764</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>75</v>
+        <v>1193</v>
       </c>
       <c r="D147" s="22" t="s">
-        <v>807</v>
+        <v>769</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" thickBot="1">
       <c r="A148" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B148" s="22" t="s">
-        <v>794</v>
+        <v>764</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1205</v>
+        <v>1194</v>
       </c>
       <c r="D148" s="22" t="s">
-        <v>808</v>
+        <v>774</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" thickBot="1">
       <c r="A149" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B149" s="22" t="s">
-        <v>809</v>
+        <v>764</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1206</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>814</v>
+        <v>1195</v>
+      </c>
+      <c r="D149" s="22" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" thickBot="1">
       <c r="A150" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B150" s="22" t="s">
-        <v>809</v>
+        <v>764</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>1207</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>815</v>
+        <v>736</v>
+      </c>
+      <c r="D150" s="22" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" thickBot="1">
       <c r="A151" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B151" s="22" t="s">
-        <v>809</v>
+        <v>764</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1208</v>
+        <v>1178</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>816</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" thickBot="1">
       <c r="A152" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B152" s="22" t="s">
-        <v>809</v>
+        <v>764</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1209</v>
+        <v>1164</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>817</v>
+        <v>781</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" thickBot="1">
       <c r="A153" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B153" s="22" t="s">
-        <v>809</v>
+        <v>764</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1210</v>
+        <v>1197</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>818</v>
+        <v>782</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15" thickBot="1">
       <c r="A154" s="22" t="s">
-        <v>794</v>
+        <v>1188</v>
       </c>
       <c r="B154" s="22" t="s">
-        <v>809</v>
+        <v>764</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1211</v>
-      </c>
-      <c r="D154" s="22" t="s">
-        <v>819</v>
+        <v>1198</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" thickBot="1">
@@ -25068,13 +25089,13 @@
         <v>794</v>
       </c>
       <c r="B155" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>1212</v>
+        <v>72</v>
       </c>
       <c r="D155" s="22" t="s">
-        <v>820</v>
+        <v>666</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" thickBot="1">
@@ -25082,13 +25103,13 @@
         <v>794</v>
       </c>
       <c r="B156" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1213</v>
+        <v>1200</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>821</v>
+        <v>797</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" thickBot="1">
@@ -25096,13 +25117,13 @@
         <v>794</v>
       </c>
       <c r="B157" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>84</v>
+        <v>1201</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>822</v>
+        <v>798</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" thickBot="1">
@@ -25110,13 +25131,13 @@
         <v>794</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>1214</v>
+        <v>1202</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>823</v>
+        <v>799</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" thickBot="1">
@@ -25124,13 +25145,13 @@
         <v>794</v>
       </c>
       <c r="B159" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1215</v>
+        <v>1203</v>
       </c>
       <c r="D159" s="22" t="s">
-        <v>824</v>
+        <v>805</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" thickBot="1">
@@ -25138,13 +25159,13 @@
         <v>794</v>
       </c>
       <c r="B160" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1216</v>
+        <v>1204</v>
       </c>
       <c r="D160" s="22" t="s">
-        <v>831</v>
+        <v>806</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" thickBot="1">
@@ -25152,13 +25173,13 @@
         <v>794</v>
       </c>
       <c r="B161" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>1217</v>
+        <v>75</v>
       </c>
       <c r="D161" s="22" t="s">
-        <v>832</v>
+        <v>807</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15" thickBot="1">
@@ -25166,13 +25187,13 @@
         <v>794</v>
       </c>
       <c r="B162" s="22" t="s">
-        <v>833</v>
+        <v>794</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1218</v>
+        <v>1205</v>
       </c>
       <c r="D162" s="22" t="s">
-        <v>834</v>
+        <v>808</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15" thickBot="1">
@@ -25180,13 +25201,13 @@
         <v>794</v>
       </c>
       <c r="B163" s="22" t="s">
-        <v>833</v>
+        <v>794</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D163" s="23" t="s">
-        <v>835</v>
+        <v>1222</v>
+      </c>
+      <c r="D163" s="22" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15" thickBot="1">
@@ -25194,26 +25215,250 @@
         <v>794</v>
       </c>
       <c r="B164" s="22" t="s">
-        <v>833</v>
+        <v>794</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
       <c r="D164" s="22" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="29.4" thickBot="1">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="15" thickBot="1">
       <c r="A165" s="22" t="s">
         <v>794</v>
       </c>
       <c r="B165" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="15" thickBot="1">
+      <c r="A166" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B166" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="15" thickBot="1">
+      <c r="A167" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B167" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D167" s="22" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="15" thickBot="1">
+      <c r="A168" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B168" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D168" s="22" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="15" thickBot="1">
+      <c r="A169" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B169" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D169" s="22" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="15" thickBot="1">
+      <c r="A170" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B170" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D170" s="22" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="15" thickBot="1">
+      <c r="A171" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B171" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D171" s="22" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="15" thickBot="1">
+      <c r="A172" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B172" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D172" s="22" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="15" thickBot="1">
+      <c r="A173" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B173" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D173" s="22" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="15" thickBot="1">
+      <c r="A174" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B174" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D174" s="22" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="15" thickBot="1">
+      <c r="A175" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B175" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D175" s="22" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="15" thickBot="1">
+      <c r="A176" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B176" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D176" s="22" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="15" thickBot="1">
+      <c r="A177" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B177" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D177" s="22" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="15" thickBot="1">
+      <c r="A178" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B178" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D165" s="22" t="s">
+      <c r="C178" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D178" s="22" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="15" thickBot="1">
+      <c r="A179" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B179" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D179" s="23" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="15" thickBot="1">
+      <c r="A180" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B180" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D180" s="22" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="15" thickBot="1">
+      <c r="A181" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B181" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D181" s="22" t="s">
         <v>837</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add hour function #3
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D46E1-8633-4AB8-B84D-07460F4D0FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE4ADE7-67FC-42C0-93CC-F3D445D99B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView minimized="1" xWindow="31230" yWindow="1545" windowWidth="21600" windowHeight="11325" activeTab="5" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1228">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -3283,9 +3283,6 @@
   </si>
   <si>
     <t>LM</t>
-  </si>
-  <si>
-    <t>ADEp</t>
   </si>
   <si>
     <t>heure</t>
@@ -4466,8 +4463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -5708,7 +5705,7 @@
         <v>666</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>697</v>
@@ -5774,7 +5771,7 @@
         <v>717</v>
       </c>
       <c r="Y15" s="22" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="Z15" s="22"/>
       <c r="AA15" s="22"/>
@@ -6051,7 +6048,7 @@
         <v>783</v>
       </c>
       <c r="W18" s="23" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
@@ -6193,7 +6190,7 @@
         <v>832</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="S20" s="22"/>
       <c r="T20" s="22"/>
@@ -6292,10 +6289,10 @@
         <v>830</v>
       </c>
       <c r="X21" s="22" t="s">
+        <v>1226</v>
+      </c>
+      <c r="Y21" s="22" t="s">
         <v>1227</v>
-      </c>
-      <c r="Y21" s="22" t="s">
-        <v>1228</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
@@ -6406,8 +6403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCCB31-F863-40F4-95B5-0C6BE514FCA4}">
   <dimension ref="A1:FR108"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="L75" sqref="L75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
@@ -16413,7 +16410,7 @@
     </row>
     <row r="75" spans="1:120" ht="19.8" customHeight="1" thickBot="1">
       <c r="A75" s="26" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B75" s="43" t="s">
         <v>874</v>
@@ -21024,10 +21021,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C72DEFF-7720-4B8E-B4D3-1283341468DF}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -21341,19 +21338,6 @@
       <c r="E18" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1">
-      <c r="A19" s="22" t="s">
-        <v>768</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22066,8 +22050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
   <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -22401,7 +22385,7 @@
         <v>622</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1">
@@ -22417,7 +22401,7 @@
         <v>642</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1">
@@ -22425,7 +22409,7 @@
         <v>643</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1">
@@ -22518,7 +22502,7 @@
     </row>
     <row r="56" spans="1:2" ht="15" thickBot="1">
       <c r="A56" s="22" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>392</v>
@@ -22630,7 +22614,7 @@
     </row>
     <row r="70" spans="1:2" ht="15" thickBot="1">
       <c r="A70" s="22" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>393</v>
@@ -22638,7 +22622,7 @@
     </row>
     <row r="71" spans="1:2" ht="15" thickBot="1">
       <c r="A71" s="22" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>392</v>
@@ -22646,7 +22630,7 @@
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1">
       <c r="A72" s="22" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>392</v>
@@ -22702,7 +22686,7 @@
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1">
       <c r="A79" s="22" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>392</v>
@@ -22910,7 +22894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE84406-98AE-4E64-999D-911172EB9954}">
   <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -22924,16 +22908,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>1088</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="C1" s="55" t="s">
         <v>1089</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="D1" s="55" t="s">
         <v>1090</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
@@ -22944,7 +22928,7 @@
         <v>563</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>564</v>
@@ -22958,7 +22942,7 @@
         <v>563</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>565</v>
@@ -22972,7 +22956,7 @@
         <v>563</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>567</v>
@@ -22986,7 +22970,7 @@
         <v>563</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>568</v>
@@ -23014,7 +22998,7 @@
         <v>563</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>571</v>
@@ -23028,7 +23012,7 @@
         <v>563</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>572</v>
@@ -23042,7 +23026,7 @@
         <v>563</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>573</v>
@@ -23056,7 +23040,7 @@
         <v>563</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>574</v>
@@ -23070,7 +23054,7 @@
         <v>563</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>575</v>
@@ -23084,7 +23068,7 @@
         <v>563</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>577</v>
@@ -23098,7 +23082,7 @@
         <v>563</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>578</v>
@@ -23112,7 +23096,7 @@
         <v>579</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>564</v>
@@ -23126,7 +23110,7 @@
         <v>579</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>580</v>
@@ -23140,7 +23124,7 @@
         <v>579</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>581</v>
@@ -23154,7 +23138,7 @@
         <v>579</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>582</v>
@@ -23182,7 +23166,7 @@
         <v>579</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>584</v>
@@ -23196,7 +23180,7 @@
         <v>579</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>585</v>
@@ -23210,7 +23194,7 @@
         <v>579</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>586</v>
@@ -23224,7 +23208,7 @@
         <v>579</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>587</v>
@@ -23280,7 +23264,7 @@
         <v>579</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>591</v>
@@ -23294,7 +23278,7 @@
         <v>579</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>592</v>
@@ -23308,7 +23292,7 @@
         <v>593</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>564</v>
@@ -23322,7 +23306,7 @@
         <v>593</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>580</v>
@@ -23336,7 +23320,7 @@
         <v>593</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>594</v>
@@ -23350,7 +23334,7 @@
         <v>593</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>595</v>
@@ -23364,7 +23348,7 @@
         <v>593</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>596</v>
@@ -23392,7 +23376,7 @@
         <v>593</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>600</v>
@@ -23420,7 +23404,7 @@
         <v>593</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>602</v>
@@ -23434,7 +23418,7 @@
         <v>593</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>603</v>
@@ -23448,7 +23432,7 @@
         <v>593</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>604</v>
@@ -23462,7 +23446,7 @@
         <v>593</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>607</v>
@@ -23476,7 +23460,7 @@
         <v>593</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>608</v>
@@ -23490,7 +23474,7 @@
         <v>593</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>610</v>
@@ -23504,7 +23488,7 @@
         <v>593</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>616</v>
@@ -23518,7 +23502,7 @@
         <v>593</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>617</v>
@@ -23532,7 +23516,7 @@
         <v>593</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>618</v>
@@ -23546,7 +23530,7 @@
         <v>593</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>620</v>
@@ -23560,7 +23544,7 @@
         <v>593</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>622</v>
@@ -23574,7 +23558,7 @@
         <v>593</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>623</v>
@@ -23588,7 +23572,7 @@
         <v>593</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>624</v>
@@ -23602,7 +23586,7 @@
         <v>625</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>594</v>
@@ -23616,7 +23600,7 @@
         <v>625</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>626</v>
@@ -23630,7 +23614,7 @@
         <v>625</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>629</v>
@@ -23644,7 +23628,7 @@
         <v>625</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>630</v>
@@ -23658,7 +23642,7 @@
         <v>625</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>632</v>
@@ -23672,7 +23656,7 @@
         <v>625</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>633</v>
@@ -23686,7 +23670,7 @@
         <v>625</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>634</v>
@@ -23700,7 +23684,7 @@
         <v>625</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>635</v>
@@ -23714,7 +23698,7 @@
         <v>625</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>636</v>
@@ -23728,7 +23712,7 @@
         <v>625</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>637</v>
@@ -23742,7 +23726,7 @@
         <v>625</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>638</v>
@@ -23756,7 +23740,7 @@
         <v>625</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D60" s="22" t="s">
         <v>639</v>
@@ -23770,7 +23754,7 @@
         <v>625</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D61" s="22" t="s">
         <v>640</v>
@@ -23784,7 +23768,7 @@
         <v>625</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>641</v>
@@ -23798,7 +23782,7 @@
         <v>625</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>644</v>
@@ -23812,7 +23796,7 @@
         <v>625</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>652</v>
@@ -23826,7 +23810,7 @@
         <v>625</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>653</v>
@@ -23840,7 +23824,7 @@
         <v>625</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D66" s="22" t="s">
         <v>655</v>
@@ -23854,7 +23838,7 @@
         <v>625</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D67" s="22" t="s">
         <v>656</v>
@@ -23868,7 +23852,7 @@
         <v>625</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>657</v>
@@ -23882,7 +23866,7 @@
         <v>625</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>658</v>
@@ -23896,7 +23880,7 @@
         <v>625</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="D70" s="22" t="s">
         <v>662</v>
@@ -23910,7 +23894,7 @@
         <v>625</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D71" s="22" t="s">
         <v>663</v>
@@ -23924,7 +23908,7 @@
         <v>625</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D72" s="22" t="s">
         <v>664</v>
@@ -23938,7 +23922,7 @@
         <v>665</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D73" s="25" t="s">
         <v>626</v>
@@ -23966,7 +23950,7 @@
         <v>665</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D75" s="25" t="s">
         <v>668</v>
@@ -23980,7 +23964,7 @@
         <v>665</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="D76" s="25" t="s">
         <v>669</v>
@@ -23994,7 +23978,7 @@
         <v>665</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>670</v>
@@ -24022,7 +24006,7 @@
         <v>665</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D79" s="25" t="s">
         <v>672</v>
@@ -24106,7 +24090,7 @@
         <v>665</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D85" s="25" t="s">
         <v>678</v>
@@ -24120,7 +24104,7 @@
         <v>665</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>682</v>
@@ -24134,7 +24118,7 @@
         <v>665</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D87" s="25" t="s">
         <v>683</v>
@@ -24148,7 +24132,7 @@
         <v>665</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D88" s="25" t="s">
         <v>684</v>
@@ -24162,7 +24146,7 @@
         <v>665</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D89" s="25" t="s">
         <v>685</v>
@@ -24190,7 +24174,7 @@
         <v>665</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="D91" s="25" t="s">
         <v>687</v>
@@ -24204,7 +24188,7 @@
         <v>665</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D92" s="25" t="s">
         <v>688</v>
@@ -24218,7 +24202,7 @@
         <v>665</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D93" s="25" t="s">
         <v>689</v>
@@ -24232,7 +24216,7 @@
         <v>665</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D94" s="25" t="s">
         <v>690</v>
@@ -24246,7 +24230,7 @@
         <v>665</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D95" s="25" t="s">
         <v>691</v>
@@ -24260,7 +24244,7 @@
         <v>665</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D96" s="25" t="s">
         <v>692</v>
@@ -24274,7 +24258,7 @@
         <v>665</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D97" s="22" t="s">
         <v>694</v>
@@ -24288,7 +24272,7 @@
         <v>665</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D98" s="22" t="s">
         <v>695</v>
@@ -24302,7 +24286,7 @@
         <v>665</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D99" s="25" t="s">
         <v>693</v>
@@ -24310,7 +24294,7 @@
     </row>
     <row r="100" spans="1:4" ht="15" thickBot="1">
       <c r="A100" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B100" s="22" t="s">
         <v>696</v>
@@ -24324,7 +24308,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" thickBot="1">
       <c r="A101" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B101" s="22" t="s">
         <v>696</v>
@@ -24338,13 +24322,13 @@
     </row>
     <row r="102" spans="1:4" ht="15" thickBot="1">
       <c r="A102" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B102" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D102" s="22" t="s">
         <v>698</v>
@@ -24352,13 +24336,13 @@
     </row>
     <row r="103" spans="1:4" ht="15" thickBot="1">
       <c r="A103" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B103" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D103" s="22" t="s">
         <v>699</v>
@@ -24366,13 +24350,13 @@
     </row>
     <row r="104" spans="1:4" ht="15" thickBot="1">
       <c r="A104" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B104" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D104" s="22" t="s">
         <v>700</v>
@@ -24380,13 +24364,13 @@
     </row>
     <row r="105" spans="1:4" ht="15" thickBot="1">
       <c r="A105" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B105" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D105" s="22" t="s">
         <v>701</v>
@@ -24394,13 +24378,13 @@
     </row>
     <row r="106" spans="1:4" ht="15" thickBot="1">
       <c r="A106" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B106" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D106" s="22" t="s">
         <v>702</v>
@@ -24408,13 +24392,13 @@
     </row>
     <row r="107" spans="1:4" ht="15" thickBot="1">
       <c r="A107" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B107" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D107" s="22" t="s">
         <v>703</v>
@@ -24422,13 +24406,13 @@
     </row>
     <row r="108" spans="1:4" ht="15" thickBot="1">
       <c r="A108" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B108" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="D108" s="22" t="s">
         <v>717</v>
@@ -24436,13 +24420,13 @@
     </row>
     <row r="109" spans="1:4" ht="15" thickBot="1">
       <c r="A109" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B109" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D109" s="22" t="s">
         <v>717</v>
@@ -24450,16 +24434,16 @@
     </row>
     <row r="110" spans="1:4" ht="15" thickBot="1">
       <c r="A110" s="22" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B110" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" thickBot="1">
@@ -24484,7 +24468,7 @@
         <v>718</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="D112" s="22" t="s">
         <v>722</v>
@@ -24498,7 +24482,7 @@
         <v>718</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="D113" s="22" t="s">
         <v>723</v>
@@ -24512,7 +24496,7 @@
         <v>718</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="D114" s="22" t="s">
         <v>724</v>
@@ -24540,7 +24524,7 @@
         <v>718</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="D116" s="22" t="s">
         <v>725</v>
@@ -24554,7 +24538,7 @@
         <v>718</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D117" s="22" t="s">
         <v>727</v>
@@ -24568,7 +24552,7 @@
         <v>718</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="D118" s="22" t="s">
         <v>728</v>
@@ -24582,7 +24566,7 @@
         <v>718</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="D119" s="22" t="s">
         <v>729</v>
@@ -24596,7 +24580,7 @@
         <v>718</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="D120" s="22" t="s">
         <v>730</v>
@@ -24610,7 +24594,7 @@
         <v>718</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="D121" s="22" t="s">
         <v>732</v>
@@ -24624,7 +24608,7 @@
         <v>718</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="D122" s="22" t="s">
         <v>737</v>
@@ -24638,7 +24622,7 @@
         <v>718</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="D123" s="22" t="s">
         <v>740</v>
@@ -24652,7 +24636,7 @@
         <v>718</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D124" s="22" t="s">
         <v>741</v>
@@ -24666,7 +24650,7 @@
         <v>718</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D125" s="22" t="s">
         <v>750</v>
@@ -24680,7 +24664,7 @@
         <v>718</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D126" s="22" t="s">
         <v>751</v>
@@ -24694,7 +24678,7 @@
         <v>718</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D127" s="22" t="s">
         <v>752</v>
@@ -24708,7 +24692,7 @@
         <v>718</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D128" s="22" t="s">
         <v>753</v>
@@ -24722,7 +24706,7 @@
         <v>718</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D129" s="22" t="s">
         <v>754</v>
@@ -24736,7 +24720,7 @@
         <v>718</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D130" s="22" t="s">
         <v>755</v>
@@ -24756,7 +24740,7 @@
         <v>718</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D131" s="22" t="s">
         <v>757</v>
@@ -24770,7 +24754,7 @@
         <v>718</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D132" s="22" t="s">
         <v>758</v>
@@ -24798,7 +24782,7 @@
         <v>759</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D134" s="57" t="s">
         <v>750</v>
@@ -24840,7 +24824,7 @@
         <v>784</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D137" s="22" t="s">
         <v>786</v>
@@ -24854,7 +24838,7 @@
         <v>784</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D138" s="22" t="s">
         <v>787</v>
@@ -24868,7 +24852,7 @@
         <v>784</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D139" s="22" t="s">
         <v>788</v>
@@ -24896,7 +24880,7 @@
         <v>784</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D141" s="22" t="s">
         <v>790</v>
@@ -24910,7 +24894,7 @@
         <v>784</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D142" s="22" t="s">
         <v>791</v>
@@ -24918,13 +24902,13 @@
     </row>
     <row r="143" spans="1:12" ht="15" thickBot="1">
       <c r="A143" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B143" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D143" s="22" t="s">
         <v>765</v>
@@ -24932,13 +24916,13 @@
     </row>
     <row r="144" spans="1:12" ht="15" thickBot="1">
       <c r="A144" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B144" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D144" s="22" t="s">
         <v>766</v>
@@ -24946,13 +24930,13 @@
     </row>
     <row r="145" spans="1:4" ht="15" thickBot="1">
       <c r="A145" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B145" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D145" s="22" t="s">
         <v>767</v>
@@ -24960,13 +24944,13 @@
     </row>
     <row r="146" spans="1:4" ht="15" thickBot="1">
       <c r="A146" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B146" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D146" s="22" t="s">
         <v>768</v>
@@ -24974,13 +24958,13 @@
     </row>
     <row r="147" spans="1:4" ht="15" thickBot="1">
       <c r="A147" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B147" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="D147" s="22" t="s">
         <v>769</v>
@@ -24988,13 +24972,13 @@
     </row>
     <row r="148" spans="1:4" ht="15" thickBot="1">
       <c r="A148" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B148" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D148" s="22" t="s">
         <v>774</v>
@@ -25002,13 +24986,13 @@
     </row>
     <row r="149" spans="1:4" ht="15" thickBot="1">
       <c r="A149" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B149" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D149" s="22" t="s">
         <v>776</v>
@@ -25016,7 +25000,7 @@
     </row>
     <row r="150" spans="1:4" ht="15" thickBot="1">
       <c r="A150" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B150" s="22" t="s">
         <v>764</v>
@@ -25030,27 +25014,27 @@
     </row>
     <row r="151" spans="1:4" ht="15" thickBot="1">
       <c r="A151" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B151" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" thickBot="1">
       <c r="A152" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B152" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D152" s="22" t="s">
         <v>781</v>
@@ -25058,13 +25042,13 @@
     </row>
     <row r="153" spans="1:4" ht="15" thickBot="1">
       <c r="A153" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B153" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D153" s="22" t="s">
         <v>782</v>
@@ -25072,16 +25056,16 @@
     </row>
     <row r="154" spans="1:4" ht="15" thickBot="1">
       <c r="A154" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B154" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>1198</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>1199</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" thickBot="1">
@@ -25106,7 +25090,7 @@
         <v>794</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="D156" s="22" t="s">
         <v>797</v>
@@ -25120,7 +25104,7 @@
         <v>794</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="D157" s="22" t="s">
         <v>798</v>
@@ -25134,7 +25118,7 @@
         <v>794</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D158" s="22" t="s">
         <v>799</v>
@@ -25148,7 +25132,7 @@
         <v>794</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="D159" s="22" t="s">
         <v>805</v>
@@ -25162,7 +25146,7 @@
         <v>794</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D160" s="22" t="s">
         <v>806</v>
@@ -25190,7 +25174,7 @@
         <v>794</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D162" s="22" t="s">
         <v>808</v>
@@ -25204,7 +25188,7 @@
         <v>794</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D163" s="22" t="s">
         <v>832</v>
@@ -25218,7 +25202,7 @@
         <v>794</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D164" s="22" t="s">
         <v>831</v>
@@ -25232,7 +25216,7 @@
         <v>809</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>814</v>
@@ -25246,7 +25230,7 @@
         <v>809</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>815</v>
@@ -25260,7 +25244,7 @@
         <v>809</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D167" s="22" t="s">
         <v>816</v>
@@ -25274,7 +25258,7 @@
         <v>809</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D168" s="22" t="s">
         <v>817</v>
@@ -25288,7 +25272,7 @@
         <v>809</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D169" s="22" t="s">
         <v>818</v>
@@ -25302,7 +25286,7 @@
         <v>809</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="D170" s="22" t="s">
         <v>819</v>
@@ -25316,7 +25300,7 @@
         <v>809</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="D171" s="22" t="s">
         <v>820</v>
@@ -25330,7 +25314,7 @@
         <v>809</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D172" s="22" t="s">
         <v>821</v>
@@ -25358,7 +25342,7 @@
         <v>809</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="D174" s="22" t="s">
         <v>823</v>
@@ -25372,7 +25356,7 @@
         <v>809</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="D175" s="22" t="s">
         <v>824</v>
@@ -25386,10 +25370,10 @@
         <v>809</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D176" s="22" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" thickBot="1">
@@ -25400,10 +25384,10 @@
         <v>809</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="D177" s="22" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" thickBot="1">
@@ -25414,7 +25398,7 @@
         <v>833</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D178" s="22" t="s">
         <v>834</v>
@@ -25428,7 +25412,7 @@
         <v>833</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="D179" s="23" t="s">
         <v>835</v>
@@ -25442,7 +25426,7 @@
         <v>833</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="D180" s="22" t="s">
         <v>836</v>
@@ -25456,7 +25440,7 @@
         <v>833</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D181" s="22" t="s">
         <v>837</v>

</xml_diff>

<commit_message>
Add cq check #11
Add cq check #11
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6D358D-800D-463E-B7C7-432C1C9056E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798A208A-0A53-4F9B-894F-D47099A20CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31575" yWindow="3015" windowWidth="21930" windowHeight="11325" activeTab="5" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2489" uniqueCount="1227">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -3294,12 +3294,6 @@
     <t>Puits_qPCR_ADNe_Neg_Pos</t>
   </si>
   <si>
-    <t>Cq_ech_Neg_Pos_ADNe</t>
-  </si>
-  <si>
-    <t>Nbr_Copies_reaction_Neg_Pos_ADNe</t>
-  </si>
-  <si>
     <t>Nbr_echantillon_librairie_ADNe</t>
   </si>
   <si>
@@ -3724,6 +3718,9 @@
   </si>
   <si>
     <t>Notes_purification_librairies_ADNe</t>
+  </si>
+  <si>
+    <t>cq</t>
   </si>
 </sst>
 </file>
@@ -4464,7 +4461,7 @@
   <dimension ref="A1:AX22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -5705,7 +5702,7 @@
         <v>666</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>697</v>
@@ -5771,7 +5768,7 @@
         <v>717</v>
       </c>
       <c r="Y15" s="22" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="Z15" s="22"/>
       <c r="AA15" s="22"/>
@@ -6048,7 +6045,7 @@
         <v>783</v>
       </c>
       <c r="W18" s="23" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
@@ -6190,7 +6187,7 @@
         <v>832</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="S20" s="22"/>
       <c r="T20" s="22"/>
@@ -6289,10 +6286,10 @@
         <v>830</v>
       </c>
       <c r="X21" s="22" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="Y21" s="22" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
@@ -16410,7 +16407,7 @@
     </row>
     <row r="75" spans="1:120" ht="19.8" customHeight="1" thickBot="1">
       <c r="A75" s="26" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="B75" s="43" t="s">
         <v>874</v>
@@ -21029,7 +21026,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.88671875" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21254,7 +21251,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29.4" thickBot="1">
+    <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>658</v>
       </c>
@@ -21322,7 +21319,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29.4" thickBot="1">
+    <row r="18" spans="1:5" ht="15" thickBot="1">
       <c r="A18" s="22" t="s">
         <v>806</v>
       </c>
@@ -22048,10 +22045,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -22505,7 +22502,7 @@
         <v>1082</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>392</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1">
@@ -22577,7 +22574,7 @@
         <v>743</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>392</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" thickBot="1">
@@ -22622,7 +22619,7 @@
     </row>
     <row r="71" spans="1:2" ht="15" thickBot="1">
       <c r="A71" s="22" t="s">
-        <v>1084</v>
+        <v>746</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>392</v>
@@ -22630,7 +22627,7 @@
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1">
       <c r="A72" s="22" t="s">
-        <v>1085</v>
+        <v>771</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>392</v>
@@ -22638,7 +22635,7 @@
     </row>
     <row r="73" spans="1:2" ht="15" thickBot="1">
       <c r="A73" s="22" t="s">
-        <v>746</v>
+        <v>772</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>392</v>
@@ -22646,7 +22643,7 @@
     </row>
     <row r="74" spans="1:2" ht="15" thickBot="1">
       <c r="A74" s="22" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>392</v>
@@ -22654,7 +22651,7 @@
     </row>
     <row r="75" spans="1:2" ht="15" thickBot="1">
       <c r="A75" s="22" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>392</v>
@@ -22662,15 +22659,15 @@
     </row>
     <row r="76" spans="1:2" ht="15" thickBot="1">
       <c r="A76" s="22" t="s">
-        <v>775</v>
+        <v>799</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15" thickBot="1">
       <c r="A77" s="22" t="s">
-        <v>776</v>
+        <v>1084</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>392</v>
@@ -22678,15 +22675,15 @@
     </row>
     <row r="78" spans="1:2" ht="15" thickBot="1">
       <c r="A78" s="22" t="s">
-        <v>799</v>
+        <v>812</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1">
       <c r="A79" s="22" t="s">
-        <v>1086</v>
+        <v>813</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>392</v>
@@ -22694,7 +22691,7 @@
     </row>
     <row r="80" spans="1:2" ht="15" thickBot="1">
       <c r="A80" s="22" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>392</v>
@@ -22702,15 +22699,15 @@
     </row>
     <row r="81" spans="1:2" ht="15" thickBot="1">
       <c r="A81" s="22" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" thickBot="1">
       <c r="A82" s="22" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>392</v>
@@ -22718,15 +22715,15 @@
     </row>
     <row r="83" spans="1:2" ht="15" thickBot="1">
       <c r="A83" s="22" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15" thickBot="1">
       <c r="A84" s="22" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>392</v>
@@ -22734,7 +22731,7 @@
     </row>
     <row r="85" spans="1:2" ht="15" thickBot="1">
       <c r="A85" s="22" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>392</v>
@@ -22742,7 +22739,7 @@
     </row>
     <row r="86" spans="1:2" ht="15" thickBot="1">
       <c r="A86" s="22" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>392</v>
@@ -22750,7 +22747,7 @@
     </row>
     <row r="87" spans="1:2" ht="15" thickBot="1">
       <c r="A87" s="22" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>392</v>
@@ -22758,7 +22755,7 @@
     </row>
     <row r="88" spans="1:2" ht="15" thickBot="1">
       <c r="A88" s="22" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>392</v>
@@ -22766,7 +22763,7 @@
     </row>
     <row r="89" spans="1:2" ht="15" thickBot="1">
       <c r="A89" s="22" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>392</v>
@@ -22774,7 +22771,7 @@
     </row>
     <row r="90" spans="1:2" ht="15" thickBot="1">
       <c r="A90" s="22" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>392</v>
@@ -22782,7 +22779,7 @@
     </row>
     <row r="91" spans="1:2" ht="15" thickBot="1">
       <c r="A91" s="22" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>392</v>
@@ -22790,15 +22787,15 @@
     </row>
     <row r="92" spans="1:2" ht="15" thickBot="1">
       <c r="A92" s="22" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" thickBot="1">
       <c r="A93" s="22" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>392</v>
@@ -22806,15 +22803,15 @@
     </row>
     <row r="94" spans="1:2" ht="15" thickBot="1">
       <c r="A94" s="22" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15" thickBot="1">
       <c r="A95" s="22" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>392</v>
@@ -22822,7 +22819,7 @@
     </row>
     <row r="96" spans="1:2" ht="15" thickBot="1">
       <c r="A96" s="22" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>392</v>
@@ -22830,7 +22827,7 @@
     </row>
     <row r="97" spans="1:2" ht="15" thickBot="1">
       <c r="A97" s="22" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>392</v>
@@ -22838,7 +22835,7 @@
     </row>
     <row r="98" spans="1:2" ht="15" thickBot="1">
       <c r="A98" s="22" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>392</v>
@@ -22846,7 +22843,7 @@
     </row>
     <row r="99" spans="1:2" ht="15" thickBot="1">
       <c r="A99" s="22" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>392</v>
@@ -22854,7 +22851,7 @@
     </row>
     <row r="100" spans="1:2" ht="15" thickBot="1">
       <c r="A100" s="22" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>392</v>
@@ -22862,25 +22859,9 @@
     </row>
     <row r="101" spans="1:2" ht="15" thickBot="1">
       <c r="A101" s="22" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="15" thickBot="1">
-      <c r="A102" s="22" t="s">
-        <v>845</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="15" thickBot="1">
-      <c r="A103" s="22" t="s">
-        <v>846</v>
-      </c>
-      <c r="B103" s="1" t="s">
         <v>392</v>
       </c>
     </row>
@@ -22908,16 +22889,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="54" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C1" s="55" t="s">
         <v>1087</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="D1" s="55" t="s">
         <v>1088</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
@@ -22928,7 +22909,7 @@
         <v>563</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>564</v>
@@ -22942,7 +22923,7 @@
         <v>563</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>565</v>
@@ -22956,7 +22937,7 @@
         <v>563</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>567</v>
@@ -22970,7 +22951,7 @@
         <v>563</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>568</v>
@@ -22998,7 +22979,7 @@
         <v>563</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>571</v>
@@ -23012,7 +22993,7 @@
         <v>563</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>572</v>
@@ -23026,7 +23007,7 @@
         <v>563</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>573</v>
@@ -23040,7 +23021,7 @@
         <v>563</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>574</v>
@@ -23054,7 +23035,7 @@
         <v>563</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>575</v>
@@ -23068,7 +23049,7 @@
         <v>563</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>577</v>
@@ -23082,7 +23063,7 @@
         <v>563</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>578</v>
@@ -23096,7 +23077,7 @@
         <v>579</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>564</v>
@@ -23110,7 +23091,7 @@
         <v>579</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>580</v>
@@ -23124,7 +23105,7 @@
         <v>579</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>581</v>
@@ -23138,7 +23119,7 @@
         <v>579</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>582</v>
@@ -23166,7 +23147,7 @@
         <v>579</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>584</v>
@@ -23180,7 +23161,7 @@
         <v>579</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>585</v>
@@ -23194,7 +23175,7 @@
         <v>579</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>586</v>
@@ -23208,7 +23189,7 @@
         <v>579</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>587</v>
@@ -23264,7 +23245,7 @@
         <v>579</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>591</v>
@@ -23278,7 +23259,7 @@
         <v>579</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>592</v>
@@ -23292,7 +23273,7 @@
         <v>593</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>564</v>
@@ -23306,7 +23287,7 @@
         <v>593</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>580</v>
@@ -23320,7 +23301,7 @@
         <v>593</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>594</v>
@@ -23334,7 +23315,7 @@
         <v>593</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>595</v>
@@ -23348,7 +23329,7 @@
         <v>593</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>596</v>
@@ -23376,7 +23357,7 @@
         <v>593</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>600</v>
@@ -23404,7 +23385,7 @@
         <v>593</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>602</v>
@@ -23418,7 +23399,7 @@
         <v>593</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>603</v>
@@ -23432,7 +23413,7 @@
         <v>593</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>604</v>
@@ -23446,7 +23427,7 @@
         <v>593</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>607</v>
@@ -23460,7 +23441,7 @@
         <v>593</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>608</v>
@@ -23474,7 +23455,7 @@
         <v>593</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>610</v>
@@ -23488,7 +23469,7 @@
         <v>593</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>616</v>
@@ -23502,7 +23483,7 @@
         <v>593</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>617</v>
@@ -23516,7 +23497,7 @@
         <v>593</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>618</v>
@@ -23530,7 +23511,7 @@
         <v>593</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>620</v>
@@ -23544,7 +23525,7 @@
         <v>593</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>622</v>
@@ -23558,7 +23539,7 @@
         <v>593</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>623</v>
@@ -23572,7 +23553,7 @@
         <v>593</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>624</v>
@@ -23586,7 +23567,7 @@
         <v>625</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>594</v>
@@ -23600,7 +23581,7 @@
         <v>625</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>626</v>
@@ -23614,7 +23595,7 @@
         <v>625</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>629</v>
@@ -23628,7 +23609,7 @@
         <v>625</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>630</v>
@@ -23642,7 +23623,7 @@
         <v>625</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>632</v>
@@ -23656,7 +23637,7 @@
         <v>625</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>633</v>
@@ -23670,7 +23651,7 @@
         <v>625</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>634</v>
@@ -23684,7 +23665,7 @@
         <v>625</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>635</v>
@@ -23698,7 +23679,7 @@
         <v>625</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>636</v>
@@ -23712,7 +23693,7 @@
         <v>625</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>637</v>
@@ -23726,7 +23707,7 @@
         <v>625</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>638</v>
@@ -23740,7 +23721,7 @@
         <v>625</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="D60" s="22" t="s">
         <v>639</v>
@@ -23754,7 +23735,7 @@
         <v>625</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D61" s="22" t="s">
         <v>640</v>
@@ -23768,7 +23749,7 @@
         <v>625</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>641</v>
@@ -23782,7 +23763,7 @@
         <v>625</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>644</v>
@@ -23796,7 +23777,7 @@
         <v>625</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>652</v>
@@ -23810,7 +23791,7 @@
         <v>625</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>653</v>
@@ -23824,7 +23805,7 @@
         <v>625</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="D66" s="22" t="s">
         <v>655</v>
@@ -23838,7 +23819,7 @@
         <v>625</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="D67" s="22" t="s">
         <v>656</v>
@@ -23852,7 +23833,7 @@
         <v>625</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>657</v>
@@ -23866,7 +23847,7 @@
         <v>625</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>658</v>
@@ -23880,7 +23861,7 @@
         <v>625</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="D70" s="22" t="s">
         <v>662</v>
@@ -23894,7 +23875,7 @@
         <v>625</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D71" s="22" t="s">
         <v>663</v>
@@ -23908,7 +23889,7 @@
         <v>625</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D72" s="22" t="s">
         <v>664</v>
@@ -23922,7 +23903,7 @@
         <v>665</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="D73" s="25" t="s">
         <v>626</v>
@@ -23950,7 +23931,7 @@
         <v>665</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="D75" s="25" t="s">
         <v>668</v>
@@ -23964,7 +23945,7 @@
         <v>665</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="D76" s="25" t="s">
         <v>669</v>
@@ -23978,7 +23959,7 @@
         <v>665</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>670</v>
@@ -24006,7 +23987,7 @@
         <v>665</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="D79" s="25" t="s">
         <v>672</v>
@@ -24090,7 +24071,7 @@
         <v>665</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="D85" s="25" t="s">
         <v>678</v>
@@ -24104,7 +24085,7 @@
         <v>665</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>682</v>
@@ -24118,7 +24099,7 @@
         <v>665</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="D87" s="25" t="s">
         <v>683</v>
@@ -24132,7 +24113,7 @@
         <v>665</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="D88" s="25" t="s">
         <v>684</v>
@@ -24146,7 +24127,7 @@
         <v>665</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="D89" s="25" t="s">
         <v>685</v>
@@ -24174,7 +24155,7 @@
         <v>665</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="D91" s="25" t="s">
         <v>687</v>
@@ -24188,7 +24169,7 @@
         <v>665</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="D92" s="25" t="s">
         <v>688</v>
@@ -24202,7 +24183,7 @@
         <v>665</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="D93" s="25" t="s">
         <v>689</v>
@@ -24216,7 +24197,7 @@
         <v>665</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="D94" s="25" t="s">
         <v>690</v>
@@ -24230,7 +24211,7 @@
         <v>665</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="D95" s="25" t="s">
         <v>691</v>
@@ -24244,7 +24225,7 @@
         <v>665</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="D96" s="25" t="s">
         <v>692</v>
@@ -24258,7 +24239,7 @@
         <v>665</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D97" s="22" t="s">
         <v>694</v>
@@ -24272,7 +24253,7 @@
         <v>665</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D98" s="22" t="s">
         <v>695</v>
@@ -24286,7 +24267,7 @@
         <v>665</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="D99" s="25" t="s">
         <v>693</v>
@@ -24294,7 +24275,7 @@
     </row>
     <row r="100" spans="1:4" ht="15" thickBot="1">
       <c r="A100" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B100" s="22" t="s">
         <v>696</v>
@@ -24308,7 +24289,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" thickBot="1">
       <c r="A101" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B101" s="22" t="s">
         <v>696</v>
@@ -24322,13 +24303,13 @@
     </row>
     <row r="102" spans="1:4" ht="15" thickBot="1">
       <c r="A102" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B102" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D102" s="22" t="s">
         <v>698</v>
@@ -24336,13 +24317,13 @@
     </row>
     <row r="103" spans="1:4" ht="15" thickBot="1">
       <c r="A103" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B103" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="D103" s="22" t="s">
         <v>699</v>
@@ -24350,13 +24331,13 @@
     </row>
     <row r="104" spans="1:4" ht="15" thickBot="1">
       <c r="A104" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B104" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D104" s="22" t="s">
         <v>700</v>
@@ -24364,7 +24345,7 @@
     </row>
     <row r="105" spans="1:4" ht="15" thickBot="1">
       <c r="A105" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B105" s="22" t="s">
         <v>696</v>
@@ -24378,13 +24359,13 @@
     </row>
     <row r="106" spans="1:4" ht="15" thickBot="1">
       <c r="A106" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B106" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="D106" s="22" t="s">
         <v>702</v>
@@ -24392,13 +24373,13 @@
     </row>
     <row r="107" spans="1:4" ht="15" thickBot="1">
       <c r="A107" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B107" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="D107" s="22" t="s">
         <v>703</v>
@@ -24406,13 +24387,13 @@
     </row>
     <row r="108" spans="1:4" ht="15" thickBot="1">
       <c r="A108" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B108" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="D108" s="22" t="s">
         <v>717</v>
@@ -24420,13 +24401,13 @@
     </row>
     <row r="109" spans="1:4" ht="15" thickBot="1">
       <c r="A109" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B109" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D109" s="22" t="s">
         <v>717</v>
@@ -24434,16 +24415,16 @@
     </row>
     <row r="110" spans="1:4" ht="15" thickBot="1">
       <c r="A110" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B110" s="22" t="s">
         <v>696</v>
       </c>
       <c r="C110" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D110" s="22" t="s">
         <v>1222</v>
-      </c>
-      <c r="D110" s="22" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" thickBot="1">
@@ -24468,7 +24449,7 @@
         <v>718</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="D112" s="22" t="s">
         <v>722</v>
@@ -24482,7 +24463,7 @@
         <v>718</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="D113" s="22" t="s">
         <v>723</v>
@@ -24496,7 +24477,7 @@
         <v>718</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="D114" s="22" t="s">
         <v>724</v>
@@ -24524,7 +24505,7 @@
         <v>718</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="D116" s="22" t="s">
         <v>725</v>
@@ -24538,7 +24519,7 @@
         <v>718</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="D117" s="22" t="s">
         <v>727</v>
@@ -24552,7 +24533,7 @@
         <v>718</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="D118" s="22" t="s">
         <v>728</v>
@@ -24566,7 +24547,7 @@
         <v>718</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="D119" s="22" t="s">
         <v>729</v>
@@ -24580,7 +24561,7 @@
         <v>718</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="D120" s="22" t="s">
         <v>730</v>
@@ -24594,7 +24575,7 @@
         <v>718</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="D121" s="22" t="s">
         <v>732</v>
@@ -24608,7 +24589,7 @@
         <v>718</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="D122" s="22" t="s">
         <v>737</v>
@@ -24622,7 +24603,7 @@
         <v>718</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="D123" s="22" t="s">
         <v>740</v>
@@ -24636,7 +24617,7 @@
         <v>718</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="D124" s="22" t="s">
         <v>741</v>
@@ -24650,7 +24631,7 @@
         <v>718</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="D125" s="22" t="s">
         <v>750</v>
@@ -24664,7 +24645,7 @@
         <v>718</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D126" s="22" t="s">
         <v>751</v>
@@ -24678,7 +24659,7 @@
         <v>718</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="D127" s="22" t="s">
         <v>752</v>
@@ -24692,7 +24673,7 @@
         <v>718</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="D128" s="22" t="s">
         <v>753</v>
@@ -24706,7 +24687,7 @@
         <v>718</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="D129" s="22" t="s">
         <v>754</v>
@@ -24720,7 +24701,7 @@
         <v>718</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="D130" s="22" t="s">
         <v>755</v>
@@ -24740,7 +24721,7 @@
         <v>718</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D131" s="22" t="s">
         <v>757</v>
@@ -24754,7 +24735,7 @@
         <v>718</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D132" s="22" t="s">
         <v>758</v>
@@ -24782,7 +24763,7 @@
         <v>759</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="D134" s="57" t="s">
         <v>750</v>
@@ -24824,7 +24805,7 @@
         <v>784</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="D137" s="22" t="s">
         <v>786</v>
@@ -24838,7 +24819,7 @@
         <v>784</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="D138" s="22" t="s">
         <v>787</v>
@@ -24852,7 +24833,7 @@
         <v>784</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="D139" s="22" t="s">
         <v>788</v>
@@ -24880,7 +24861,7 @@
         <v>784</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="D141" s="22" t="s">
         <v>790</v>
@@ -24894,7 +24875,7 @@
         <v>784</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="D142" s="22" t="s">
         <v>791</v>
@@ -24902,13 +24883,13 @@
     </row>
     <row r="143" spans="1:12" ht="15" thickBot="1">
       <c r="A143" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B143" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="D143" s="22" t="s">
         <v>765</v>
@@ -24916,13 +24897,13 @@
     </row>
     <row r="144" spans="1:12" ht="15" thickBot="1">
       <c r="A144" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B144" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="D144" s="22" t="s">
         <v>766</v>
@@ -24930,13 +24911,13 @@
     </row>
     <row r="145" spans="1:4" ht="15" thickBot="1">
       <c r="A145" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B145" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="D145" s="22" t="s">
         <v>767</v>
@@ -24944,13 +24925,13 @@
     </row>
     <row r="146" spans="1:4" ht="15" thickBot="1">
       <c r="A146" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B146" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="D146" s="22" t="s">
         <v>768</v>
@@ -24958,13 +24939,13 @@
     </row>
     <row r="147" spans="1:4" ht="15" thickBot="1">
       <c r="A147" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B147" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="D147" s="22" t="s">
         <v>769</v>
@@ -24972,13 +24953,13 @@
     </row>
     <row r="148" spans="1:4" ht="15" thickBot="1">
       <c r="A148" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B148" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="D148" s="22" t="s">
         <v>774</v>
@@ -24986,13 +24967,13 @@
     </row>
     <row r="149" spans="1:4" ht="15" thickBot="1">
       <c r="A149" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B149" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="D149" s="22" t="s">
         <v>776</v>
@@ -25000,7 +24981,7 @@
     </row>
     <row r="150" spans="1:4" ht="15" thickBot="1">
       <c r="A150" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B150" s="22" t="s">
         <v>764</v>
@@ -25014,27 +24995,27 @@
     </row>
     <row r="151" spans="1:4" ht="15" thickBot="1">
       <c r="A151" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B151" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" thickBot="1">
       <c r="A152" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B152" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="D152" s="22" t="s">
         <v>781</v>
@@ -25042,13 +25023,13 @@
     </row>
     <row r="153" spans="1:4" ht="15" thickBot="1">
       <c r="A153" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B153" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="D153" s="22" t="s">
         <v>782</v>
@@ -25056,16 +25037,16 @@
     </row>
     <row r="154" spans="1:4" ht="15" thickBot="1">
       <c r="A154" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B154" s="22" t="s">
         <v>764</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" thickBot="1">
@@ -25090,7 +25071,7 @@
         <v>794</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D156" s="22" t="s">
         <v>797</v>
@@ -25104,7 +25085,7 @@
         <v>794</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D157" s="22" t="s">
         <v>798</v>
@@ -25118,7 +25099,7 @@
         <v>794</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D158" s="22" t="s">
         <v>799</v>
@@ -25132,7 +25113,7 @@
         <v>794</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D159" s="22" t="s">
         <v>805</v>
@@ -25146,7 +25127,7 @@
         <v>794</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="D160" s="22" t="s">
         <v>806</v>
@@ -25174,7 +25155,7 @@
         <v>794</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="D162" s="22" t="s">
         <v>808</v>
@@ -25188,7 +25169,7 @@
         <v>794</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D163" s="22" t="s">
         <v>832</v>
@@ -25202,7 +25183,7 @@
         <v>794</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D164" s="22" t="s">
         <v>831</v>
@@ -25216,7 +25197,7 @@
         <v>809</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>814</v>
@@ -25230,7 +25211,7 @@
         <v>809</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>815</v>
@@ -25244,7 +25225,7 @@
         <v>809</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="D167" s="22" t="s">
         <v>816</v>
@@ -25258,7 +25239,7 @@
         <v>809</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="D168" s="22" t="s">
         <v>817</v>
@@ -25272,7 +25253,7 @@
         <v>809</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="D169" s="22" t="s">
         <v>818</v>
@@ -25286,7 +25267,7 @@
         <v>809</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="D170" s="22" t="s">
         <v>819</v>
@@ -25300,7 +25281,7 @@
         <v>809</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="D171" s="22" t="s">
         <v>820</v>
@@ -25314,7 +25295,7 @@
         <v>809</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="D172" s="22" t="s">
         <v>821</v>
@@ -25342,7 +25323,7 @@
         <v>809</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D174" s="22" t="s">
         <v>823</v>
@@ -25356,7 +25337,7 @@
         <v>809</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="D175" s="22" t="s">
         <v>824</v>
@@ -25370,10 +25351,10 @@
         <v>809</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D176" s="22" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" thickBot="1">
@@ -25384,10 +25365,10 @@
         <v>809</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D177" s="22" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" thickBot="1">
@@ -25398,7 +25379,7 @@
         <v>833</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="D178" s="22" t="s">
         <v>834</v>
@@ -25412,7 +25393,7 @@
         <v>833</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="D179" s="23" t="s">
         <v>835</v>
@@ -25426,7 +25407,7 @@
         <v>833</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="D180" s="22" t="s">
         <v>836</v>
@@ -25440,7 +25421,7 @@
         <v>833</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="D181" s="22" t="s">
         <v>837</v>

</xml_diff>

<commit_message>
Last update before testing it ....
</commit_message>
<xml_diff>
--- a/inst/BD_format.xlsx
+++ b/inst/BD_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourreta\Documents\Github\GenomicsMLI-DFO\BD-LabGeno-IML_gestion\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798A208A-0A53-4F9B-894F-D47099A20CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9DC5D5-CAD4-408A-B6F5-6CE0A3521CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{ABA34925-8846-4775-8702-4D4077D49CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2489" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1227">
   <si>
     <t>Numero_unique_groupe</t>
   </si>
@@ -3627,9 +3627,6 @@
     <t>Responsable_courbe</t>
   </si>
   <si>
-    <t>Notes_courbes_standard</t>
-  </si>
-  <si>
     <t>Notes_courbe_ADNe</t>
   </si>
   <si>
@@ -3721,6 +3718,9 @@
   </si>
   <si>
     <t>cq</t>
+  </si>
+  <si>
+    <t>Inhibition_ADNe</t>
   </si>
 </sst>
 </file>
@@ -4460,8 +4460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752619B-3059-47B9-8FCC-423DBBDD3D2D}">
   <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -5702,7 +5702,7 @@
         <v>666</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>697</v>
@@ -5720,7 +5720,7 @@
         <v>701</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>702</v>
+        <v>1226</v>
       </c>
       <c r="J15" s="22" t="s">
         <v>703</v>
@@ -5768,7 +5768,7 @@
         <v>717</v>
       </c>
       <c r="Y15" s="22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="Z15" s="22"/>
       <c r="AA15" s="22"/>
@@ -6045,7 +6045,7 @@
         <v>783</v>
       </c>
       <c r="W18" s="23" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
@@ -6187,7 +6187,7 @@
         <v>832</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="S20" s="22"/>
       <c r="T20" s="22"/>
@@ -6286,10 +6286,10 @@
         <v>830</v>
       </c>
       <c r="X21" s="22" t="s">
+        <v>1223</v>
+      </c>
+      <c r="Y21" s="22" t="s">
         <v>1224</v>
-      </c>
-      <c r="Y21" s="22" t="s">
-        <v>1225</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
@@ -6401,7 +6401,7 @@
   <dimension ref="A1:FR108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.5546875" defaultRowHeight="14.4"/>
@@ -16407,7 +16407,7 @@
     </row>
     <row r="75" spans="1:120" ht="19.8" customHeight="1" thickBot="1">
       <c r="A75" s="26" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B75" s="43" t="s">
         <v>874</v>
@@ -16553,7 +16553,7 @@
     </row>
     <row r="76" spans="1:120" ht="15" thickBot="1">
       <c r="A76" s="26" t="s">
-        <v>702</v>
+        <v>1226</v>
       </c>
       <c r="B76" s="43" t="s">
         <v>909</v>
@@ -22047,8 +22047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0667210D-89BC-4B76-9822-A84D7E526363}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -22502,7 +22502,7 @@
         <v>1082</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1">
@@ -22574,7 +22574,7 @@
         <v>743</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" thickBot="1">
@@ -22873,10 +22873,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE84406-98AE-4E64-999D-911172EB9954}">
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -23049,7 +23049,7 @@
         <v>563</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>577</v>
@@ -23063,7 +23063,7 @@
         <v>563</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>578</v>
@@ -23245,7 +23245,7 @@
         <v>579</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>591</v>
@@ -23259,7 +23259,7 @@
         <v>579</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>592</v>
@@ -23539,7 +23539,7 @@
         <v>593</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>623</v>
@@ -23553,7 +23553,7 @@
         <v>593</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>624</v>
@@ -23875,7 +23875,7 @@
         <v>625</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D71" s="22" t="s">
         <v>663</v>
@@ -23889,7 +23889,7 @@
         <v>625</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D72" s="22" t="s">
         <v>664</v>
@@ -24239,7 +24239,7 @@
         <v>665</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="D97" s="22" t="s">
         <v>694</v>
@@ -24253,7 +24253,7 @@
         <v>665</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D98" s="22" t="s">
         <v>695</v>
@@ -24407,10 +24407,10 @@
         <v>696</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1219</v>
+        <v>702</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>717</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" thickBot="1">
@@ -24421,24 +24421,24 @@
         <v>696</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>1222</v>
+        <v>717</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" thickBot="1">
       <c r="A111" s="22" t="s">
-        <v>718</v>
+        <v>1156</v>
       </c>
       <c r="B111" s="22" t="s">
-        <v>718</v>
+        <v>696</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>719</v>
+        <v>1219</v>
+      </c>
+      <c r="D111" s="22" t="s">
+        <v>1221</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" thickBot="1">
@@ -24449,10 +24449,10 @@
         <v>718</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1163</v>
-      </c>
-      <c r="D112" s="22" t="s">
-        <v>722</v>
+        <v>785</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" thickBot="1">
@@ -24463,10 +24463,10 @@
         <v>718</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="D113" s="22" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" thickBot="1">
@@ -24477,10 +24477,10 @@
         <v>718</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" thickBot="1">
@@ -24491,10 +24491,10 @@
         <v>718</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>72</v>
+        <v>1165</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>666</v>
+        <v>724</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" thickBot="1">
@@ -24505,10 +24505,10 @@
         <v>718</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1166</v>
+        <v>72</v>
       </c>
       <c r="D116" s="22" t="s">
-        <v>725</v>
+        <v>666</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" thickBot="1">
@@ -24519,10 +24519,10 @@
         <v>718</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="D117" s="22" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" thickBot="1">
@@ -24533,10 +24533,10 @@
         <v>718</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="D118" s="22" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" thickBot="1">
@@ -24547,10 +24547,10 @@
         <v>718</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="D119" s="22" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" thickBot="1">
@@ -24561,10 +24561,10 @@
         <v>718</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D120" s="22" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" thickBot="1">
@@ -24575,10 +24575,10 @@
         <v>718</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="D121" s="22" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" thickBot="1">
@@ -24589,10 +24589,10 @@
         <v>718</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" thickBot="1">
@@ -24603,10 +24603,10 @@
         <v>718</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" thickBot="1">
@@ -24617,10 +24617,10 @@
         <v>718</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="D124" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" thickBot="1">
@@ -24631,10 +24631,10 @@
         <v>718</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="D125" s="22" t="s">
-        <v>750</v>
+        <v>741</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" thickBot="1">
@@ -24645,10 +24645,10 @@
         <v>718</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="D126" s="22" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" thickBot="1">
@@ -24659,10 +24659,10 @@
         <v>718</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D127" s="22" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" thickBot="1">
@@ -24673,10 +24673,10 @@
         <v>718</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D128" s="22" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="15" thickBot="1">
@@ -24687,10 +24687,10 @@
         <v>718</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1161</v>
+        <v>1178</v>
       </c>
       <c r="D129" s="22" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="15" thickBot="1">
@@ -24701,17 +24701,11 @@
         <v>718</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1179</v>
+        <v>1161</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>755</v>
-      </c>
-      <c r="G130" s="57"/>
-      <c r="H130" s="57"/>
-      <c r="I130" s="56"/>
-      <c r="J130" s="56"/>
-      <c r="K130" s="56"/>
-      <c r="L130" s="56"/>
+        <v>754</v>
+      </c>
     </row>
     <row r="131" spans="1:12" ht="15" thickBot="1">
       <c r="A131" s="22" t="s">
@@ -24721,11 +24715,17 @@
         <v>718</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1219</v>
+        <v>1179</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>757</v>
-      </c>
+        <v>755</v>
+      </c>
+      <c r="G131" s="57"/>
+      <c r="H131" s="57"/>
+      <c r="I131" s="56"/>
+      <c r="J131" s="56"/>
+      <c r="K131" s="56"/>
+      <c r="L131" s="56"/>
     </row>
     <row r="132" spans="1:12" ht="15" thickBot="1">
       <c r="A132" s="22" t="s">
@@ -24735,10 +24735,10 @@
         <v>718</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="15" thickBot="1">
@@ -24746,13 +24746,13 @@
         <v>718</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>759</v>
+        <v>718</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D133" s="57" t="s">
-        <v>719</v>
+        <v>1219</v>
+      </c>
+      <c r="D133" s="22" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="15" thickBot="1">
@@ -24763,10 +24763,10 @@
         <v>759</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1175</v>
+        <v>785</v>
       </c>
       <c r="D134" s="57" t="s">
-        <v>750</v>
+        <v>719</v>
       </c>
     </row>
     <row r="135" spans="1:12" ht="15" thickBot="1">
@@ -24774,13 +24774,13 @@
         <v>718</v>
       </c>
       <c r="B135" s="22" t="s">
-        <v>784</v>
+        <v>759</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>719</v>
+        <v>1175</v>
+      </c>
+      <c r="D135" s="57" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="136" spans="1:12" ht="15" thickBot="1">
@@ -24791,10 +24791,10 @@
         <v>784</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D136" s="22" t="s">
-        <v>666</v>
+        <v>785</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="137" spans="1:12" ht="15" thickBot="1">
@@ -24805,10 +24805,10 @@
         <v>784</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1180</v>
+        <v>72</v>
       </c>
       <c r="D137" s="22" t="s">
-        <v>786</v>
+        <v>666</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="15" thickBot="1">
@@ -24819,10 +24819,10 @@
         <v>784</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D138" s="22" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="139" spans="1:12" ht="15" thickBot="1">
@@ -24833,10 +24833,10 @@
         <v>784</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D139" s="22" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="15" thickBot="1">
@@ -24847,10 +24847,10 @@
         <v>784</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>428</v>
+        <v>1182</v>
       </c>
       <c r="D140" s="22" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="15" thickBot="1">
@@ -24861,10 +24861,10 @@
         <v>784</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1183</v>
+        <v>428</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="142" spans="1:12" ht="15" thickBot="1">
@@ -24875,24 +24875,24 @@
         <v>784</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="143" spans="1:12" ht="15" thickBot="1">
       <c r="A143" s="22" t="s">
-        <v>1185</v>
+        <v>718</v>
       </c>
       <c r="B143" s="22" t="s">
-        <v>764</v>
+        <v>784</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>765</v>
+        <v>791</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="15" thickBot="1">
@@ -24903,10 +24903,10 @@
         <v>764</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" thickBot="1">
@@ -24917,10 +24917,10 @@
         <v>764</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" thickBot="1">
@@ -24931,10 +24931,10 @@
         <v>764</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D146" s="22" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" thickBot="1">
@@ -24945,10 +24945,10 @@
         <v>764</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D147" s="22" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" thickBot="1">
@@ -24959,10 +24959,10 @@
         <v>764</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D148" s="22" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" thickBot="1">
@@ -24973,10 +24973,10 @@
         <v>764</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D149" s="22" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" thickBot="1">
@@ -24987,10 +24987,10 @@
         <v>764</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>736</v>
+        <v>1192</v>
       </c>
       <c r="D150" s="22" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" thickBot="1">
@@ -25001,10 +25001,10 @@
         <v>764</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1175</v>
+        <v>736</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>1193</v>
+        <v>777</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" thickBot="1">
@@ -25015,10 +25015,10 @@
         <v>764</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1161</v>
+        <v>1175</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>781</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" thickBot="1">
@@ -25029,10 +25029,10 @@
         <v>764</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1194</v>
+        <v>1161</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15" thickBot="1">
@@ -25043,24 +25043,24 @@
         <v>764</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1195</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>1196</v>
+        <v>1194</v>
+      </c>
+      <c r="D154" s="22" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" thickBot="1">
       <c r="A155" s="22" t="s">
-        <v>794</v>
+        <v>1185</v>
       </c>
       <c r="B155" s="22" t="s">
-        <v>794</v>
+        <v>764</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D155" s="22" t="s">
-        <v>666</v>
+        <v>1218</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>1195</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" thickBot="1">
@@ -25071,10 +25071,10 @@
         <v>794</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1197</v>
+        <v>72</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>797</v>
+        <v>666</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" thickBot="1">
@@ -25085,10 +25085,10 @@
         <v>794</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" thickBot="1">
@@ -25099,10 +25099,10 @@
         <v>794</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" thickBot="1">
@@ -25113,10 +25113,10 @@
         <v>794</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D159" s="22" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" thickBot="1">
@@ -25127,10 +25127,10 @@
         <v>794</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D160" s="22" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" thickBot="1">
@@ -25141,10 +25141,10 @@
         <v>794</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>75</v>
+        <v>1200</v>
       </c>
       <c r="D161" s="22" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15" thickBot="1">
@@ -25155,10 +25155,10 @@
         <v>794</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>1202</v>
+        <v>75</v>
       </c>
       <c r="D162" s="22" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15" thickBot="1">
@@ -25169,10 +25169,10 @@
         <v>794</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>1219</v>
+        <v>1201</v>
       </c>
       <c r="D163" s="22" t="s">
-        <v>832</v>
+        <v>808</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15" thickBot="1">
@@ -25183,10 +25183,10 @@
         <v>794</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D164" s="22" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15" thickBot="1">
@@ -25194,13 +25194,13 @@
         <v>794</v>
       </c>
       <c r="B165" s="22" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>1203</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>814</v>
+        <v>1219</v>
+      </c>
+      <c r="D165" s="22" t="s">
+        <v>831</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15" thickBot="1">
@@ -25211,10 +25211,10 @@
         <v>809</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15" thickBot="1">
@@ -25225,10 +25225,10 @@
         <v>809</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>1205</v>
-      </c>
-      <c r="D167" s="22" t="s">
-        <v>816</v>
+        <v>1203</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15" thickBot="1">
@@ -25239,10 +25239,10 @@
         <v>809</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="D168" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15" thickBot="1">
@@ -25253,10 +25253,10 @@
         <v>809</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="D169" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15" thickBot="1">
@@ -25267,10 +25267,10 @@
         <v>809</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="D170" s="22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15" thickBot="1">
@@ -25281,10 +25281,10 @@
         <v>809</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="D171" s="22" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15" thickBot="1">
@@ -25295,10 +25295,10 @@
         <v>809</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="D172" s="22" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15" thickBot="1">
@@ -25309,10 +25309,10 @@
         <v>809</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>84</v>
+        <v>1209</v>
       </c>
       <c r="D173" s="22" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15" thickBot="1">
@@ -25323,10 +25323,10 @@
         <v>809</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>1211</v>
+        <v>84</v>
       </c>
       <c r="D174" s="22" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15" thickBot="1">
@@ -25337,10 +25337,10 @@
         <v>809</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="D175" s="22" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15" thickBot="1">
@@ -25351,10 +25351,10 @@
         <v>809</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>1220</v>
+        <v>1211</v>
       </c>
       <c r="D176" s="22" t="s">
-        <v>1224</v>
+        <v>824</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" thickBot="1">
@@ -25368,7 +25368,7 @@
         <v>1219</v>
       </c>
       <c r="D177" s="22" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" thickBot="1">
@@ -25376,13 +25376,13 @@
         <v>794</v>
       </c>
       <c r="B178" s="22" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>1213</v>
+        <v>1218</v>
       </c>
       <c r="D178" s="22" t="s">
-        <v>834</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15" thickBot="1">
@@ -25393,10 +25393,10 @@
         <v>833</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D179" s="23" t="s">
-        <v>835</v>
+        <v>1212</v>
+      </c>
+      <c r="D179" s="22" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15" thickBot="1">
@@ -25407,10 +25407,10 @@
         <v>833</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D180" s="22" t="s">
-        <v>836</v>
+        <v>1213</v>
+      </c>
+      <c r="D180" s="23" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" thickBot="1">
@@ -25421,9 +25421,23 @@
         <v>833</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="D181" s="22" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="15" thickBot="1">
+      <c r="A182" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="B182" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D182" s="22" t="s">
         <v>837</v>
       </c>
     </row>

</xml_diff>